<commit_message>
more works - also obtained measue of macro uncertainty from Jurado, Ludvigson...
</commit_message>
<xml_diff>
--- a/Code/Data/Quarterly.xlsx
+++ b/Code/Data/Quarterly.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -300,12 +300,18 @@
   <si>
     <t>GovSpending</t>
   </si>
+  <si>
+    <t>GZSpread</t>
+  </si>
+  <si>
+    <t>NBERDates</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,8 +381,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,6 +396,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,13 +430,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -460,11 +477,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="4"/>
     <cellStyle name="Normale 2" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -743,13 +764,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK937"/>
+  <dimension ref="A1:AM937"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="AD54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="AF232" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AI20" sqref="AI20"/>
+      <selection pane="bottomRight" activeCell="AL280" sqref="AL280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -764,10 +785,12 @@
     <col min="18" max="18" width="21.28515625" style="9" customWidth="1"/>
     <col min="19" max="35" width="22.140625" style="9" customWidth="1"/>
     <col min="36" max="37" width="22.42578125" style="9" customWidth="1"/>
-    <col min="38" max="16384" width="9.140625" style="9"/>
+    <col min="38" max="38" width="22" style="3"/>
+    <col min="39" max="39" width="22" style="14"/>
+    <col min="40" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -879,8 +902,14 @@
       <c r="AK1" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:37">
+      <c r="AL1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -992,8 +1021,14 @@
       <c r="AK2" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:37">
+      <c r="AL2" s="2">
+        <v>3</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1105,8 +1140,14 @@
       <c r="AK3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:37">
+      <c r="AL3" s="11">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1218,8 +1259,14 @@
       <c r="AK4" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:37">
+      <c r="AL4" s="11">
+        <v>37</v>
+      </c>
+      <c r="AM4" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1331,8 +1378,14 @@
       <c r="AK5" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:37">
+      <c r="AL5" s="11">
+        <v>37</v>
+      </c>
+      <c r="AM5" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39">
       <c r="B6" s="4">
         <v>1950</v>
       </c>
@@ -1369,8 +1422,11 @@
       <c r="S6" s="10">
         <v>-0.11431313472008581</v>
       </c>
-    </row>
-    <row r="7" spans="1:37">
+      <c r="AM6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39">
       <c r="B7" s="4">
         <v>1950.25</v>
       </c>
@@ -1407,8 +1463,11 @@
       <c r="S7" s="10">
         <v>-2.2894475299317971E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:37">
+      <c r="AM7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39">
       <c r="B8" s="4">
         <v>1950.5</v>
       </c>
@@ -1445,8 +1504,11 @@
       <c r="S8" s="10">
         <v>5.9200624915389521E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:37">
+      <c r="AM8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39">
       <c r="B9" s="4">
         <v>1950.75</v>
       </c>
@@ -1483,8 +1545,11 @@
       <c r="S9" s="10">
         <v>6.3127903890477968E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:37">
+      <c r="AM9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39">
       <c r="B10" s="4">
         <v>1951</v>
       </c>
@@ -1521,8 +1586,11 @@
       <c r="S10" s="10">
         <v>6.8106865509809711E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:37">
+      <c r="AM10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39">
       <c r="B11" s="4">
         <v>1951.25</v>
       </c>
@@ -1559,8 +1627,11 @@
       <c r="S11" s="10">
         <v>9.7488465004791219E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:37">
+      <c r="AM11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39">
       <c r="B12" s="4">
         <v>1951.5</v>
       </c>
@@ -1597,8 +1668,11 @@
       <c r="S12" s="10">
         <v>6.0856412442280378E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:37">
+      <c r="AM12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39">
       <c r="B13" s="4">
         <v>1951.75</v>
       </c>
@@ -1635,8 +1709,11 @@
       <c r="S13" s="10">
         <v>6.7322906534108176E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:37">
+      <c r="AM13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39">
       <c r="B14" s="4">
         <v>1952</v>
       </c>
@@ -1676,8 +1753,11 @@
       <c r="S14" s="10">
         <v>0.11976733748280652</v>
       </c>
-    </row>
-    <row r="15" spans="1:37">
+      <c r="AM14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39">
       <c r="B15" s="4">
         <v>1952.25</v>
       </c>
@@ -1717,8 +1797,11 @@
       <c r="S15" s="10">
         <v>5.8630031929538778E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:37">
+      <c r="AM15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39">
       <c r="B16" s="4">
         <v>1952.5</v>
       </c>
@@ -1758,8 +1841,11 @@
       <c r="S16" s="10">
         <v>9.6876224119912549E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:19">
+      <c r="AM16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:39">
       <c r="B17" s="4">
         <v>1952.75</v>
       </c>
@@ -1799,8 +1885,11 @@
       <c r="S17" s="10">
         <v>0.17188637199025875</v>
       </c>
-    </row>
-    <row r="18" spans="2:19">
+      <c r="AM17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:39">
       <c r="B18" s="4">
         <v>1953</v>
       </c>
@@ -1840,8 +1929,11 @@
       <c r="S18" s="10">
         <v>0.13352623987310855</v>
       </c>
-    </row>
-    <row r="19" spans="2:19">
+      <c r="AM18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:39">
       <c r="B19" s="4">
         <v>1953.25</v>
       </c>
@@ -1881,8 +1973,11 @@
       <c r="S19" s="10">
         <v>0.10057663511503792</v>
       </c>
-    </row>
-    <row r="20" spans="2:19">
+      <c r="AM19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:39">
       <c r="B20" s="4">
         <v>1953.5</v>
       </c>
@@ -1922,8 +2017,11 @@
       <c r="S20" s="10">
         <v>1.8029831858980383E-2</v>
       </c>
-    </row>
-    <row r="21" spans="2:19">
+      <c r="AM20" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="21" spans="2:39">
       <c r="B21" s="4">
         <v>1953.75</v>
       </c>
@@ -1963,8 +2061,11 @@
       <c r="S21" s="10">
         <v>-6.2348933979749652E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:19">
+      <c r="AM21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:39">
       <c r="B22" s="4">
         <v>1954</v>
       </c>
@@ -2004,8 +2105,11 @@
       <c r="S22" s="10">
         <v>-0.12012209642471756</v>
       </c>
-    </row>
-    <row r="23" spans="2:19">
+      <c r="AM22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:39">
       <c r="B23" s="4">
         <v>1954.25</v>
       </c>
@@ -2045,8 +2149,11 @@
       <c r="S23" s="10">
         <v>-0.12434067138761502</v>
       </c>
-    </row>
-    <row r="24" spans="2:19">
+      <c r="AM23" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="24" spans="2:39">
       <c r="B24" s="4">
         <v>1954.5</v>
       </c>
@@ -2089,8 +2196,11 @@
       <c r="S24" s="10">
         <v>-0.12031549177222742</v>
       </c>
-    </row>
-    <row r="25" spans="2:19">
+      <c r="AM24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:39">
       <c r="B25" s="4">
         <v>1954.75</v>
       </c>
@@ -2133,8 +2243,11 @@
       <c r="S25" s="10">
         <v>-7.8885558912420869E-2</v>
       </c>
-    </row>
-    <row r="26" spans="2:19">
+      <c r="AM25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:39">
       <c r="B26" s="4">
         <v>1955</v>
       </c>
@@ -2177,8 +2290,11 @@
       <c r="S26" s="10">
         <v>1.1078536585903007E-2</v>
       </c>
-    </row>
-    <row r="27" spans="2:19">
+      <c r="AM26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:39">
       <c r="B27" s="4">
         <v>1955.25</v>
       </c>
@@ -2221,8 +2337,11 @@
       <c r="S27" s="10">
         <v>4.7660711165628818E-2</v>
       </c>
-    </row>
-    <row r="28" spans="2:19">
+      <c r="AM27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:39">
       <c r="B28" s="4">
         <v>1955.5</v>
       </c>
@@ -2265,8 +2384,11 @@
       <c r="S28" s="10">
         <v>3.4274571697712544E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:19">
+      <c r="AM28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:39">
       <c r="B29" s="4">
         <v>1955.75</v>
       </c>
@@ -2309,8 +2431,11 @@
       <c r="S29" s="10">
         <v>7.0927088627340429E-2</v>
       </c>
-    </row>
-    <row r="30" spans="2:19">
+      <c r="AM29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:39">
       <c r="B30" s="4">
         <v>1956</v>
       </c>
@@ -2353,8 +2478,11 @@
       <c r="S30" s="10">
         <v>3.0678640282992033E-2</v>
       </c>
-    </row>
-    <row r="31" spans="2:19">
+      <c r="AM30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:39">
       <c r="B31" s="4">
         <v>1956.25</v>
       </c>
@@ -2397,8 +2525,11 @@
       <c r="S31" s="10">
         <v>-1.5160167036325251E-2</v>
       </c>
-    </row>
-    <row r="32" spans="2:19">
+      <c r="AM31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:39">
       <c r="B32" s="4">
         <v>1956.5</v>
       </c>
@@ -2441,8 +2572,11 @@
       <c r="S32" s="10">
         <v>-8.1167141299843572E-3</v>
       </c>
-    </row>
-    <row r="33" spans="2:37">
+      <c r="AM32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:39">
       <c r="B33" s="4">
         <v>1956.75</v>
       </c>
@@ -2485,8 +2619,11 @@
       <c r="S33" s="10">
         <v>3.0833846677127231E-2</v>
       </c>
-    </row>
-    <row r="34" spans="2:37">
+      <c r="AM33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:39">
       <c r="B34" s="4">
         <v>1957</v>
       </c>
@@ -2529,8 +2666,11 @@
       <c r="S34" s="10">
         <v>-5.7196074377090962E-3</v>
       </c>
-    </row>
-    <row r="35" spans="2:37">
+      <c r="AM34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:39">
       <c r="B35" s="4">
         <v>1957.25</v>
       </c>
@@ -2573,8 +2713,11 @@
       <c r="S35" s="10">
         <v>-8.1547169078575815E-2</v>
       </c>
-    </row>
-    <row r="36" spans="2:37">
+      <c r="AM35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:39">
       <c r="B36" s="4">
         <v>1957.5</v>
       </c>
@@ -2617,8 +2760,11 @@
       <c r="S36" s="10">
         <v>-0.11278996872284601</v>
       </c>
-    </row>
-    <row r="37" spans="2:37">
+      <c r="AM36" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="37" spans="2:39">
       <c r="B37" s="4">
         <v>1957.75</v>
       </c>
@@ -2661,8 +2807,11 @@
       <c r="S37" s="10">
         <v>-0.20580850785103549</v>
       </c>
-    </row>
-    <row r="38" spans="2:37">
+      <c r="AM37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:39">
       <c r="B38" s="4">
         <v>1958</v>
       </c>
@@ -2705,8 +2854,11 @@
       <c r="S38" s="10">
         <v>-0.28366895483664478</v>
       </c>
-    </row>
-    <row r="39" spans="2:37">
+      <c r="AM38" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:39">
       <c r="B39" s="4">
         <v>1958.25</v>
       </c>
@@ -2749,8 +2901,11 @@
       <c r="S39" s="10">
         <v>-0.26634761620783082</v>
       </c>
-    </row>
-    <row r="40" spans="2:37">
+      <c r="AM39" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="40" spans="2:39">
       <c r="B40" s="4">
         <v>1958.5</v>
       </c>
@@ -2793,8 +2948,11 @@
       <c r="S40" s="10">
         <v>-0.19154025681984282</v>
       </c>
-    </row>
-    <row r="41" spans="2:37">
+      <c r="AM40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:39">
       <c r="B41" s="4">
         <v>1958.75</v>
       </c>
@@ -2837,8 +2995,11 @@
       <c r="S41" s="10">
         <v>-0.14187872282057556</v>
       </c>
-    </row>
-    <row r="42" spans="2:37">
+      <c r="AM41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:39">
       <c r="B42" s="4">
         <v>1959</v>
       </c>
@@ -2884,8 +3045,11 @@
       <c r="S42" s="10">
         <v>-5.1920519961963923E-2</v>
       </c>
-    </row>
-    <row r="43" spans="2:37">
+      <c r="AM42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:39">
       <c r="B43" s="4">
         <v>1959.25</v>
       </c>
@@ -2931,8 +3095,11 @@
       <c r="S43" s="10">
         <v>-8.9935538290975489E-3</v>
       </c>
-    </row>
-    <row r="44" spans="2:37">
+      <c r="AM43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:39">
       <c r="B44" s="4">
         <v>1959.5</v>
       </c>
@@ -2979,8 +3146,11 @@
         <v>-6.1327866335059371E-2</v>
       </c>
       <c r="AK44" s="3"/>
-    </row>
-    <row r="45" spans="2:37">
+      <c r="AM44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:39">
       <c r="B45" s="4">
         <v>1959.75</v>
       </c>
@@ -3027,8 +3197,11 @@
         <v>-9.6121041384898798E-2</v>
       </c>
       <c r="AK45" s="3"/>
-    </row>
-    <row r="46" spans="2:37">
+      <c r="AM45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:39">
       <c r="B46" s="4">
         <v>1960</v>
       </c>
@@ -3080,8 +3253,11 @@
       <c r="AK46" s="3">
         <v>144.233</v>
       </c>
-    </row>
-    <row r="47" spans="2:37">
+      <c r="AM46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:39">
       <c r="B47" s="4">
         <v>1960.25</v>
       </c>
@@ -3133,8 +3309,11 @@
       <c r="AK47" s="3">
         <v>147.417</v>
       </c>
-    </row>
-    <row r="48" spans="2:37">
+      <c r="AM47" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="48" spans="2:39">
       <c r="B48" s="4">
         <v>1960.5</v>
       </c>
@@ -3186,8 +3365,11 @@
       <c r="AK48" s="3">
         <v>150.459</v>
       </c>
-    </row>
-    <row r="49" spans="2:37">
+      <c r="AM48" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:39">
       <c r="B49" s="4">
         <v>1960.75</v>
       </c>
@@ -3239,8 +3421,11 @@
       <c r="AK49" s="3">
         <v>153.78</v>
       </c>
-    </row>
-    <row r="50" spans="2:37">
+      <c r="AM49" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:39">
       <c r="B50" s="4">
         <v>1961</v>
       </c>
@@ -3292,8 +3477,11 @@
       <c r="AK50" s="3">
         <v>157.25399999999999</v>
       </c>
-    </row>
-    <row r="51" spans="2:37">
+      <c r="AM50" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="51" spans="2:39">
       <c r="B51" s="4">
         <v>1961.25</v>
       </c>
@@ -3345,8 +3533,11 @@
       <c r="AK51" s="3">
         <v>160.73699999999999</v>
       </c>
-    </row>
-    <row r="52" spans="2:37">
+      <c r="AM51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:39">
       <c r="B52" s="4">
         <v>1961.5</v>
       </c>
@@ -3398,8 +3589,11 @@
       <c r="AK52" s="3">
         <v>162.661</v>
       </c>
-    </row>
-    <row r="53" spans="2:37">
+      <c r="AM52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:39">
       <c r="B53" s="4">
         <v>1961.75</v>
       </c>
@@ -3451,8 +3645,11 @@
       <c r="AK53" s="3">
         <v>166.34399999999999</v>
       </c>
-    </row>
-    <row r="54" spans="2:37">
+      <c r="AM53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:39">
       <c r="B54" s="4">
         <v>1962</v>
       </c>
@@ -3504,8 +3701,11 @@
       <c r="AK54" s="3">
         <v>170.892</v>
       </c>
-    </row>
-    <row r="55" spans="2:37">
+      <c r="AM54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:39">
       <c r="B55" s="4">
         <v>1962.25</v>
       </c>
@@ -3557,8 +3757,11 @@
       <c r="AK55" s="3">
         <v>173.125</v>
       </c>
-    </row>
-    <row r="56" spans="2:37">
+      <c r="AM55" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:39">
       <c r="B56" s="4">
         <v>1962.5</v>
       </c>
@@ -3610,8 +3813,11 @@
       <c r="AK56" s="3">
         <v>175.59700000000001</v>
       </c>
-    </row>
-    <row r="57" spans="2:37">
+      <c r="AM56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:39">
       <c r="B57" s="4">
         <v>1962.75</v>
       </c>
@@ -3663,8 +3869,11 @@
       <c r="AK57" s="3">
         <v>178.20599999999999</v>
       </c>
-    </row>
-    <row r="58" spans="2:37">
+      <c r="AM57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:39">
       <c r="B58" s="4">
         <v>1963</v>
       </c>
@@ -3716,8 +3925,11 @@
       <c r="AK58" s="3">
         <v>179.393</v>
       </c>
-    </row>
-    <row r="59" spans="2:37">
+      <c r="AM58" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:39">
       <c r="B59" s="4">
         <v>1963.25</v>
       </c>
@@ -3769,8 +3981,11 @@
       <c r="AK59" s="3">
         <v>180.369</v>
       </c>
-    </row>
-    <row r="60" spans="2:37">
+      <c r="AM59" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:39">
       <c r="B60" s="4">
         <v>1963.5</v>
       </c>
@@ -3822,8 +4037,11 @@
       <c r="AK60" s="3">
         <v>184.86199999999999</v>
       </c>
-    </row>
-    <row r="61" spans="2:37">
+      <c r="AM60" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:39">
       <c r="B61" s="4">
         <v>1963.75</v>
       </c>
@@ -3875,8 +4093,11 @@
       <c r="AK61" s="3">
         <v>186.792</v>
       </c>
-    </row>
-    <row r="62" spans="2:37">
+      <c r="AM61" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:39">
       <c r="B62" s="4">
         <v>1964</v>
       </c>
@@ -3928,8 +4149,11 @@
       <c r="AK62" s="3">
         <v>190.07499999999999</v>
       </c>
-    </row>
-    <row r="63" spans="2:37">
+      <c r="AM62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:39">
       <c r="B63" s="4">
         <v>1964.25</v>
       </c>
@@ -3981,8 +4205,11 @@
       <c r="AK63" s="3">
         <v>192.97</v>
       </c>
-    </row>
-    <row r="64" spans="2:37">
+      <c r="AM63" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:39">
       <c r="B64" s="4">
         <v>1964.5</v>
       </c>
@@ -4034,8 +4261,11 @@
       <c r="AK64" s="3">
         <v>193.29499999999999</v>
       </c>
-    </row>
-    <row r="65" spans="2:37">
+      <c r="AM64" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:39">
       <c r="B65" s="4">
         <v>1964.75</v>
       </c>
@@ -4087,8 +4317,11 @@
       <c r="AK65" s="3">
         <v>192.97300000000001</v>
       </c>
-    </row>
-    <row r="66" spans="2:37">
+      <c r="AM65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:39">
       <c r="B66" s="4">
         <v>1965</v>
       </c>
@@ -4140,8 +4373,11 @@
       <c r="AK66" s="3">
         <v>196.19800000000001</v>
       </c>
-    </row>
-    <row r="67" spans="2:37">
+      <c r="AM66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:39">
       <c r="B67" s="4">
         <v>1965.25</v>
       </c>
@@ -4193,8 +4429,11 @@
       <c r="AK67" s="3">
         <v>200.08799999999999</v>
       </c>
-    </row>
-    <row r="68" spans="2:37">
+      <c r="AM67" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:39">
       <c r="B68" s="4">
         <v>1965.5</v>
       </c>
@@ -4246,8 +4485,11 @@
       <c r="AK68" s="3">
         <v>208.98</v>
       </c>
-    </row>
-    <row r="69" spans="2:37">
+      <c r="AM68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:39">
       <c r="B69" s="4">
         <v>1965.75</v>
       </c>
@@ -4299,8 +4541,11 @@
       <c r="AK69" s="3">
         <v>214.261</v>
       </c>
-    </row>
-    <row r="70" spans="2:37">
+      <c r="AM69" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:39">
       <c r="B70" s="4">
         <v>1966</v>
       </c>
@@ -4352,8 +4597,11 @@
       <c r="AK70" s="3">
         <v>221.114</v>
       </c>
-    </row>
-    <row r="71" spans="2:37">
+      <c r="AM70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:39">
       <c r="B71" s="4">
         <v>1966.25</v>
       </c>
@@ -4405,8 +4653,11 @@
       <c r="AK71" s="3">
         <v>227.47900000000001</v>
       </c>
-    </row>
-    <row r="72" spans="2:37">
+      <c r="AM71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:39">
       <c r="B72" s="4">
         <v>1966.5</v>
       </c>
@@ -4458,8 +4709,11 @@
       <c r="AK72" s="3">
         <v>235.64400000000001</v>
       </c>
-    </row>
-    <row r="73" spans="2:37">
+      <c r="AM72" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:39">
       <c r="B73" s="4">
         <v>1966.75</v>
       </c>
@@ -4511,8 +4765,11 @@
       <c r="AK73" s="3">
         <v>243.76300000000001</v>
       </c>
-    </row>
-    <row r="74" spans="2:37">
+      <c r="AM73" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:39">
       <c r="B74" s="4">
         <v>1967</v>
       </c>
@@ -4564,8 +4821,11 @@
       <c r="AK74" s="3">
         <v>255.41499999999999</v>
       </c>
-    </row>
-    <row r="75" spans="2:37">
+      <c r="AM74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:39">
       <c r="B75" s="4">
         <v>1967.25</v>
       </c>
@@ -4617,8 +4877,11 @@
       <c r="AK75" s="3">
         <v>256.92200000000003</v>
       </c>
-    </row>
-    <row r="76" spans="2:37">
+      <c r="AM75" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:39">
       <c r="B76" s="4">
         <v>1967.5</v>
       </c>
@@ -4670,8 +4933,11 @@
       <c r="AK76" s="3">
         <v>264.19900000000001</v>
       </c>
-    </row>
-    <row r="77" spans="2:37">
+      <c r="AM76" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:39">
       <c r="B77" s="4">
         <v>1967.75</v>
       </c>
@@ -4739,8 +5005,11 @@
       <c r="AK77" s="3">
         <v>268.38499999999999</v>
       </c>
-    </row>
-    <row r="78" spans="2:37">
+      <c r="AM77" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:39">
       <c r="B78" s="4">
         <v>1968</v>
       </c>
@@ -4808,8 +5077,11 @@
       <c r="AK78" s="3">
         <v>277.11099999999999</v>
       </c>
-    </row>
-    <row r="79" spans="2:37">
+      <c r="AM78" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:39">
       <c r="B79" s="4">
         <v>1968.25</v>
       </c>
@@ -4877,8 +5149,11 @@
       <c r="AK79" s="3">
         <v>286.70800000000003</v>
       </c>
-    </row>
-    <row r="80" spans="2:37">
+      <c r="AM79" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:39">
       <c r="B80" s="4">
         <v>1968.5</v>
       </c>
@@ -4946,8 +5221,11 @@
       <c r="AK80" s="3">
         <v>292.21499999999997</v>
       </c>
-    </row>
-    <row r="81" spans="2:37">
+      <c r="AM80" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:39">
       <c r="B81" s="4">
         <v>1968.75</v>
       </c>
@@ -5039,8 +5317,11 @@
       <c r="AK81" s="3">
         <v>298.98200000000003</v>
       </c>
-    </row>
-    <row r="82" spans="2:37">
+      <c r="AM81" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:39">
       <c r="B82" s="4">
         <v>1969</v>
       </c>
@@ -5132,8 +5413,11 @@
       <c r="AK82" s="3">
         <v>300.56599999999997</v>
       </c>
-    </row>
-    <row r="83" spans="2:37">
+      <c r="AM82" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:39">
       <c r="B83" s="4">
         <v>1969.25</v>
       </c>
@@ -5225,8 +5509,11 @@
       <c r="AK83" s="3">
         <v>307.101</v>
       </c>
-    </row>
-    <row r="84" spans="2:37">
+      <c r="AM83" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:39">
       <c r="B84" s="4">
         <v>1969.5</v>
       </c>
@@ -5318,8 +5605,11 @@
       <c r="AK84" s="3">
         <v>313.91699999999997</v>
       </c>
-    </row>
-    <row r="85" spans="2:37">
+      <c r="AM84" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:39">
       <c r="B85" s="4">
         <v>1969.75</v>
       </c>
@@ -5411,8 +5701,11 @@
       <c r="AK85" s="3">
         <v>318.24299999999999</v>
       </c>
-    </row>
-    <row r="86" spans="2:37">
+      <c r="AM85" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:39">
       <c r="B86" s="4">
         <v>1970</v>
       </c>
@@ -5504,8 +5797,11 @@
       <c r="AK86" s="3">
         <v>325.87799999999999</v>
       </c>
-    </row>
-    <row r="87" spans="2:37">
+      <c r="AM86" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:39">
       <c r="B87" s="4">
         <v>1970.25</v>
       </c>
@@ -5605,8 +5901,11 @@
       <c r="AK87" s="3">
         <v>339.04899999999998</v>
       </c>
-    </row>
-    <row r="88" spans="2:37">
+      <c r="AM87" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:39">
       <c r="B88" s="4">
         <v>1970.5</v>
       </c>
@@ -5706,8 +6005,11 @@
       <c r="AK88" s="3">
         <v>346.41199999999998</v>
       </c>
-    </row>
-    <row r="89" spans="2:37">
+      <c r="AM88" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="2:39">
       <c r="B89" s="4">
         <v>1970.75</v>
       </c>
@@ -5807,8 +6109,11 @@
       <c r="AK89" s="3">
         <v>354.25</v>
       </c>
-    </row>
-    <row r="90" spans="2:37">
+      <c r="AM89" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="90" spans="2:39">
       <c r="B90" s="4">
         <v>1971</v>
       </c>
@@ -5908,8 +6213,11 @@
       <c r="AK90" s="3">
         <v>358.56599999999997</v>
       </c>
-    </row>
-    <row r="91" spans="2:37">
+      <c r="AM90" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:39">
       <c r="B91" s="4">
         <v>1971.25</v>
       </c>
@@ -6009,8 +6317,11 @@
       <c r="AK91" s="3">
         <v>373.20600000000002</v>
       </c>
-    </row>
-    <row r="92" spans="2:37">
+      <c r="AM91" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:39">
       <c r="B92" s="4">
         <v>1971.5</v>
       </c>
@@ -6110,8 +6421,11 @@
       <c r="AK92" s="3">
         <v>377.13200000000001</v>
       </c>
-    </row>
-    <row r="93" spans="2:37">
+      <c r="AM92" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:39">
       <c r="B93" s="4">
         <v>1971.75</v>
       </c>
@@ -6211,8 +6525,11 @@
       <c r="AK93" s="3">
         <v>383.30599999999998</v>
       </c>
-    </row>
-    <row r="94" spans="2:37">
+      <c r="AM93" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:39">
       <c r="B94" s="4">
         <v>1972</v>
       </c>
@@ -6312,8 +6629,11 @@
       <c r="AK94" s="3">
         <v>399.428</v>
       </c>
-    </row>
-    <row r="95" spans="2:37">
+      <c r="AM94" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:39">
       <c r="B95" s="4">
         <v>1972.25</v>
       </c>
@@ -6413,8 +6733,11 @@
       <c r="AK95" s="3">
         <v>403.92899999999997</v>
       </c>
-    </row>
-    <row r="96" spans="2:37">
+      <c r="AM95" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="2:39">
       <c r="B96" s="4">
         <v>1972.5</v>
       </c>
@@ -6514,8 +6837,11 @@
       <c r="AK96" s="3">
         <v>404.90800000000002</v>
       </c>
-    </row>
-    <row r="97" spans="2:37">
+      <c r="AM96" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:39">
       <c r="B97" s="4">
         <v>1972.75</v>
       </c>
@@ -6615,8 +6941,11 @@
       <c r="AK97" s="3">
         <v>419.28500000000003</v>
       </c>
-    </row>
-    <row r="98" spans="2:37">
+      <c r="AM97" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:39">
       <c r="B98" s="4">
         <v>1973</v>
       </c>
@@ -6716,8 +7045,14 @@
       <c r="AK98" s="3">
         <v>426.92700000000002</v>
       </c>
-    </row>
-    <row r="99" spans="2:37">
+      <c r="AL98" s="3">
+        <v>1.026</v>
+      </c>
+      <c r="AM98" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:39">
       <c r="B99" s="4">
         <v>1973.25</v>
       </c>
@@ -6817,8 +7152,14 @@
       <c r="AK99" s="3">
         <v>439.10700000000003</v>
       </c>
-    </row>
-    <row r="100" spans="2:37">
+      <c r="AL99" s="3">
+        <v>1.0113000000000001</v>
+      </c>
+      <c r="AM99" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:39">
       <c r="B100" s="4">
         <v>1973.5</v>
       </c>
@@ -6918,8 +7259,14 @@
       <c r="AK100" s="3">
         <v>437.62900000000002</v>
       </c>
-    </row>
-    <row r="101" spans="2:37">
+      <c r="AL100" s="3">
+        <v>0.97560000000000002</v>
+      </c>
+      <c r="AM100" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:39">
       <c r="B101" s="4">
         <v>1973.75</v>
       </c>
@@ -7019,8 +7366,14 @@
       <c r="AK101" s="3">
         <v>451.01900000000001</v>
       </c>
-    </row>
-    <row r="102" spans="2:37">
+      <c r="AL101" s="3">
+        <v>1.2197</v>
+      </c>
+      <c r="AM101" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="102" spans="2:39">
       <c r="B102" s="4">
         <v>1974</v>
       </c>
@@ -7120,8 +7473,14 @@
       <c r="AK102" s="3">
         <v>465.64299999999997</v>
       </c>
-    </row>
-    <row r="103" spans="2:37">
+      <c r="AL102" s="3">
+        <v>1.1686000000000001</v>
+      </c>
+      <c r="AM102" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="2:39">
       <c r="B103" s="4">
         <v>1974.25</v>
       </c>
@@ -7221,8 +7580,14 @@
       <c r="AK103" s="3">
         <v>477.34800000000001</v>
       </c>
-    </row>
-    <row r="104" spans="2:37">
+      <c r="AL103" s="3">
+        <v>1.6315</v>
+      </c>
+      <c r="AM103" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="2:39">
       <c r="B104" s="4">
         <v>1974.5</v>
       </c>
@@ -7322,8 +7687,14 @@
       <c r="AK104" s="3">
         <v>507.012</v>
       </c>
-    </row>
-    <row r="105" spans="2:37">
+      <c r="AL104" s="3">
+        <v>2.1772</v>
+      </c>
+      <c r="AM104" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:39">
       <c r="B105" s="4">
         <v>1974.75</v>
       </c>
@@ -7423,8 +7794,14 @@
       <c r="AK105" s="3">
         <v>521.20899999999995</v>
       </c>
-    </row>
-    <row r="106" spans="2:37">
+      <c r="AL105" s="3">
+        <v>2.1158999999999999</v>
+      </c>
+      <c r="AM105" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="2:39">
       <c r="B106" s="4">
         <v>1975</v>
       </c>
@@ -7524,8 +7901,14 @@
       <c r="AK106" s="3">
         <v>550.06500000000005</v>
       </c>
-    </row>
-    <row r="107" spans="2:37">
+      <c r="AL106" s="3">
+        <v>1.5933999999999999</v>
+      </c>
+      <c r="AM106" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:39">
       <c r="B107" s="4">
         <v>1975.25</v>
       </c>
@@ -7625,8 +8008,14 @@
       <c r="AK107" s="3">
         <v>571.86400000000003</v>
       </c>
-    </row>
-    <row r="108" spans="2:37">
+      <c r="AL107" s="3">
+        <v>1.4368000000000001</v>
+      </c>
+      <c r="AM107" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:39">
       <c r="B108" s="4">
         <v>1975.5</v>
       </c>
@@ -7726,8 +8115,14 @@
       <c r="AK108" s="3">
         <v>583.50099999999998</v>
       </c>
-    </row>
-    <row r="109" spans="2:37">
+      <c r="AL108" s="3">
+        <v>1.3525</v>
+      </c>
+      <c r="AM108" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="2:39">
       <c r="B109" s="4">
         <v>1975.75</v>
       </c>
@@ -7827,8 +8222,14 @@
       <c r="AK109" s="3">
         <v>600.04899999999998</v>
       </c>
-    </row>
-    <row r="110" spans="2:37">
+      <c r="AL109" s="3">
+        <v>1.1652</v>
+      </c>
+      <c r="AM109" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="2:39">
       <c r="B110" s="4">
         <v>1976</v>
       </c>
@@ -7928,8 +8329,14 @@
       <c r="AK110" s="3">
         <v>609.58299999999997</v>
       </c>
-    </row>
-    <row r="111" spans="2:37">
+      <c r="AL110" s="3">
+        <v>1.0137</v>
+      </c>
+      <c r="AM110" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:39">
       <c r="B111" s="4">
         <v>1976.25</v>
       </c>
@@ -8029,8 +8436,14 @@
       <c r="AK111" s="3">
         <v>606.86699999999996</v>
       </c>
-    </row>
-    <row r="112" spans="2:37">
+      <c r="AL111" s="3">
+        <v>0.99609999999999999</v>
+      </c>
+      <c r="AM111" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:39">
       <c r="B112" s="4">
         <v>1976.5</v>
       </c>
@@ -8130,8 +8543,14 @@
       <c r="AK112" s="3">
         <v>619.59900000000005</v>
       </c>
-    </row>
-    <row r="113" spans="2:37">
+      <c r="AL112" s="3">
+        <v>0.89380000000000004</v>
+      </c>
+      <c r="AM112" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="2:39">
       <c r="B113" s="4">
         <v>1976.75</v>
       </c>
@@ -8231,8 +8650,14 @@
       <c r="AK113" s="3">
         <v>630.202</v>
       </c>
-    </row>
-    <row r="114" spans="2:37">
+      <c r="AL113" s="3">
+        <v>0.95240000000000002</v>
+      </c>
+      <c r="AM113" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="2:39">
       <c r="B114" s="4">
         <v>1977</v>
       </c>
@@ -8332,8 +8757,14 @@
       <c r="AK114" s="3">
         <v>645.40800000000002</v>
       </c>
-    </row>
-    <row r="115" spans="2:37">
+      <c r="AL114" s="3">
+        <v>0.90690000000000004</v>
+      </c>
+      <c r="AM114" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="2:39">
       <c r="B115" s="4">
         <v>1977.25</v>
       </c>
@@ -8433,8 +8864,14 @@
       <c r="AK115" s="3">
         <v>657.41399999999999</v>
       </c>
-    </row>
-    <row r="116" spans="2:37">
+      <c r="AL115" s="3">
+        <v>0.84830000000000005</v>
+      </c>
+      <c r="AM115" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="2:39">
       <c r="B116" s="4">
         <v>1977.5</v>
       </c>
@@ -8534,8 +8971,14 @@
       <c r="AK116" s="3">
         <v>669.00099999999998</v>
       </c>
-    </row>
-    <row r="117" spans="2:37">
+      <c r="AL116" s="3">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="AM116" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="2:39">
       <c r="B117" s="4">
         <v>1977.75</v>
       </c>
@@ -8636,8 +9079,14 @@
       <c r="AK117" s="3">
         <v>688.77099999999996</v>
       </c>
-    </row>
-    <row r="118" spans="2:37">
+      <c r="AL117" s="3">
+        <v>0.88529999999999998</v>
+      </c>
+      <c r="AM117" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:39">
       <c r="B118" s="4">
         <v>1978</v>
       </c>
@@ -8743,8 +9192,14 @@
       <c r="AK118" s="3">
         <v>702.39099999999996</v>
       </c>
-    </row>
-    <row r="119" spans="2:37">
+      <c r="AL118" s="3">
+        <v>0.74839999999999995</v>
+      </c>
+      <c r="AM118" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:39">
       <c r="B119" s="4">
         <v>1978.25</v>
       </c>
@@ -8850,8 +9305,14 @@
       <c r="AK119" s="3">
         <v>721.91099999999994</v>
       </c>
-    </row>
-    <row r="120" spans="2:37">
+      <c r="AL119" s="3">
+        <v>0.69720000000000004</v>
+      </c>
+      <c r="AM119" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="2:39">
       <c r="B120" s="4">
         <v>1978.5</v>
       </c>
@@ -8957,8 +9418,14 @@
       <c r="AK120" s="3">
         <v>749.36099999999999</v>
       </c>
-    </row>
-    <row r="121" spans="2:37">
+      <c r="AL120" s="3">
+        <v>0.61029999999999995</v>
+      </c>
+      <c r="AM120" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="2:39">
       <c r="B121" s="4">
         <v>1978.75</v>
       </c>
@@ -9064,8 +9531,14 @@
       <c r="AK121" s="3">
         <v>767.10799999999995</v>
       </c>
-    </row>
-    <row r="122" spans="2:37">
+      <c r="AL121" s="3">
+        <v>0.63759999999999994</v>
+      </c>
+      <c r="AM121" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="2:39">
       <c r="B122" s="4">
         <v>1979</v>
       </c>
@@ -9171,8 +9644,14 @@
       <c r="AK122" s="3">
         <v>776.40300000000002</v>
       </c>
-    </row>
-    <row r="123" spans="2:37">
+      <c r="AL122" s="3">
+        <v>0.66539999999999999</v>
+      </c>
+      <c r="AM122" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="2:39">
       <c r="B123" s="4">
         <v>1979.25</v>
       </c>
@@ -9278,8 +9757,14 @@
       <c r="AK123" s="3">
         <v>799.70899999999995</v>
       </c>
-    </row>
-    <row r="124" spans="2:37">
+      <c r="AL123" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="AM123" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="2:39">
       <c r="B124" s="4">
         <v>1979.5</v>
       </c>
@@ -9385,8 +9870,14 @@
       <c r="AK124" s="3">
         <v>829.63800000000003</v>
       </c>
-    </row>
-    <row r="125" spans="2:37">
+      <c r="AL124" s="3">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="AM124" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="2:39">
       <c r="B125" s="4">
         <v>1979.75</v>
       </c>
@@ -9492,8 +9983,14 @@
       <c r="AK125" s="3">
         <v>851.73599999999999</v>
       </c>
-    </row>
-    <row r="126" spans="2:37">
+      <c r="AL125" s="3">
+        <v>0.77180000000000004</v>
+      </c>
+      <c r="AM125" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="2:39">
       <c r="B126" s="4">
         <v>1980</v>
       </c>
@@ -9599,8 +10096,14 @@
       <c r="AK126" s="3">
         <v>892.89499999999998</v>
       </c>
-    </row>
-    <row r="127" spans="2:37">
+      <c r="AL126" s="3">
+        <v>0.92379999999999995</v>
+      </c>
+      <c r="AM126" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="127" spans="2:39">
       <c r="B127" s="4">
         <v>1980.25</v>
       </c>
@@ -9706,8 +10209,14 @@
       <c r="AK127" s="3">
         <v>922.79700000000003</v>
       </c>
-    </row>
-    <row r="128" spans="2:37">
+      <c r="AL127" s="3">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="AM127" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:39">
       <c r="B128" s="4">
         <v>1980.5</v>
       </c>
@@ -9813,8 +10322,14 @@
       <c r="AK128" s="3">
         <v>956.08</v>
       </c>
-    </row>
-    <row r="129" spans="2:37">
+      <c r="AL128" s="3">
+        <v>0.8629</v>
+      </c>
+      <c r="AM128" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="129" spans="2:39">
       <c r="B129" s="4">
         <v>1980.75</v>
       </c>
@@ -9920,8 +10435,14 @@
       <c r="AK129" s="3">
         <v>970.56500000000005</v>
       </c>
-    </row>
-    <row r="130" spans="2:37">
+      <c r="AL129" s="3">
+        <v>0.98980000000000001</v>
+      </c>
+      <c r="AM129" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="2:39">
       <c r="B130" s="4">
         <v>1981</v>
       </c>
@@ -10027,8 +10548,14 @@
       <c r="AK130" s="3">
         <v>1022.5940000000001</v>
       </c>
-    </row>
-    <row r="131" spans="2:37">
+      <c r="AL130" s="3">
+        <v>0.96340000000000003</v>
+      </c>
+      <c r="AM130" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="2:39">
       <c r="B131" s="4">
         <v>1981.25</v>
       </c>
@@ -10134,8 +10661,14 @@
       <c r="AK131" s="3">
         <v>1037.4059999999999</v>
       </c>
-    </row>
-    <row r="132" spans="2:37">
+      <c r="AL131" s="3">
+        <v>1.1214999999999999</v>
+      </c>
+      <c r="AM131" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="2:39">
       <c r="B132" s="4">
         <v>1981.5</v>
       </c>
@@ -10241,8 +10774,14 @@
       <c r="AK132" s="3">
         <v>1063.556</v>
       </c>
-    </row>
-    <row r="133" spans="2:37">
+      <c r="AL132" s="3">
+        <v>1.1418999999999999</v>
+      </c>
+      <c r="AM132" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="133" spans="2:39">
       <c r="B133" s="4">
         <v>1981.75</v>
       </c>
@@ -10348,8 +10887,14 @@
       <c r="AK133" s="3">
         <v>1102.2429999999999</v>
       </c>
-    </row>
-    <row r="134" spans="2:37">
+      <c r="AL133" s="3">
+        <v>1.4448000000000001</v>
+      </c>
+      <c r="AM133" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="2:39">
       <c r="B134" s="4">
         <v>1982</v>
       </c>
@@ -10455,8 +11000,14 @@
       <c r="AK134" s="3">
         <v>1122.585</v>
       </c>
-    </row>
-    <row r="135" spans="2:37">
+      <c r="AL134" s="3">
+        <v>1.5509999999999999</v>
+      </c>
+      <c r="AM134" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="2:39">
       <c r="B135" s="4">
         <v>1982.25</v>
       </c>
@@ -10562,8 +11113,14 @@
       <c r="AK135" s="3">
         <v>1150.144</v>
       </c>
-    </row>
-    <row r="136" spans="2:37">
+      <c r="AL135" s="3">
+        <v>1.5548999999999999</v>
+      </c>
+      <c r="AM135" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="2:39">
       <c r="B136" s="4">
         <v>1982.5</v>
       </c>
@@ -10669,8 +11226,14 @@
       <c r="AK136" s="3">
         <v>1185.9459999999999</v>
       </c>
-    </row>
-    <row r="137" spans="2:37">
+      <c r="AL136" s="3">
+        <v>1.6774</v>
+      </c>
+      <c r="AM136" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="2:39">
       <c r="B137" s="4">
         <v>1982.75</v>
       </c>
@@ -10776,8 +11339,14 @@
       <c r="AK137" s="3">
         <v>1222.288</v>
       </c>
-    </row>
-    <row r="138" spans="2:37">
+      <c r="AL137" s="3">
+        <v>1.5542</v>
+      </c>
+      <c r="AM137" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="138" spans="2:39">
       <c r="B138" s="4">
         <v>1983</v>
       </c>
@@ -10883,8 +11452,14 @@
       <c r="AK138" s="3">
         <v>1245.6400000000001</v>
       </c>
-    </row>
-    <row r="139" spans="2:37">
+      <c r="AL138" s="3">
+        <v>1.1416999999999999</v>
+      </c>
+      <c r="AM138" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="2:39">
       <c r="B139" s="4">
         <v>1983.25</v>
       </c>
@@ -10990,8 +11565,14 @@
       <c r="AK139" s="3">
         <v>1255.644</v>
       </c>
-    </row>
-    <row r="140" spans="2:37">
+      <c r="AL139" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="AM139" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="2:39">
       <c r="B140" s="4">
         <v>1983.5</v>
       </c>
@@ -11097,8 +11678,14 @@
       <c r="AK140" s="3">
         <v>1289.0360000000001</v>
       </c>
-    </row>
-    <row r="141" spans="2:37">
+      <c r="AL140" s="3">
+        <v>0.88780000000000003</v>
+      </c>
+      <c r="AM140" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="2:39">
       <c r="B141" s="4">
         <v>1983.75</v>
       </c>
@@ -11204,8 +11791,14 @@
       <c r="AK141" s="3">
         <v>1299.511</v>
       </c>
-    </row>
-    <row r="142" spans="2:37">
+      <c r="AL141" s="3">
+        <v>0.94359999999999999</v>
+      </c>
+      <c r="AM141" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="2:39">
       <c r="B142" s="4">
         <v>1984</v>
       </c>
@@ -11311,8 +11904,14 @@
       <c r="AK142" s="3">
         <v>1320.7560000000001</v>
       </c>
-    </row>
-    <row r="143" spans="2:37">
+      <c r="AL142" s="3">
+        <v>0.95289999999999997</v>
+      </c>
+      <c r="AM142" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="2:39">
       <c r="B143" s="4">
         <v>1984.25</v>
       </c>
@@ -11418,8 +12017,14 @@
       <c r="AK143" s="3">
         <v>1349.9459999999999</v>
       </c>
-    </row>
-    <row r="144" spans="2:37">
+      <c r="AL143" s="3">
+        <v>0.877</v>
+      </c>
+      <c r="AM143" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="2:39">
       <c r="B144" s="4">
         <v>1984.5</v>
       </c>
@@ -11525,8 +12130,14 @@
       <c r="AK144" s="3">
         <v>1380.136</v>
       </c>
-    </row>
-    <row r="145" spans="2:37">
+      <c r="AL144" s="3">
+        <v>0.95779999999999998</v>
+      </c>
+      <c r="AM144" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="2:39">
       <c r="B145" s="4">
         <v>1984.75</v>
       </c>
@@ -11632,8 +12243,14 @@
       <c r="AK145" s="3">
         <v>1423.837</v>
       </c>
-    </row>
-    <row r="146" spans="2:37">
+      <c r="AL145" s="3">
+        <v>0.99639999999999995</v>
+      </c>
+      <c r="AM145" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:39">
       <c r="B146" s="4">
         <v>1985</v>
       </c>
@@ -11739,8 +12356,14 @@
       <c r="AK146" s="3">
         <v>1450.9880000000001</v>
       </c>
-    </row>
-    <row r="147" spans="2:37">
+      <c r="AL146" s="3">
+        <v>1.0276000000000001</v>
+      </c>
+      <c r="AM146" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="2:39">
       <c r="B147" s="4">
         <v>1985.25</v>
       </c>
@@ -11846,8 +12469,14 @@
       <c r="AK147" s="3">
         <v>1483.5319999999999</v>
       </c>
-    </row>
-    <row r="148" spans="2:37">
+      <c r="AL147" s="3">
+        <v>1.1998</v>
+      </c>
+      <c r="AM147" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="2:39">
       <c r="B148" s="4">
         <v>1985.5</v>
       </c>
@@ -11953,8 +12582,14 @@
       <c r="AK148" s="3">
         <v>1514.894</v>
       </c>
-    </row>
-    <row r="149" spans="2:37">
+      <c r="AL148" s="3">
+        <v>1.2437</v>
+      </c>
+      <c r="AM148" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="2:39">
       <c r="B149" s="4">
         <v>1985.75</v>
       </c>
@@ -12060,8 +12695,14 @@
       <c r="AK149" s="3">
         <v>1537.9590000000001</v>
       </c>
-    </row>
-    <row r="150" spans="2:37">
+      <c r="AL149" s="3">
+        <v>1.4291</v>
+      </c>
+      <c r="AM149" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="2:39">
       <c r="B150" s="4">
         <v>1986</v>
       </c>
@@ -12170,8 +12811,14 @@
       <c r="AK150" s="3">
         <v>1557.8050000000001</v>
       </c>
-    </row>
-    <row r="151" spans="2:37">
+      <c r="AL150" s="3">
+        <v>1.8412999999999999</v>
+      </c>
+      <c r="AM150" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="2:39">
       <c r="B151" s="4">
         <v>1986.25</v>
       </c>
@@ -12280,8 +12927,14 @@
       <c r="AK151" s="3">
         <v>1583.0150000000001</v>
       </c>
-    </row>
-    <row r="152" spans="2:37">
+      <c r="AL151" s="3">
+        <v>1.972</v>
+      </c>
+      <c r="AM151" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="2:39">
       <c r="B152" s="4">
         <v>1986.5</v>
       </c>
@@ -12390,8 +13043,14 @@
       <c r="AK152" s="3">
         <v>1625.337</v>
       </c>
-    </row>
-    <row r="153" spans="2:37">
+      <c r="AL152" s="3">
+        <v>2.0950000000000002</v>
+      </c>
+      <c r="AM152" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="2:39">
       <c r="B153" s="4">
         <v>1986.75</v>
       </c>
@@ -12500,8 +13159,14 @@
       <c r="AK153" s="3">
         <v>1625.423</v>
       </c>
-    </row>
-    <row r="154" spans="2:37">
+      <c r="AL153" s="3">
+        <v>1.9807999999999999</v>
+      </c>
+      <c r="AM153" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="2:39">
       <c r="B154" s="4">
         <v>1987</v>
       </c>
@@ -12610,8 +13275,14 @@
       <c r="AK154" s="3">
         <v>1646.039</v>
       </c>
-    </row>
-    <row r="155" spans="2:37">
+      <c r="AL154" s="3">
+        <v>1.8228</v>
+      </c>
+      <c r="AM154" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="2:39">
       <c r="B155" s="4">
         <v>1987.25</v>
       </c>
@@ -12720,8 +13391,14 @@
       <c r="AK155" s="3">
         <v>1671.575</v>
       </c>
-    </row>
-    <row r="156" spans="2:37">
+      <c r="AL155" s="3">
+        <v>1.6871</v>
+      </c>
+      <c r="AM155" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="2:39">
       <c r="B156" s="4">
         <v>1987.5</v>
       </c>
@@ -12830,8 +13507,14 @@
       <c r="AK156" s="3">
         <v>1686.721</v>
       </c>
-    </row>
-    <row r="157" spans="2:37">
+      <c r="AL156" s="3">
+        <v>1.6107</v>
+      </c>
+      <c r="AM156" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="2:39">
       <c r="B157" s="4">
         <v>1987.75</v>
       </c>
@@ -12940,8 +13623,14 @@
       <c r="AK157" s="3">
         <v>1720.3420000000001</v>
       </c>
-    </row>
-    <row r="158" spans="2:37">
+      <c r="AL157" s="3">
+        <v>1.5905</v>
+      </c>
+      <c r="AM157" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="2:39">
       <c r="B158" s="4">
         <v>1988</v>
       </c>
@@ -13050,8 +13739,14 @@
       <c r="AK158" s="3">
         <v>1734.528</v>
       </c>
-    </row>
-    <row r="159" spans="2:37">
+      <c r="AL158" s="3">
+        <v>1.593</v>
+      </c>
+      <c r="AM158" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="2:39">
       <c r="B159" s="4">
         <v>1988.25</v>
       </c>
@@ -13160,8 +13855,14 @@
       <c r="AK159" s="3">
         <v>1750.068</v>
       </c>
-    </row>
-    <row r="160" spans="2:37">
+      <c r="AL159" s="3">
+        <v>1.4676</v>
+      </c>
+      <c r="AM159" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="2:39">
       <c r="B160" s="4">
         <v>1988.5</v>
       </c>
@@ -13270,8 +13971,14 @@
       <c r="AK160" s="3">
         <v>1762.318</v>
       </c>
-    </row>
-    <row r="161" spans="2:37">
+      <c r="AL160" s="3">
+        <v>1.4797</v>
+      </c>
+      <c r="AM160" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="2:39">
       <c r="B161" s="4">
         <v>1988.75</v>
       </c>
@@ -13380,8 +14087,14 @@
       <c r="AK161" s="3">
         <v>1810.922</v>
       </c>
-    </row>
-    <row r="162" spans="2:37">
+      <c r="AL161" s="3">
+        <v>1.524</v>
+      </c>
+      <c r="AM161" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="2:39">
       <c r="B162" s="4">
         <v>1989</v>
       </c>
@@ -13490,8 +14203,14 @@
       <c r="AK162" s="3">
         <v>1844.66</v>
       </c>
-    </row>
-    <row r="163" spans="2:37">
+      <c r="AL162" s="3">
+        <v>1.5034000000000001</v>
+      </c>
+      <c r="AM162" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="2:39">
       <c r="B163" s="4">
         <v>1989.25</v>
       </c>
@@ -13600,8 +14319,14 @@
       <c r="AK163" s="3">
         <v>1882.377</v>
       </c>
-    </row>
-    <row r="164" spans="2:37">
+      <c r="AL163" s="3">
+        <v>1.7632000000000001</v>
+      </c>
+      <c r="AM163" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="2:39">
       <c r="B164" s="4">
         <v>1989.5</v>
       </c>
@@ -13710,8 +14435,14 @@
       <c r="AK164" s="3">
         <v>1914.59</v>
       </c>
-    </row>
-    <row r="165" spans="2:37">
+      <c r="AL164" s="3">
+        <v>1.7269000000000001</v>
+      </c>
+      <c r="AM164" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="2:39">
       <c r="B165" s="4">
         <v>1989.75</v>
       </c>
@@ -13820,8 +14551,14 @@
       <c r="AK165" s="3">
         <v>1946.346</v>
       </c>
-    </row>
-    <row r="166" spans="2:37">
+      <c r="AL165" s="3">
+        <v>1.6442000000000001</v>
+      </c>
+      <c r="AM165" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="2:39">
       <c r="B166" s="4">
         <v>1990</v>
       </c>
@@ -13930,8 +14667,14 @@
       <c r="AK166" s="3">
         <v>1998.202</v>
       </c>
-    </row>
-    <row r="167" spans="2:37">
+      <c r="AL166" s="3">
+        <v>1.4482999999999999</v>
+      </c>
+      <c r="AM166" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="2:39">
       <c r="B167" s="4">
         <v>1990.25</v>
       </c>
@@ -14040,8 +14783,14 @@
       <c r="AK167" s="3">
         <v>2033.1410000000001</v>
       </c>
-    </row>
-    <row r="168" spans="2:37">
+      <c r="AL167" s="3">
+        <v>1.2152000000000001</v>
+      </c>
+      <c r="AM167" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="2:39">
       <c r="B168" s="4">
         <v>1990.5</v>
       </c>
@@ -14150,8 +14899,14 @@
       <c r="AK168" s="3">
         <v>2059.8829999999998</v>
       </c>
-    </row>
-    <row r="169" spans="2:37">
+      <c r="AL168" s="3">
+        <v>1.2535000000000001</v>
+      </c>
+      <c r="AM168" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="169" spans="2:39">
       <c r="B169" s="4">
         <v>1990.75</v>
       </c>
@@ -14260,8 +15015,14 @@
       <c r="AK169" s="3">
         <v>2130.4740000000002</v>
       </c>
-    </row>
-    <row r="170" spans="2:37">
+      <c r="AL169" s="3">
+        <v>1.6213</v>
+      </c>
+      <c r="AM169" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="2:39">
       <c r="B170" s="4">
         <v>1991</v>
       </c>
@@ -14370,8 +15131,14 @@
       <c r="AK170" s="3">
         <v>2069.788</v>
       </c>
-    </row>
-    <row r="171" spans="2:37">
+      <c r="AL170" s="3">
+        <v>1.5216000000000001</v>
+      </c>
+      <c r="AM170" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="2:39">
       <c r="B171" s="4">
         <v>1991.25</v>
       </c>
@@ -14480,8 +15247,14 @@
       <c r="AK171" s="3">
         <v>2147.7759999999998</v>
       </c>
-    </row>
-    <row r="172" spans="2:37">
+      <c r="AL171" s="3">
+        <v>1.4752000000000001</v>
+      </c>
+      <c r="AM171" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="2:39">
       <c r="B172" s="4">
         <v>1991.5</v>
       </c>
@@ -14590,8 +15363,14 @@
       <c r="AK172" s="3">
         <v>2209.8029999999999</v>
       </c>
-    </row>
-    <row r="173" spans="2:37">
+      <c r="AL172" s="3">
+        <v>1.4875</v>
+      </c>
+      <c r="AM172" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="2:39">
       <c r="B173" s="4">
         <v>1991.75</v>
       </c>
@@ -14700,8 +15479,14 @@
       <c r="AK173" s="3">
         <v>2239.2049999999999</v>
       </c>
-    </row>
-    <row r="174" spans="2:37">
+      <c r="AL173" s="3">
+        <v>1.5107999999999999</v>
+      </c>
+      <c r="AM173" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="2:39">
       <c r="B174" s="4">
         <v>1992</v>
       </c>
@@ -14810,8 +15595,14 @@
       <c r="AK174" s="3">
         <v>2294.8359999999998</v>
       </c>
-    </row>
-    <row r="175" spans="2:37">
+      <c r="AL174" s="3">
+        <v>1.3742000000000001</v>
+      </c>
+      <c r="AM174" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="2:39">
       <c r="B175" s="4">
         <v>1992.25</v>
       </c>
@@ -14920,8 +15711,14 @@
       <c r="AK175" s="3">
         <v>2326.569</v>
       </c>
-    </row>
-    <row r="176" spans="2:37">
+      <c r="AL175" s="3">
+        <v>1.3351999999999999</v>
+      </c>
+      <c r="AM175" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="2:39">
       <c r="B176" s="4">
         <v>1992.5</v>
       </c>
@@ -15030,8 +15827,14 @@
       <c r="AK176" s="3">
         <v>2355.7150000000001</v>
       </c>
-    </row>
-    <row r="177" spans="2:37">
+      <c r="AL176" s="3">
+        <v>1.5062</v>
+      </c>
+      <c r="AM176" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="2:39">
       <c r="B177" s="4">
         <v>1992.75</v>
       </c>
@@ -15140,8 +15943,14 @@
       <c r="AK177" s="3">
         <v>2379.8249999999998</v>
       </c>
-    </row>
-    <row r="178" spans="2:37">
+      <c r="AL177" s="3">
+        <v>1.4388000000000001</v>
+      </c>
+      <c r="AM177" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="2:39">
       <c r="B178" s="4">
         <v>1993</v>
       </c>
@@ -15250,8 +16059,14 @@
       <c r="AK178" s="3">
         <v>2383.922</v>
       </c>
-    </row>
-    <row r="179" spans="2:37">
+      <c r="AL178" s="3">
+        <v>1.4533</v>
+      </c>
+      <c r="AM178" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="2:39">
       <c r="B179" s="4">
         <v>1993.25</v>
       </c>
@@ -15360,8 +16175,14 @@
       <c r="AK179" s="3">
         <v>2398.116</v>
       </c>
-    </row>
-    <row r="180" spans="2:37">
+      <c r="AL179" s="3">
+        <v>1.4012</v>
+      </c>
+      <c r="AM179" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="2:39">
       <c r="B180" s="4">
         <v>1993.5</v>
       </c>
@@ -15470,8 +16291,14 @@
       <c r="AK180" s="3">
         <v>2423.5149999999999</v>
       </c>
-    </row>
-    <row r="181" spans="2:37">
+      <c r="AL180" s="3">
+        <v>1.4315</v>
+      </c>
+      <c r="AM180" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="2:39">
       <c r="B181" s="4">
         <v>1993.75</v>
       </c>
@@ -15580,8 +16407,14 @@
       <c r="AK181" s="3">
         <v>2445.4540000000002</v>
       </c>
-    </row>
-    <row r="182" spans="2:37">
+      <c r="AL181" s="3">
+        <v>1.3460000000000001</v>
+      </c>
+      <c r="AM181" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="2:39">
       <c r="B182" s="4">
         <v>1994</v>
       </c>
@@ -15690,8 +16523,14 @@
       <c r="AK182" s="3">
         <v>2429.8609999999999</v>
       </c>
-    </row>
-    <row r="183" spans="2:37">
+      <c r="AL182" s="3">
+        <v>1.2428999999999999</v>
+      </c>
+      <c r="AM182" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="2:39">
       <c r="B183" s="4">
         <v>1994.25</v>
       </c>
@@ -15800,8 +16639,14 @@
       <c r="AK183" s="3">
         <v>2460.3200000000002</v>
       </c>
-    </row>
-    <row r="184" spans="2:37">
+      <c r="AL183" s="3">
+        <v>1.2508999999999999</v>
+      </c>
+      <c r="AM183" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="2:39">
       <c r="B184" s="4">
         <v>1994.5</v>
       </c>
@@ -15910,8 +16755,14 @@
       <c r="AK184" s="3">
         <v>2508.239</v>
       </c>
-    </row>
-    <row r="185" spans="2:37">
+      <c r="AL184" s="3">
+        <v>1.2150000000000001</v>
+      </c>
+      <c r="AM184" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="2:39">
       <c r="B185" s="4">
         <v>1994.75</v>
       </c>
@@ -16020,8 +16871,14 @@
       <c r="AK185" s="3">
         <v>2544.7040000000002</v>
       </c>
-    </row>
-    <row r="186" spans="2:37">
+      <c r="AL185" s="3">
+        <v>1.2815000000000001</v>
+      </c>
+      <c r="AM185" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="2:39">
       <c r="B186" s="4">
         <v>1995</v>
       </c>
@@ -16130,8 +16987,14 @@
       <c r="AK186" s="3">
         <v>2582.4229999999998</v>
       </c>
-    </row>
-    <row r="187" spans="2:37">
+      <c r="AL186" s="3">
+        <v>1.2770999999999999</v>
+      </c>
+      <c r="AM186" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="2:39">
       <c r="B187" s="4">
         <v>1995.25</v>
       </c>
@@ -16240,8 +17103,14 @@
       <c r="AK187" s="3">
         <v>2610.5210000000002</v>
       </c>
-    </row>
-    <row r="188" spans="2:37">
+      <c r="AL187" s="3">
+        <v>1.3073999999999999</v>
+      </c>
+      <c r="AM187" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="2:39">
       <c r="B188" s="4">
         <v>1995.5</v>
       </c>
@@ -16350,8 +17219,14 @@
       <c r="AK188" s="3">
         <v>2598.7829999999999</v>
       </c>
-    </row>
-    <row r="189" spans="2:37">
+      <c r="AL188" s="3">
+        <v>1.3132999999999999</v>
+      </c>
+      <c r="AM188" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="2:39">
       <c r="B189" s="4">
         <v>1995.75</v>
       </c>
@@ -16460,8 +17335,14 @@
       <c r="AK189" s="3">
         <v>2615.3960000000002</v>
       </c>
-    </row>
-    <row r="190" spans="2:37">
+      <c r="AL189" s="3">
+        <v>1.4167000000000001</v>
+      </c>
+      <c r="AM189" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="2:39">
       <c r="B190" s="4">
         <v>1996</v>
       </c>
@@ -16570,8 +17451,14 @@
       <c r="AK190" s="3">
         <v>2669.9789999999998</v>
       </c>
-    </row>
-    <row r="191" spans="2:37">
+      <c r="AL190" s="3">
+        <v>1.3314999999999999</v>
+      </c>
+      <c r="AM190" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="2:39">
       <c r="B191" s="4">
         <v>1996.25</v>
       </c>
@@ -16680,8 +17567,14 @@
       <c r="AK191" s="3">
         <v>2695.1970000000001</v>
       </c>
-    </row>
-    <row r="192" spans="2:37">
+      <c r="AL191" s="3">
+        <v>1.2784</v>
+      </c>
+      <c r="AM191" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="2:39">
       <c r="B192" s="4">
         <v>1996.5</v>
       </c>
@@ -16790,8 +17683,14 @@
       <c r="AK192" s="3">
         <v>2701.8009999999999</v>
       </c>
-    </row>
-    <row r="193" spans="2:37">
+      <c r="AL192" s="3">
+        <v>1.2848999999999999</v>
+      </c>
+      <c r="AM192" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="2:39">
       <c r="B193" s="4">
         <v>1996.75</v>
       </c>
@@ -16900,8 +17799,14 @@
       <c r="AK193" s="3">
         <v>2720.88</v>
       </c>
-    </row>
-    <row r="194" spans="2:37">
+      <c r="AL193" s="3">
+        <v>1.3058000000000001</v>
+      </c>
+      <c r="AM193" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="2:39">
       <c r="B194" s="4">
         <v>1997</v>
       </c>
@@ -17010,8 +17915,14 @@
       <c r="AK194" s="3">
         <v>2740.5309999999999</v>
       </c>
-    </row>
-    <row r="195" spans="2:37">
+      <c r="AL194" s="3">
+        <v>1.2424999999999999</v>
+      </c>
+      <c r="AM194" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="2:39">
       <c r="B195" s="4">
         <v>1997.25</v>
       </c>
@@ -17120,8 +18031,14 @@
       <c r="AK195" s="3">
         <v>2741.5520000000001</v>
       </c>
-    </row>
-    <row r="196" spans="2:37">
+      <c r="AL195" s="3">
+        <v>1.1975</v>
+      </c>
+      <c r="AM195" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="2:39">
       <c r="B196" s="4">
         <v>1997.5</v>
       </c>
@@ -17230,8 +18147,14 @@
       <c r="AK196" s="3">
         <v>2784.9659999999999</v>
       </c>
-    </row>
-    <row r="197" spans="2:37">
+      <c r="AL196" s="3">
+        <v>1.2225999999999999</v>
+      </c>
+      <c r="AM196" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="2:39">
       <c r="B197" s="4">
         <v>1997.75</v>
       </c>
@@ -17340,8 +18263,14 @@
       <c r="AK197" s="3">
         <v>2822.3620000000001</v>
       </c>
-    </row>
-    <row r="198" spans="2:37">
+      <c r="AL197" s="3">
+        <v>1.3562000000000001</v>
+      </c>
+      <c r="AM197" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="2:39">
       <c r="B198" s="4">
         <v>1998</v>
       </c>
@@ -17450,8 +18379,14 @@
       <c r="AK198" s="3">
         <v>2809.4340000000002</v>
       </c>
-    </row>
-    <row r="199" spans="2:37">
+      <c r="AL198" s="3">
+        <v>1.3443000000000001</v>
+      </c>
+      <c r="AM198" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="2:39">
       <c r="B199" s="4">
         <v>1998.25</v>
       </c>
@@ -17560,8 +18495,14 @@
       <c r="AK199" s="3">
         <v>2837.5010000000002</v>
       </c>
-    </row>
-    <row r="200" spans="2:37">
+      <c r="AL199" s="3">
+        <v>1.3249</v>
+      </c>
+      <c r="AM199" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="2:39">
       <c r="B200" s="4">
         <v>1998.5</v>
       </c>
@@ -17670,8 +18611,14 @@
       <c r="AK200" s="3">
         <v>2866.201</v>
       </c>
-    </row>
-    <row r="201" spans="2:37">
+      <c r="AL200" s="3">
+        <v>2.0169000000000001</v>
+      </c>
+      <c r="AM200" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="2:39">
       <c r="B201" s="4">
         <v>1998.75</v>
       </c>
@@ -17780,8 +18727,14 @@
       <c r="AK201" s="3">
         <v>2909.2220000000002</v>
       </c>
-    </row>
-    <row r="202" spans="2:37">
+      <c r="AL201" s="3">
+        <v>2.1269</v>
+      </c>
+      <c r="AM201" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="2:39">
       <c r="B202" s="4">
         <v>1999</v>
       </c>
@@ -17890,8 +18843,14 @@
       <c r="AK202" s="3">
         <v>2931.922</v>
       </c>
-    </row>
-    <row r="203" spans="2:37">
+      <c r="AL202" s="3">
+        <v>1.833</v>
+      </c>
+      <c r="AM202" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="2:39">
       <c r="B203" s="4">
         <v>1999.25</v>
       </c>
@@ -18000,8 +18959,14 @@
       <c r="AK203" s="3">
         <v>2960.587</v>
       </c>
-    </row>
-    <row r="204" spans="2:37">
+      <c r="AL203" s="3">
+        <v>1.7621</v>
+      </c>
+      <c r="AM203" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="2:39">
       <c r="B204" s="4">
         <v>1999.5</v>
       </c>
@@ -18110,8 +19075,14 @@
       <c r="AK204" s="3">
         <v>3003.4059999999999</v>
       </c>
-    </row>
-    <row r="205" spans="2:37">
+      <c r="AL204" s="3">
+        <v>2.0268999999999999</v>
+      </c>
+      <c r="AM204" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="2:39">
       <c r="B205" s="4">
         <v>1999.75</v>
       </c>
@@ -18220,8 +19191,14 @@
       <c r="AK205" s="3">
         <v>3087.3989999999999</v>
       </c>
-    </row>
-    <row r="206" spans="2:37">
+      <c r="AL205" s="3">
+        <v>2.0446</v>
+      </c>
+      <c r="AM205" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="2:39">
       <c r="B206" s="4">
         <v>2000</v>
       </c>
@@ -18330,8 +19307,14 @@
       <c r="AK206" s="3">
         <v>3075.69</v>
       </c>
-    </row>
-    <row r="207" spans="2:37">
+      <c r="AL206" s="3">
+        <v>2.3315999999999999</v>
+      </c>
+      <c r="AM206" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="2:39">
       <c r="B207" s="4">
         <v>2000.25</v>
       </c>
@@ -18440,8 +19423,14 @@
       <c r="AK207" s="3">
         <v>3132.4560000000001</v>
       </c>
-    </row>
-    <row r="208" spans="2:37">
+      <c r="AL207" s="3">
+        <v>2.835</v>
+      </c>
+      <c r="AM207" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="2:39">
       <c r="B208" s="4">
         <v>2000.5</v>
       </c>
@@ -18550,8 +19539,14 @@
       <c r="AK208" s="3">
         <v>3152.7979999999998</v>
       </c>
-    </row>
-    <row r="209" spans="2:37">
+      <c r="AL208" s="3">
+        <v>3.2391999999999999</v>
+      </c>
+      <c r="AM208" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="2:39">
       <c r="B209" s="4">
         <v>2000.75</v>
       </c>
@@ -18660,8 +19655,14 @@
       <c r="AK209" s="3">
         <v>3207.261</v>
       </c>
-    </row>
-    <row r="210" spans="2:37">
+      <c r="AL209" s="3">
+        <v>3.6334</v>
+      </c>
+      <c r="AM209" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="2:39">
       <c r="B210" s="4">
         <v>2001</v>
       </c>
@@ -18770,8 +19771,14 @@
       <c r="AK210" s="3">
         <v>3280.6959999999999</v>
       </c>
-    </row>
-    <row r="211" spans="2:37">
+      <c r="AL210" s="3">
+        <v>3.2886000000000002</v>
+      </c>
+      <c r="AM210" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="2:39">
       <c r="B211" s="4">
         <v>2001.25</v>
       </c>
@@ -18880,8 +19887,14 @@
       <c r="AK211" s="3">
         <v>3358.6410000000001</v>
       </c>
-    </row>
-    <row r="212" spans="2:37">
+      <c r="AL211" s="3">
+        <v>3.1236000000000002</v>
+      </c>
+      <c r="AM211" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="2:39">
       <c r="B212" s="4">
         <v>2001.5</v>
       </c>
@@ -18990,8 +20003,14 @@
       <c r="AK212" s="3">
         <v>3375.623</v>
       </c>
-    </row>
-    <row r="213" spans="2:37">
+      <c r="AL212" s="3">
+        <v>3.3347000000000002</v>
+      </c>
+      <c r="AM212" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="2:39">
       <c r="B213" s="4">
         <v>2001.75</v>
       </c>
@@ -19100,8 +20119,14 @@
       <c r="AK213" s="3">
         <v>3434.6640000000002</v>
       </c>
-    </row>
-    <row r="214" spans="2:37">
+      <c r="AL213" s="3">
+        <v>3.0945</v>
+      </c>
+      <c r="AM213" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="214" spans="2:39">
       <c r="B214" s="4">
         <v>2002</v>
       </c>
@@ -19210,8 +20235,14 @@
       <c r="AK214" s="3">
         <v>3506.482</v>
       </c>
-    </row>
-    <row r="215" spans="2:37">
+      <c r="AL214" s="3">
+        <v>2.7568000000000001</v>
+      </c>
+      <c r="AM214" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="2:39">
       <c r="B215" s="4">
         <v>2002.25</v>
       </c>
@@ -19320,8 +20351,14 @@
       <c r="AK215" s="3">
         <v>3554.2069999999999</v>
       </c>
-    </row>
-    <row r="216" spans="2:37">
+      <c r="AL215" s="3">
+        <v>3.1526999999999998</v>
+      </c>
+      <c r="AM215" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="2:39">
       <c r="B216" s="4">
         <v>2002.5</v>
       </c>
@@ -19430,8 +20467,14 @@
       <c r="AK216" s="3">
         <v>3596.9650000000001</v>
       </c>
-    </row>
-    <row r="217" spans="2:37">
+      <c r="AL216" s="3">
+        <v>4.1440999999999999</v>
+      </c>
+      <c r="AM216" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="2:39">
       <c r="B217" s="4">
         <v>2002.75</v>
       </c>
@@ -19540,8 +20583,14 @@
       <c r="AK217" s="3">
         <v>3683.1709999999998</v>
       </c>
-    </row>
-    <row r="218" spans="2:37">
+      <c r="AL217" s="3">
+        <v>3.87</v>
+      </c>
+      <c r="AM217" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="2:39">
       <c r="B218" s="4">
         <v>2003</v>
       </c>
@@ -19650,8 +20699,14 @@
       <c r="AK218" s="3">
         <v>3747.962</v>
       </c>
-    </row>
-    <row r="219" spans="2:37">
+      <c r="AL218" s="3">
+        <v>3.2366999999999999</v>
+      </c>
+      <c r="AM218" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="2:39">
       <c r="B219" s="4">
         <v>2003.25</v>
       </c>
@@ -19760,8 +20815,14 @@
       <c r="AK219" s="3">
         <v>3806.8409999999999</v>
       </c>
-    </row>
-    <row r="220" spans="2:37">
+      <c r="AL219" s="3">
+        <v>2.6349999999999998</v>
+      </c>
+      <c r="AM219" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="2:39">
       <c r="B220" s="4">
         <v>2003.5</v>
       </c>
@@ -19870,8 +20931,14 @@
       <c r="AK220" s="3">
         <v>3837.3429999999998</v>
       </c>
-    </row>
-    <row r="221" spans="2:37">
+      <c r="AL220" s="3">
+        <v>2.359</v>
+      </c>
+      <c r="AM220" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="2:39">
       <c r="B221" s="4">
         <v>2003.75</v>
       </c>
@@ -19980,8 +21047,14 @@
       <c r="AK221" s="3">
         <v>3872.2370000000001</v>
       </c>
-    </row>
-    <row r="222" spans="2:37">
+      <c r="AL221" s="3">
+        <v>1.982</v>
+      </c>
+      <c r="AM221" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="2:39">
       <c r="B222" s="4">
         <v>2004</v>
       </c>
@@ -20090,8 +21163,14 @@
       <c r="AK222" s="3">
         <v>3951.5810000000001</v>
       </c>
-    </row>
-    <row r="223" spans="2:37">
+      <c r="AL222" s="3">
+        <v>1.8884000000000001</v>
+      </c>
+      <c r="AM222" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="2:39">
       <c r="B223" s="4">
         <v>2004.25</v>
       </c>
@@ -20200,8 +21279,14 @@
       <c r="AK223" s="3">
         <v>3981.4940000000001</v>
       </c>
-    </row>
-    <row r="224" spans="2:37">
+      <c r="AL223" s="3">
+        <v>1.8445</v>
+      </c>
+      <c r="AM223" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="2:39">
       <c r="B224" s="4">
         <v>2004.5</v>
       </c>
@@ -20310,8 +21395,14 @@
       <c r="AK224" s="3">
         <v>4049.4580000000001</v>
       </c>
-    </row>
-    <row r="225" spans="2:37">
+      <c r="AL224" s="3">
+        <v>1.8208</v>
+      </c>
+      <c r="AM224" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="2:39">
       <c r="B225" s="4">
         <v>2004.75</v>
       </c>
@@ -20420,8 +21511,14 @@
       <c r="AK225" s="3">
         <v>4095.1129999999998</v>
       </c>
-    </row>
-    <row r="226" spans="2:37">
+      <c r="AL225" s="3">
+        <v>1.6519999999999999</v>
+      </c>
+      <c r="AM225" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="2:39">
       <c r="B226" s="4">
         <v>2005</v>
       </c>
@@ -20530,8 +21627,14 @@
       <c r="AK226" s="3">
         <v>4195.5519999999997</v>
       </c>
-    </row>
-    <row r="227" spans="2:37">
+      <c r="AL226" s="3">
+        <v>1.8519000000000001</v>
+      </c>
+      <c r="AM226" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="2:39">
       <c r="B227" s="4">
         <v>2005.25</v>
       </c>
@@ -20640,8 +21743,14 @@
       <c r="AK227" s="3">
         <v>4239.652</v>
       </c>
-    </row>
-    <row r="228" spans="2:37">
+      <c r="AL227" s="3">
+        <v>1.9699</v>
+      </c>
+      <c r="AM227" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="2:39">
       <c r="B228" s="4">
         <v>2005.5</v>
       </c>
@@ -20750,8 +21859,14 @@
       <c r="AK228" s="3">
         <v>4364.34</v>
       </c>
-    </row>
-    <row r="229" spans="2:37">
+      <c r="AL228" s="3">
+        <v>1.7806999999999999</v>
+      </c>
+      <c r="AM228" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="2:39">
       <c r="B229" s="4">
         <v>2005.75</v>
       </c>
@@ -20860,8 +21975,14 @@
       <c r="AK229" s="3">
         <v>4414.4449999999997</v>
       </c>
-    </row>
-    <row r="230" spans="2:37">
+      <c r="AL229" s="3">
+        <v>1.8502000000000001</v>
+      </c>
+      <c r="AM229" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="2:39">
       <c r="B230" s="4">
         <v>2006</v>
       </c>
@@ -20970,8 +22091,14 @@
       <c r="AK230" s="3">
         <v>4453.6220000000003</v>
       </c>
-    </row>
-    <row r="231" spans="2:37">
+      <c r="AL230" s="3">
+        <v>1.6903999999999999</v>
+      </c>
+      <c r="AM230" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="2:39">
       <c r="B231" s="4">
         <v>2006.25</v>
       </c>
@@ -21080,8 +22207,14 @@
       <c r="AK231" s="3">
         <v>4516.5510000000004</v>
       </c>
-    </row>
-    <row r="232" spans="2:37">
+      <c r="AL231" s="3">
+        <v>1.6846000000000001</v>
+      </c>
+      <c r="AM231" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="2:39">
       <c r="B232" s="4">
         <v>2006.5</v>
       </c>
@@ -21190,8 +22323,14 @@
       <c r="AK232" s="3">
         <v>4563.9780000000001</v>
       </c>
-    </row>
-    <row r="233" spans="2:37">
+      <c r="AL232" s="3">
+        <v>1.772</v>
+      </c>
+      <c r="AM232" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="2:39">
       <c r="B233" s="4">
         <v>2006.75</v>
       </c>
@@ -21300,8 +22439,14 @@
       <c r="AK233" s="3">
         <v>4545.7259999999997</v>
       </c>
-    </row>
-    <row r="234" spans="2:37">
+      <c r="AL233" s="3">
+        <v>1.6173999999999999</v>
+      </c>
+      <c r="AM233" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="2:39">
       <c r="B234" s="4">
         <v>2007</v>
       </c>
@@ -21410,8 +22555,14 @@
       <c r="AK234" s="3">
         <v>4752.1880000000001</v>
       </c>
-    </row>
-    <row r="235" spans="2:37">
+      <c r="AL234" s="3">
+        <v>1.5329999999999999</v>
+      </c>
+      <c r="AM234" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="2:39">
       <c r="B235" s="4">
         <v>2007.25</v>
       </c>
@@ -21520,8 +22671,14 @@
       <c r="AK235" s="3">
         <v>4801.8549999999996</v>
       </c>
-    </row>
-    <row r="236" spans="2:37">
+      <c r="AL235" s="3">
+        <v>1.6978</v>
+      </c>
+      <c r="AM235" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="2:39">
       <c r="B236" s="4">
         <v>2007.5</v>
       </c>
@@ -21630,8 +22787,14 @@
       <c r="AK236" s="3">
         <v>4849.2650000000003</v>
       </c>
-    </row>
-    <row r="237" spans="2:37">
+      <c r="AL236" s="3">
+        <v>2.2343999999999999</v>
+      </c>
+      <c r="AM236" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="2:39">
       <c r="B237" s="4">
         <v>2007.75</v>
       </c>
@@ -21740,8 +22903,14 @@
       <c r="AK237" s="3">
         <v>4931.232</v>
       </c>
-    </row>
-    <row r="238" spans="2:37">
+      <c r="AL237" s="3">
+        <v>2.7972999999999999</v>
+      </c>
+      <c r="AM237" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="2:39">
       <c r="B238" s="4">
         <v>2008</v>
       </c>
@@ -21850,8 +23019,14 @@
       <c r="AK238" s="3">
         <v>5000.1760000000004</v>
       </c>
-    </row>
-    <row r="239" spans="2:37">
+      <c r="AL238" s="3">
+        <v>3.5019999999999998</v>
+      </c>
+      <c r="AM238" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="2:39">
       <c r="B239" s="4">
         <v>2008.25</v>
       </c>
@@ -21960,8 +23135,14 @@
       <c r="AK239" s="3">
         <v>5365.0709999999999</v>
       </c>
-    </row>
-    <row r="240" spans="2:37">
+      <c r="AL239" s="3">
+        <v>3.4013</v>
+      </c>
+      <c r="AM239" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="2:39">
       <c r="B240" s="4">
         <v>2008.5</v>
       </c>
@@ -22070,8 +23251,14 @@
       <c r="AK240" s="3">
         <v>5258.6</v>
       </c>
-    </row>
-    <row r="241" spans="2:37">
+      <c r="AL240" s="3">
+        <v>4.8465999999999996</v>
+      </c>
+      <c r="AM240" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="2:39">
       <c r="B241" s="4">
         <v>2008.75</v>
       </c>
@@ -22180,8 +23367,14 @@
       <c r="AK241" s="3">
         <v>5419.0320000000002</v>
       </c>
-    </row>
-    <row r="242" spans="2:37">
+      <c r="AL241" s="3">
+        <v>7.2518000000000002</v>
+      </c>
+      <c r="AM241" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="2:39">
       <c r="B242" s="4">
         <v>2009</v>
       </c>
@@ -22290,8 +23483,14 @@
       <c r="AK242" s="3">
         <v>5486.3149999999996</v>
       </c>
-    </row>
-    <row r="243" spans="2:37">
+      <c r="AL242" s="3">
+        <v>6.0926</v>
+      </c>
+      <c r="AM242" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="2:39">
       <c r="B243" s="4">
         <v>2009.25</v>
       </c>
@@ -22400,8 +23599,14 @@
       <c r="AK243" s="3">
         <v>5682.232</v>
       </c>
-    </row>
-    <row r="244" spans="2:37">
+      <c r="AL243" s="3">
+        <v>4.5029000000000003</v>
+      </c>
+      <c r="AM243" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="2:39">
       <c r="B244" s="4">
         <v>2009.5</v>
       </c>
@@ -22510,8 +23715,14 @@
       <c r="AK244" s="3">
         <v>5655.2539999999999</v>
       </c>
-    </row>
-    <row r="245" spans="2:37">
+      <c r="AL244" s="3">
+        <v>3.1901999999999999</v>
+      </c>
+      <c r="AM244" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="2:39">
       <c r="B245" s="4">
         <v>2009.75</v>
       </c>
@@ -22620,8 +23831,14 @@
       <c r="AK245" s="3">
         <v>5713.1570000000002</v>
       </c>
-    </row>
-    <row r="246" spans="2:37">
+      <c r="AL245" s="3">
+        <v>2.6547999999999998</v>
+      </c>
+      <c r="AM245" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="2:39">
       <c r="B246" s="4">
         <v>2010</v>
       </c>
@@ -22730,8 +23947,14 @@
       <c r="AK246" s="3">
         <v>5820.3990000000003</v>
       </c>
-    </row>
-    <row r="247" spans="2:37">
+      <c r="AL246" s="3">
+        <v>2.3338000000000001</v>
+      </c>
+      <c r="AM246" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="2:39">
       <c r="B247" s="4">
         <v>2010.25</v>
       </c>
@@ -22840,8 +24063,14 @@
       <c r="AK247" s="3">
         <v>5862.866</v>
       </c>
-    </row>
-    <row r="248" spans="2:37">
+      <c r="AL247" s="3">
+        <v>2.5171999999999999</v>
+      </c>
+      <c r="AM247" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="2:39">
       <c r="B248" s="4">
         <v>2010.5</v>
       </c>
@@ -22950,8 +24179,14 @@
       <c r="AK248" s="3">
         <v>5811.1440000000002</v>
       </c>
-    </row>
-    <row r="249" spans="2:37">
+      <c r="AL248" s="3">
+        <v>2.5743</v>
+      </c>
+      <c r="AM248" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="2:39">
       <c r="B249" s="4">
         <v>2010.75</v>
       </c>
@@ -23060,8 +24295,14 @@
       <c r="AK249" s="3">
         <v>5839.37</v>
       </c>
-    </row>
-    <row r="250" spans="2:37">
+      <c r="AL249" s="3">
+        <v>2.3157999999999999</v>
+      </c>
+      <c r="AM249" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="2:39">
       <c r="B250" s="4">
         <v>2011</v>
       </c>
@@ -23170,8 +24411,14 @@
       <c r="AK250" s="3">
         <v>5859.5</v>
       </c>
-    </row>
-    <row r="251" spans="2:37">
+      <c r="AL250" s="3">
+        <v>2.0299</v>
+      </c>
+      <c r="AM250" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="2:39">
       <c r="B251" s="4">
         <v>2011.25</v>
       </c>
@@ -23280,8 +24527,14 @@
       <c r="AK251" s="3">
         <v>5918.37</v>
       </c>
-    </row>
-    <row r="252" spans="2:37">
+      <c r="AL251" s="3">
+        <v>2.1107</v>
+      </c>
+      <c r="AM251" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="2:39">
       <c r="B252" s="4">
         <v>2011.5</v>
       </c>
@@ -23390,8 +24643,14 @@
       <c r="AK252" s="3">
         <v>5837.9179999999997</v>
       </c>
-    </row>
-    <row r="253" spans="2:37">
+      <c r="AL252" s="3">
+        <v>2.7482000000000002</v>
+      </c>
+      <c r="AM252" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="2:39">
       <c r="B253" s="4">
         <v>2011.75</v>
       </c>
@@ -23500,8 +24759,14 @@
       <c r="AK253" s="3">
         <v>5872.701</v>
       </c>
-    </row>
-    <row r="254" spans="2:37">
+      <c r="AL253" s="3">
+        <v>2.8654000000000002</v>
+      </c>
+      <c r="AM253" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="2:39">
       <c r="B254" s="4">
         <v>2012</v>
       </c>
@@ -23610,8 +24875,14 @@
       <c r="AK254" s="3">
         <v>5834.96</v>
       </c>
-    </row>
-    <row r="255" spans="2:37">
+      <c r="AL254" s="3">
+        <v>2.5446</v>
+      </c>
+      <c r="AM254" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="2:39">
       <c r="B255" s="4">
         <v>2012.25</v>
       </c>
@@ -23720,8 +24991,14 @@
       <c r="AK255" s="3">
         <v>5831.6850000000004</v>
       </c>
-    </row>
-    <row r="256" spans="2:37">
+      <c r="AL255" s="3">
+        <v>2.6608999999999998</v>
+      </c>
+      <c r="AM255" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="2:39">
       <c r="B256" s="4">
         <v>2012.5</v>
       </c>
@@ -23830,8 +25107,14 @@
       <c r="AK256" s="3">
         <v>5801.4059999999999</v>
       </c>
-    </row>
-    <row r="257" spans="2:37">
+      <c r="AL256" s="3">
+        <v>2.4359999999999999</v>
+      </c>
+      <c r="AM256" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="2:39">
       <c r="B257" s="4">
         <v>2012.75</v>
       </c>
@@ -23940,8 +25223,14 @@
       <c r="AK257" s="3">
         <v>5901.7049999999999</v>
       </c>
-    </row>
-    <row r="258" spans="2:37">
+      <c r="AL257" s="3">
+        <v>2.2204999999999999</v>
+      </c>
+      <c r="AM257" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="2:39">
       <c r="B258" s="4">
         <v>2013</v>
       </c>
@@ -24050,8 +25339,14 @@
       <c r="AK258" s="3">
         <v>5832.0619999999999</v>
       </c>
-    </row>
-    <row r="259" spans="2:37">
+      <c r="AL258" s="3">
+        <v>2.1053999999999999</v>
+      </c>
+      <c r="AM258" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="2:39">
       <c r="B259" s="4">
         <v>2013.25</v>
       </c>
@@ -24160,8 +25455,14 @@
       <c r="AK259" s="3">
         <v>5848.9759999999997</v>
       </c>
-    </row>
-    <row r="260" spans="2:37">
+      <c r="AL259" s="3">
+        <v>2.0493000000000001</v>
+      </c>
+      <c r="AM259" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="2:39">
       <c r="B260" s="4">
         <v>2013.5</v>
       </c>
@@ -24270,8 +25571,14 @@
       <c r="AK260" s="3">
         <v>5867.3109999999997</v>
       </c>
-    </row>
-    <row r="261" spans="2:37">
+      <c r="AL260" s="3">
+        <v>2.0004</v>
+      </c>
+      <c r="AM260" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="2:39">
       <c r="B261" s="4">
         <v>2013.75</v>
       </c>
@@ -24380,8 +25687,14 @@
       <c r="AK261" s="3">
         <v>5868.1459999999997</v>
       </c>
-    </row>
-    <row r="262" spans="2:37">
+      <c r="AL261" s="3">
+        <v>1.8586</v>
+      </c>
+      <c r="AM261" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="2:39">
       <c r="B262" s="4">
         <v>2014</v>
       </c>
@@ -24490,8 +25803,14 @@
       <c r="AK262" s="3">
         <v>5917.5379999999996</v>
       </c>
-    </row>
-    <row r="263" spans="2:37">
+      <c r="AL262" s="3">
+        <v>1.6918</v>
+      </c>
+      <c r="AM262" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="2:39">
       <c r="B263" s="4">
         <v>2014.25</v>
       </c>
@@ -24600,8 +25919,14 @@
       <c r="AK263" s="3">
         <v>5978.7539999999999</v>
       </c>
-    </row>
-    <row r="264" spans="2:37">
+      <c r="AL263" s="3">
+        <v>1.5889</v>
+      </c>
+      <c r="AM263" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="2:39">
       <c r="B264" s="4">
         <v>2014.5</v>
       </c>
@@ -24710,8 +26035,14 @@
       <c r="AK264" s="3">
         <v>6040.7809999999999</v>
       </c>
-    </row>
-    <row r="265" spans="2:37">
+      <c r="AL264" s="3">
+        <v>1.6941999999999999</v>
+      </c>
+      <c r="AM264" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="2:39">
       <c r="B265" s="4">
         <v>2014.75</v>
       </c>
@@ -24820,8 +26151,14 @@
       <c r="AK265" s="3">
         <v>6063.4409999999998</v>
       </c>
-    </row>
-    <row r="266" spans="2:37">
+      <c r="AL265" s="3">
+        <v>1.9925999999999999</v>
+      </c>
+      <c r="AM265" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="2:39">
       <c r="B266" s="4">
         <v>2015</v>
       </c>
@@ -24930,8 +26267,14 @@
       <c r="AK266" s="3">
         <v>6066.7039999999997</v>
       </c>
-    </row>
-    <row r="267" spans="2:37">
+      <c r="AL266" s="3">
+        <v>2.0068999999999999</v>
+      </c>
+      <c r="AM266" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="2:39">
       <c r="B267" s="4">
         <v>2015.25</v>
       </c>
@@ -25040,8 +26383,14 @@
       <c r="AK267" s="3">
         <v>6083.6419999999998</v>
       </c>
-    </row>
-    <row r="268" spans="2:37">
+      <c r="AL267" s="3">
+        <v>2.0863999999999998</v>
+      </c>
+      <c r="AM267" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="2:39">
       <c r="B268" s="4">
         <v>2015.5</v>
       </c>
@@ -25150,8 +26499,14 @@
       <c r="AK268" s="3">
         <v>6263.4809999999998</v>
       </c>
-    </row>
-    <row r="269" spans="2:37">
+      <c r="AL268" s="3">
+        <v>2.3969999999999998</v>
+      </c>
+      <c r="AM268" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="2:39">
       <c r="B269" s="4">
         <v>2015.75</v>
       </c>
@@ -25260,8 +26615,14 @@
       <c r="AK269" s="3">
         <v>6235.098</v>
       </c>
-    </row>
-    <row r="270" spans="2:37">
+      <c r="AL269" s="3">
+        <v>2.6116000000000001</v>
+      </c>
+      <c r="AM269" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="2:39">
       <c r="B270" s="4">
         <v>2016</v>
       </c>
@@ -25370,8 +26731,14 @@
       <c r="AK270" s="3">
         <v>6305.14</v>
       </c>
-    </row>
-    <row r="271" spans="2:37">
+      <c r="AL270" s="3">
+        <v>2.6930000000000001</v>
+      </c>
+      <c r="AM270" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="2:39">
       <c r="B271" s="4">
         <v>2016.25</v>
       </c>
@@ -25480,8 +26847,14 @@
       <c r="AK271" s="3">
         <v>6309.7030000000004</v>
       </c>
-    </row>
-    <row r="272" spans="2:37">
+      <c r="AL271" s="3">
+        <v>2.0855000000000001</v>
+      </c>
+      <c r="AM271" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="2:39">
       <c r="B272" s="4">
         <v>2016.5</v>
       </c>
@@ -25590,8 +26963,11 @@
       <c r="AK272" s="3">
         <v>6400.8850000000002</v>
       </c>
-    </row>
-    <row r="273" spans="2:37">
+      <c r="AM272" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="2:39">
       <c r="B273" s="4">
         <v>2016.75</v>
       </c>
@@ -25700,8 +27076,11 @@
       <c r="AK273" s="3">
         <v>6451.5810000000001</v>
       </c>
-    </row>
-    <row r="274" spans="2:37">
+      <c r="AM273" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="2:39">
       <c r="B274" s="4">
         <v>2017</v>
       </c>
@@ -25810,8 +27189,11 @@
       <c r="AK274" s="3">
         <v>6510.5370000000003</v>
       </c>
-    </row>
-    <row r="275" spans="2:37">
+      <c r="AM274" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="2:39">
       <c r="B275" s="4">
         <v>2017.25</v>
       </c>
@@ -25920,8 +27302,11 @@
       <c r="AK275" s="3">
         <v>6500.1409999999996</v>
       </c>
-    </row>
-    <row r="276" spans="2:37">
+      <c r="AM275" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="2:39">
       <c r="B276" s="4">
         <v>2017.5</v>
       </c>
@@ -26030,8 +27415,11 @@
       <c r="AK276" s="3">
         <v>6631.2030000000004</v>
       </c>
-    </row>
-    <row r="277" spans="2:37">
+      <c r="AM276" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="2:39">
       <c r="B277" s="4">
         <v>2017.75</v>
       </c>
@@ -26140,8 +27528,11 @@
       <c r="AK277" s="3">
         <v>6677.11</v>
       </c>
-    </row>
-    <row r="278" spans="2:37">
+      <c r="AM277" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="2:39">
       <c r="B278" s="4">
         <v>2018</v>
       </c>
@@ -26250,8 +27641,11 @@
       <c r="AK278" s="3">
         <v>6742.7</v>
       </c>
-    </row>
-    <row r="279" spans="2:37">
+      <c r="AM278" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="2:39">
       <c r="B279" s="4">
         <v>2018.25</v>
       </c>
@@ -26354,8 +27748,11 @@
       <c r="AK279" s="3">
         <v>6830.1419999999998</v>
       </c>
-    </row>
-    <row r="280" spans="2:37">
+      <c r="AM279" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="2:39">
       <c r="B280" s="4">
         <v>2018.5</v>
       </c>
@@ -26384,8 +27781,9 @@
       <c r="AI280" s="3"/>
       <c r="AJ280" s="3"/>
       <c r="AK280" s="3"/>
-    </row>
-    <row r="281" spans="2:37">
+      <c r="AM280" s="3"/>
+    </row>
+    <row r="281" spans="2:39">
       <c r="B281" s="4">
         <v>2018.75</v>
       </c>
@@ -26413,8 +27811,9 @@
       <c r="AI281" s="3"/>
       <c r="AJ281" s="3"/>
       <c r="AK281" s="3"/>
-    </row>
-    <row r="282" spans="2:37">
+      <c r="AM281" s="3"/>
+    </row>
+    <row r="282" spans="2:39">
       <c r="N282" s="3"/>
       <c r="O282" s="3"/>
       <c r="U282" s="3"/>
@@ -26434,8 +27833,9 @@
       <c r="AI282" s="3"/>
       <c r="AJ282" s="3"/>
       <c r="AK282" s="3"/>
-    </row>
-    <row r="283" spans="2:37">
+      <c r="AM282" s="3"/>
+    </row>
+    <row r="283" spans="2:39">
       <c r="N283" s="3"/>
       <c r="O283" s="3"/>
       <c r="U283" s="3"/>
@@ -26455,8 +27855,9 @@
       <c r="AI283" s="3"/>
       <c r="AJ283" s="3"/>
       <c r="AK283" s="3"/>
-    </row>
-    <row r="284" spans="2:37">
+      <c r="AM283" s="3"/>
+    </row>
+    <row r="284" spans="2:39">
       <c r="N284" s="3"/>
       <c r="O284" s="3"/>
       <c r="U284" s="3"/>
@@ -26476,8 +27877,9 @@
       <c r="AI284" s="3"/>
       <c r="AJ284" s="3"/>
       <c r="AK284" s="3"/>
-    </row>
-    <row r="285" spans="2:37">
+      <c r="AM284" s="3"/>
+    </row>
+    <row r="285" spans="2:39">
       <c r="N285" s="3"/>
       <c r="O285" s="3"/>
       <c r="U285" s="3"/>
@@ -26497,8 +27899,9 @@
       <c r="AI285" s="3"/>
       <c r="AJ285" s="3"/>
       <c r="AK285" s="3"/>
-    </row>
-    <row r="286" spans="2:37">
+      <c r="AM285" s="3"/>
+    </row>
+    <row r="286" spans="2:39">
       <c r="N286" s="3"/>
       <c r="O286" s="3"/>
       <c r="U286" s="3"/>
@@ -26518,8 +27921,9 @@
       <c r="AI286" s="3"/>
       <c r="AJ286" s="3"/>
       <c r="AK286" s="3"/>
-    </row>
-    <row r="287" spans="2:37">
+      <c r="AM286" s="3"/>
+    </row>
+    <row r="287" spans="2:39">
       <c r="N287" s="3"/>
       <c r="O287" s="3"/>
       <c r="U287" s="3"/>
@@ -26539,8 +27943,9 @@
       <c r="AI287" s="3"/>
       <c r="AJ287" s="3"/>
       <c r="AK287" s="3"/>
-    </row>
-    <row r="288" spans="2:37">
+      <c r="AM287" s="3"/>
+    </row>
+    <row r="288" spans="2:39">
       <c r="N288" s="3"/>
       <c r="O288" s="3"/>
       <c r="U288" s="3"/>

</xml_diff>

<commit_message>
redoing the exercise with GZ
</commit_message>
<xml_diff>
--- a/Code/Data/Quarterly.xlsx
+++ b/Code/Data/Quarterly.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="111">
   <si>
     <t>Name</t>
   </si>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t>Closing Price - Nominal</t>
-  </si>
-  <si>
-    <t>Mich5Y</t>
   </si>
   <si>
     <t>TFPUtil</t>
@@ -494,7 +491,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -527,9 +524,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -828,10 +822,10 @@
   <dimension ref="A1:BF937"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="AG6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="AH81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AL76" sqref="AL76"/>
+      <selection pane="bottomRight" activeCell="AM24" sqref="AM24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -845,20 +839,19 @@
     <col min="16" max="16" width="21.28515625" style="9" customWidth="1"/>
     <col min="17" max="18" width="22.140625" style="9" customWidth="1"/>
     <col min="19" max="19" width="22.42578125" style="9" customWidth="1"/>
-    <col min="20" max="21" width="22.42578125" style="14" customWidth="1"/>
+    <col min="20" max="21" width="22.42578125" style="13" customWidth="1"/>
     <col min="22" max="30" width="23.85546875" style="9" customWidth="1"/>
     <col min="31" max="35" width="24.28515625" style="9" customWidth="1"/>
     <col min="36" max="38" width="22.140625" style="3" customWidth="1"/>
-    <col min="39" max="39" width="21.28515625" style="3" customWidth="1"/>
+    <col min="39" max="39" width="23.140625" style="3" customWidth="1"/>
     <col min="40" max="40" width="22.140625" style="9" customWidth="1"/>
     <col min="41" max="41" width="22" style="3" customWidth="1"/>
     <col min="42" max="56" width="22.140625" style="9" customWidth="1"/>
     <col min="57" max="57" width="23.140625" style="9" customWidth="1"/>
-    <col min="58" max="58" width="23.140625" style="3" customWidth="1"/>
     <col min="59" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58">
+    <row r="1" spans="1:57">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -896,7 +889,7 @@
         <v>14</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>63</v>
@@ -908,133 +901,130 @@
         <v>57</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ1" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AK1" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL1" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AJ1" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK1" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="AL1" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="AM1" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="AO1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="AP1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AT1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AX1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="BE1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="BF1" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:58">
+    </row>
+    <row r="2" spans="1:57">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1206,11 +1196,8 @@
       <c r="BE2" s="2">
         <v>3</v>
       </c>
-      <c r="BF2" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:58">
+    </row>
+    <row r="3" spans="1:57">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1382,11 +1369,8 @@
       <c r="BE3" s="2">
         <v>1</v>
       </c>
-      <c r="BF3" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:58">
+    </row>
+    <row r="4" spans="1:57">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1558,11 +1542,8 @@
       <c r="BE4" s="2">
         <v>56</v>
       </c>
-      <c r="BF4" s="2">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:58">
+    </row>
+    <row r="5" spans="1:57">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1734,11 +1715,8 @@
       <c r="BE5" s="2">
         <v>56</v>
       </c>
-      <c r="BF5" s="2">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:58">
+    </row>
+    <row r="6" spans="1:57">
       <c r="B6" s="4">
         <v>1950</v>
       </c>
@@ -1798,7 +1776,7 @@
       </c>
       <c r="AL6" s="10"/>
     </row>
-    <row r="7" spans="1:58">
+    <row r="7" spans="1:57">
       <c r="B7" s="4">
         <v>1950.25</v>
       </c>
@@ -1858,7 +1836,7 @@
       </c>
       <c r="AL7" s="10"/>
     </row>
-    <row r="8" spans="1:58">
+    <row r="8" spans="1:57">
       <c r="B8" s="4">
         <v>1950.5</v>
       </c>
@@ -1918,7 +1896,7 @@
       </c>
       <c r="AL8" s="10"/>
     </row>
-    <row r="9" spans="1:58">
+    <row r="9" spans="1:57">
       <c r="B9" s="4">
         <v>1950.75</v>
       </c>
@@ -1978,7 +1956,7 @@
       </c>
       <c r="AL9" s="10"/>
     </row>
-    <row r="10" spans="1:58">
+    <row r="10" spans="1:57">
       <c r="B10" s="4">
         <v>1951</v>
       </c>
@@ -2038,7 +2016,7 @@
       </c>
       <c r="AL10" s="10"/>
     </row>
-    <row r="11" spans="1:58">
+    <row r="11" spans="1:57">
       <c r="B11" s="4">
         <v>1951.25</v>
       </c>
@@ -2098,7 +2076,7 @@
       </c>
       <c r="AL11" s="10"/>
     </row>
-    <row r="12" spans="1:58">
+    <row r="12" spans="1:57">
       <c r="B12" s="4">
         <v>1951.5</v>
       </c>
@@ -2158,7 +2136,7 @@
       </c>
       <c r="AL12" s="10"/>
     </row>
-    <row r="13" spans="1:58">
+    <row r="13" spans="1:57">
       <c r="B13" s="4">
         <v>1951.75</v>
       </c>
@@ -2218,7 +2196,7 @@
       </c>
       <c r="AL13" s="10"/>
     </row>
-    <row r="14" spans="1:58">
+    <row r="14" spans="1:57">
       <c r="B14" s="4">
         <v>1952</v>
       </c>
@@ -2281,7 +2259,7 @@
       </c>
       <c r="AL14" s="10"/>
     </row>
-    <row r="15" spans="1:58">
+    <row r="15" spans="1:57">
       <c r="B15" s="4">
         <v>1952.25</v>
       </c>
@@ -2344,7 +2322,7 @@
       </c>
       <c r="AL15" s="10"/>
     </row>
-    <row r="16" spans="1:58">
+    <row r="16" spans="1:57">
       <c r="B16" s="4">
         <v>1952.5</v>
       </c>
@@ -8489,7 +8467,7 @@
       <c r="AK82" s="10">
         <v>6.7428267983028159E-4</v>
       </c>
-      <c r="AL82" s="15">
+      <c r="AL82" s="14">
         <f>(AL81*3+AL85)/4</f>
         <v>741.30377499999997</v>
       </c>
@@ -8643,7 +8621,7 @@
       <c r="AK83" s="10">
         <v>1.4431821031760845E-3</v>
       </c>
-      <c r="AL83" s="15">
+      <c r="AL83" s="14">
         <f>(AL81*2+AL85*2)/4</f>
         <v>741.78224999999998</v>
       </c>
@@ -8797,7 +8775,7 @@
       <c r="AK84" s="10">
         <v>9.4843014424602788E-4</v>
       </c>
-      <c r="AL84" s="15">
+      <c r="AL84" s="14">
         <f>(AL81+AL85*3)/4</f>
         <v>742.26072499999998</v>
       </c>
@@ -9104,7 +9082,7 @@
       <c r="AK86" s="10">
         <v>4.2023128324493843E-3</v>
       </c>
-      <c r="AL86" s="15">
+      <c r="AL86" s="14">
         <f>(AL85+AL87)/2</f>
         <v>744.29759999999999</v>
       </c>
@@ -10759,7 +10737,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="97" spans="2:58">
+    <row r="97" spans="2:57">
       <c r="B97" s="4">
         <v>1972.75</v>
       </c>
@@ -10920,7 +10898,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="98" spans="2:58">
+    <row r="98" spans="2:57">
       <c r="B98" s="4">
         <v>1973</v>
       </c>
@@ -11032,6 +11010,9 @@
       <c r="AL98" s="10">
         <v>858.59870000000001</v>
       </c>
+      <c r="AM98" s="3">
+        <v>1.026</v>
+      </c>
       <c r="AP98" s="3">
         <v>0.1</v>
       </c>
@@ -11080,11 +11061,8 @@
       <c r="BE98" s="3">
         <v>0.2</v>
       </c>
-      <c r="BF98" s="3">
-        <v>1.026</v>
-      </c>
-    </row>
-    <row r="99" spans="2:58">
+    </row>
+    <row r="99" spans="2:57">
       <c r="B99" s="4">
         <v>1973.25</v>
       </c>
@@ -11196,6 +11174,9 @@
       <c r="AL99" s="10">
         <v>865.9674</v>
       </c>
+      <c r="AM99" s="3">
+        <v>1.0113000000000001</v>
+      </c>
       <c r="AP99" s="3">
         <v>0.2</v>
       </c>
@@ -11244,11 +11225,8 @@
       <c r="BE99" s="3">
         <v>0.11</v>
       </c>
-      <c r="BF99" s="3">
-        <v>1.0113000000000001</v>
-      </c>
-    </row>
-    <row r="100" spans="2:58">
+    </row>
+    <row r="100" spans="2:57">
       <c r="B100" s="4">
         <v>1973.5</v>
       </c>
@@ -11360,6 +11338,9 @@
       <c r="AL100" s="10">
         <v>862.89750000000004</v>
       </c>
+      <c r="AM100" s="3">
+        <v>0.97560000000000002</v>
+      </c>
       <c r="AP100" s="3">
         <v>0.2</v>
       </c>
@@ -11408,11 +11389,8 @@
       <c r="BE100" s="3">
         <v>0.20499999999999999</v>
       </c>
-      <c r="BF100" s="3">
-        <v>0.97560000000000002</v>
-      </c>
-    </row>
-    <row r="101" spans="2:58">
+    </row>
+    <row r="101" spans="2:57">
       <c r="B101" s="4">
         <v>1973.75</v>
       </c>
@@ -11524,6 +11502,9 @@
       <c r="AL101" s="10">
         <v>851.58979999999997</v>
       </c>
+      <c r="AM101" s="3">
+        <v>1.2197</v>
+      </c>
       <c r="AP101" s="3">
         <v>0.3</v>
       </c>
@@ -11572,11 +11553,8 @@
       <c r="BE101" s="3">
         <v>0.21</v>
       </c>
-      <c r="BF101" s="3">
-        <v>1.2197</v>
-      </c>
-    </row>
-    <row r="102" spans="2:58">
+    </row>
+    <row r="102" spans="2:57">
       <c r="B102" s="4">
         <v>1974</v>
       </c>
@@ -11688,6 +11666,9 @@
       <c r="AL102" s="10">
         <v>858.52030000000002</v>
       </c>
+      <c r="AM102" s="3">
+        <v>1.1686000000000001</v>
+      </c>
       <c r="AP102" s="3">
         <v>0.3</v>
       </c>
@@ -11736,11 +11717,8 @@
       <c r="BE102" s="3">
         <v>0.25</v>
       </c>
-      <c r="BF102" s="3">
-        <v>1.1686000000000001</v>
-      </c>
-    </row>
-    <row r="103" spans="2:58">
+    </row>
+    <row r="103" spans="2:57">
       <c r="B103" s="4">
         <v>1974.25</v>
       </c>
@@ -11852,6 +11830,9 @@
       <c r="AL103" s="10">
         <v>857.05460000000005</v>
       </c>
+      <c r="AM103" s="3">
+        <v>1.6315</v>
+      </c>
       <c r="AP103" s="3">
         <v>0.4</v>
       </c>
@@ -11900,11 +11881,8 @@
       <c r="BE103" s="3">
         <v>0.25</v>
       </c>
-      <c r="BF103" s="3">
-        <v>1.6315</v>
-      </c>
-    </row>
-    <row r="104" spans="2:58">
+    </row>
+    <row r="104" spans="2:57">
       <c r="B104" s="4">
         <v>1974.5</v>
       </c>
@@ -12013,10 +11991,13 @@
       <c r="AK104" s="10">
         <v>7.7490711264074598E-3</v>
       </c>
-      <c r="AL104" s="15">
+      <c r="AL104" s="14">
         <f>(AL103+AL105)/2</f>
         <v>841.99215000000004</v>
       </c>
+      <c r="AM104" s="3">
+        <v>2.1772</v>
+      </c>
       <c r="AP104" s="3">
         <v>0.2</v>
       </c>
@@ -12026,7 +12007,7 @@
       <c r="AR104" s="3">
         <v>0.5</v>
       </c>
-      <c r="AS104" s="13">
+      <c r="AS104" s="12">
         <v>0.8</v>
       </c>
       <c r="AT104" s="3">
@@ -12038,7 +12019,7 @@
       <c r="AV104" s="3">
         <v>10.6</v>
       </c>
-      <c r="AW104" s="13">
+      <c r="AW104" s="12">
         <v>9.6999999999999993</v>
       </c>
       <c r="AX104" s="3">
@@ -12050,7 +12031,7 @@
       <c r="AZ104" s="3">
         <v>38</v>
       </c>
-      <c r="BA104" s="13">
+      <c r="BA104" s="12">
         <v>31</v>
       </c>
       <c r="BB104" s="3">
@@ -12062,14 +12043,11 @@
       <c r="BD104" s="3">
         <v>0.22</v>
       </c>
-      <c r="BE104" s="13">
+      <c r="BE104" s="12">
         <v>0.29499999999999998</v>
       </c>
-      <c r="BF104" s="3">
-        <v>2.1772</v>
-      </c>
-    </row>
-    <row r="105" spans="2:58">
+    </row>
+    <row r="105" spans="2:57">
       <c r="B105" s="4">
         <v>1974.75</v>
       </c>
@@ -12181,6 +12159,9 @@
       <c r="AL105" s="10">
         <v>826.92970000000003</v>
       </c>
+      <c r="AM105" s="3">
+        <v>2.1158999999999999</v>
+      </c>
       <c r="AP105" s="3">
         <v>0.5</v>
       </c>
@@ -12229,11 +12210,8 @@
       <c r="BE105" s="3">
         <v>0.34</v>
       </c>
-      <c r="BF105" s="3">
-        <v>2.1158999999999999</v>
-      </c>
-    </row>
-    <row r="106" spans="2:58">
+    </row>
+    <row r="106" spans="2:57">
       <c r="B106" s="4">
         <v>1975</v>
       </c>
@@ -12345,6 +12323,9 @@
       <c r="AL106" s="10">
         <v>811.7654</v>
       </c>
+      <c r="AM106" s="3">
+        <v>1.5933999999999999</v>
+      </c>
       <c r="AP106" s="3">
         <v>0.6</v>
       </c>
@@ -12393,11 +12374,8 @@
       <c r="BE106" s="3">
         <v>0.4</v>
       </c>
-      <c r="BF106" s="3">
-        <v>1.5933999999999999</v>
-      </c>
-    </row>
-    <row r="107" spans="2:58">
+    </row>
+    <row r="107" spans="2:57">
       <c r="B107" s="4">
         <v>1975.25</v>
       </c>
@@ -12509,6 +12487,9 @@
       <c r="AL107" s="10">
         <v>817.0616</v>
       </c>
+      <c r="AM107" s="3">
+        <v>1.4368000000000001</v>
+      </c>
       <c r="AP107" s="3">
         <v>0.4</v>
       </c>
@@ -12557,11 +12538,8 @@
       <c r="BE107" s="3">
         <v>0.39</v>
       </c>
-      <c r="BF107" s="3">
-        <v>1.4368000000000001</v>
-      </c>
-    </row>
-    <row r="108" spans="2:58">
+    </row>
+    <row r="108" spans="2:57">
       <c r="B108" s="4">
         <v>1975.5</v>
       </c>
@@ -12673,6 +12651,9 @@
       <c r="AL108" s="10">
         <v>834.70159999999998</v>
       </c>
+      <c r="AM108" s="3">
+        <v>1.3525</v>
+      </c>
       <c r="AP108" s="3">
         <v>0.4</v>
       </c>
@@ -12721,11 +12702,8 @@
       <c r="BE108" s="3">
         <v>0.30499999999999999</v>
       </c>
-      <c r="BF108" s="3">
-        <v>1.3525</v>
-      </c>
-    </row>
-    <row r="109" spans="2:58">
+    </row>
+    <row r="109" spans="2:57">
       <c r="B109" s="4">
         <v>1975.75</v>
       </c>
@@ -12837,6 +12815,9 @@
       <c r="AL109" s="10">
         <v>854.5942</v>
       </c>
+      <c r="AM109" s="3">
+        <v>1.1652</v>
+      </c>
       <c r="AP109" s="3">
         <v>0.2</v>
       </c>
@@ -12885,11 +12866,8 @@
       <c r="BE109" s="3">
         <v>0.15</v>
       </c>
-      <c r="BF109" s="3">
-        <v>1.1652</v>
-      </c>
-    </row>
-    <row r="110" spans="2:58">
+    </row>
+    <row r="110" spans="2:57">
       <c r="B110" s="4">
         <v>1976</v>
       </c>
@@ -13001,6 +12979,9 @@
       <c r="AL110" s="10">
         <v>1294.8580999999999</v>
       </c>
+      <c r="AM110" s="3">
+        <v>1.0137</v>
+      </c>
       <c r="AP110" s="3">
         <v>0.3</v>
       </c>
@@ -13049,11 +13030,8 @@
       <c r="BE110" s="3">
         <v>0.18</v>
       </c>
-      <c r="BF110" s="3">
-        <v>1.0137</v>
-      </c>
-    </row>
-    <row r="111" spans="2:58">
+    </row>
+    <row r="111" spans="2:57">
       <c r="B111" s="4">
         <v>1976.25</v>
       </c>
@@ -13165,6 +13143,9 @@
       <c r="AL111" s="10">
         <v>1312.4110000000001</v>
       </c>
+      <c r="AM111" s="3">
+        <v>0.99609999999999999</v>
+      </c>
       <c r="AP111" s="3">
         <v>0.1</v>
       </c>
@@ -13213,11 +13194,8 @@
       <c r="BE111" s="3">
         <v>0.15</v>
       </c>
-      <c r="BF111" s="3">
-        <v>0.99609999999999999</v>
-      </c>
-    </row>
-    <row r="112" spans="2:58">
+    </row>
+    <row r="112" spans="2:57">
       <c r="B112" s="4">
         <v>1976.5</v>
       </c>
@@ -13329,6 +13307,9 @@
       <c r="AL112" s="10">
         <v>1339.1117999999999</v>
       </c>
+      <c r="AM112" s="3">
+        <v>0.89380000000000004</v>
+      </c>
       <c r="AP112" s="3">
         <v>0.2</v>
       </c>
@@ -13377,11 +13358,8 @@
       <c r="BE112" s="3">
         <v>0.2</v>
       </c>
-      <c r="BF112" s="3">
-        <v>0.89380000000000004</v>
-      </c>
-    </row>
-    <row r="113" spans="2:58">
+    </row>
+    <row r="113" spans="2:57">
       <c r="B113" s="4">
         <v>1976.75</v>
       </c>
@@ -13493,6 +13471,9 @@
       <c r="AL113" s="10">
         <v>1352.2916</v>
       </c>
+      <c r="AM113" s="3">
+        <v>0.95240000000000002</v>
+      </c>
       <c r="AP113" s="3">
         <v>0.3</v>
       </c>
@@ -13541,11 +13522,8 @@
       <c r="BE113" s="3">
         <v>0.18</v>
       </c>
-      <c r="BF113" s="3">
-        <v>0.95240000000000002</v>
-      </c>
-    </row>
-    <row r="114" spans="2:58">
+    </row>
+    <row r="114" spans="2:57">
       <c r="B114" s="4">
         <v>1977</v>
       </c>
@@ -13657,6 +13635,9 @@
       <c r="AL114" s="10">
         <v>1360.3936000000001</v>
       </c>
+      <c r="AM114" s="3">
+        <v>0.90690000000000004</v>
+      </c>
       <c r="AP114" s="3">
         <v>0.3</v>
       </c>
@@ -13705,11 +13686,8 @@
       <c r="BE114" s="3">
         <v>0.2</v>
       </c>
-      <c r="BF114" s="3">
-        <v>0.90690000000000004</v>
-      </c>
-    </row>
-    <row r="115" spans="2:58">
+    </row>
+    <row r="115" spans="2:57">
       <c r="B115" s="4">
         <v>1977.25</v>
       </c>
@@ -13821,6 +13799,9 @@
       <c r="AL115" s="10">
         <v>1379.1165000000001</v>
       </c>
+      <c r="AM115" s="3">
+        <v>0.84830000000000005</v>
+      </c>
       <c r="AP115" s="3">
         <v>0.2</v>
       </c>
@@ -13869,11 +13850,8 @@
       <c r="BE115" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="BF115" s="3">
-        <v>0.84830000000000005</v>
-      </c>
-    </row>
-    <row r="116" spans="2:58">
+    </row>
+    <row r="116" spans="2:57">
       <c r="B116" s="4">
         <v>1977.5</v>
       </c>
@@ -13985,6 +13963,9 @@
       <c r="AL116" s="10">
         <v>1401.3976</v>
       </c>
+      <c r="AM116" s="3">
+        <v>0.96399999999999997</v>
+      </c>
       <c r="AP116" s="3">
         <v>0.2</v>
       </c>
@@ -14033,11 +14014,8 @@
       <c r="BE116" s="3">
         <v>0.25</v>
       </c>
-      <c r="BF116" s="3">
-        <v>0.96399999999999997</v>
-      </c>
-    </row>
-    <row r="117" spans="2:58">
+    </row>
+    <row r="117" spans="2:57">
       <c r="B117" s="4">
         <v>1977.75</v>
       </c>
@@ -14148,6 +14126,9 @@
       </c>
       <c r="AL117" s="10">
         <v>1411.8925999999999</v>
+      </c>
+      <c r="AM117" s="3">
+        <v>0.88529999999999998</v>
       </c>
       <c r="AN117" s="3"/>
       <c r="AP117" s="3">
@@ -14198,11 +14179,8 @@
       <c r="BE117" s="3">
         <v>0.2</v>
       </c>
-      <c r="BF117" s="3">
-        <v>0.88529999999999998</v>
-      </c>
-    </row>
-    <row r="118" spans="2:58">
+    </row>
+    <row r="118" spans="2:57">
       <c r="B118" s="4">
         <v>1978</v>
       </c>
@@ -14315,7 +14293,7 @@
         <v>1426.7755999999999</v>
       </c>
       <c r="AM118" s="3">
-        <v>83</v>
+        <v>0.74839999999999995</v>
       </c>
       <c r="AN118" s="3">
         <v>106</v>
@@ -14368,11 +14346,8 @@
       <c r="BE118" s="3">
         <v>0.2</v>
       </c>
-      <c r="BF118" s="3">
-        <v>0.74839999999999995</v>
-      </c>
-    </row>
-    <row r="119" spans="2:58">
+    </row>
+    <row r="119" spans="2:57">
       <c r="B119" s="4">
         <v>1978.25</v>
       </c>
@@ -14484,8 +14459,8 @@
       <c r="AL119" s="10">
         <v>1420.069</v>
       </c>
-      <c r="AM119" s="12">
-        <v>75</v>
+      <c r="AM119" s="3">
+        <v>0.69720000000000004</v>
       </c>
       <c r="AN119" s="3">
         <v>99</v>
@@ -14538,11 +14513,8 @@
       <c r="BE119" s="3">
         <v>0.14499999999999999</v>
       </c>
-      <c r="BF119" s="3">
-        <v>0.69720000000000004</v>
-      </c>
-    </row>
-    <row r="120" spans="2:58">
+    </row>
+    <row r="120" spans="2:57">
       <c r="B120" s="4">
         <v>1978.5</v>
       </c>
@@ -14654,8 +14626,8 @@
       <c r="AL120" s="10">
         <v>1407.5423000000001</v>
       </c>
-      <c r="AM120" s="12">
-        <v>70</v>
+      <c r="AM120" s="3">
+        <v>0.61029999999999995</v>
       </c>
       <c r="AN120" s="3">
         <v>95</v>
@@ -14708,11 +14680,8 @@
       <c r="BE120" s="3">
         <v>0.12</v>
       </c>
-      <c r="BF120" s="3">
-        <v>0.61029999999999995</v>
-      </c>
-    </row>
-    <row r="121" spans="2:58">
+    </row>
+    <row r="121" spans="2:57">
       <c r="B121" s="4">
         <v>1978.75</v>
       </c>
@@ -14824,8 +14793,8 @@
       <c r="AL121" s="10">
         <v>1421.3958</v>
       </c>
-      <c r="AM121" s="12">
-        <v>66</v>
+      <c r="AM121" s="3">
+        <v>0.63759999999999994</v>
       </c>
       <c r="AN121" s="3">
         <v>87</v>
@@ -14878,11 +14847,8 @@
       <c r="BE121" s="3">
         <v>0.18</v>
       </c>
-      <c r="BF121" s="3">
-        <v>0.63759999999999994</v>
-      </c>
-    </row>
-    <row r="122" spans="2:58">
+    </row>
+    <row r="122" spans="2:57">
       <c r="B122" s="4">
         <v>1979</v>
       </c>
@@ -14994,8 +14960,8 @@
       <c r="AL122" s="10">
         <v>1428.5038999999999</v>
       </c>
-      <c r="AM122" s="12">
-        <v>63</v>
+      <c r="AM122" s="3">
+        <v>0.66539999999999999</v>
       </c>
       <c r="AN122" s="3">
         <v>81</v>
@@ -15048,11 +15014,8 @@
       <c r="BE122" s="3">
         <v>0.2</v>
       </c>
-      <c r="BF122" s="3">
-        <v>0.66539999999999999</v>
-      </c>
-    </row>
-    <row r="123" spans="2:58">
+    </row>
+    <row r="123" spans="2:57">
       <c r="B123" s="4">
         <v>1979.25</v>
       </c>
@@ -15164,8 +15127,8 @@
       <c r="AL123" s="10">
         <v>1426.0064</v>
       </c>
-      <c r="AM123" s="12">
-        <v>58</v>
+      <c r="AM123" s="3">
+        <v>0.69</v>
       </c>
       <c r="AN123" s="3">
         <v>73</v>
@@ -15218,11 +15181,8 @@
       <c r="BE123" s="3">
         <v>0.25</v>
       </c>
-      <c r="BF123" s="3">
-        <v>0.69</v>
-      </c>
-    </row>
-    <row r="124" spans="2:58">
+    </row>
+    <row r="124" spans="2:57">
       <c r="B124" s="4">
         <v>1979.5</v>
       </c>
@@ -15334,8 +15294,8 @@
       <c r="AL124" s="10">
         <v>1415.1719000000001</v>
       </c>
-      <c r="AM124" s="12">
-        <v>46</v>
+      <c r="AM124" s="3">
+        <v>0.65900000000000003</v>
       </c>
       <c r="AN124" s="3">
         <v>74</v>
@@ -15388,11 +15348,8 @@
       <c r="BE124" s="3">
         <v>0.15</v>
       </c>
-      <c r="BF124" s="3">
-        <v>0.65900000000000003</v>
-      </c>
-    </row>
-    <row r="125" spans="2:58">
+    </row>
+    <row r="125" spans="2:57">
       <c r="B125" s="4">
         <v>1979.75</v>
       </c>
@@ -15504,8 +15461,8 @@
       <c r="AL125" s="10">
         <v>1421.5597</v>
       </c>
-      <c r="AM125" s="12">
-        <v>51</v>
+      <c r="AM125" s="3">
+        <v>0.77180000000000004</v>
       </c>
       <c r="AN125" s="3">
         <v>80</v>
@@ -15558,11 +15515,8 @@
       <c r="BE125" s="3">
         <v>0.23</v>
       </c>
-      <c r="BF125" s="3">
-        <v>0.77180000000000004</v>
-      </c>
-    </row>
-    <row r="126" spans="2:58">
+    </row>
+    <row r="126" spans="2:57">
       <c r="B126" s="4">
         <v>1980</v>
       </c>
@@ -15674,8 +15628,8 @@
       <c r="AL126" s="10">
         <v>1434.5125</v>
       </c>
-      <c r="AM126" s="12">
-        <v>50</v>
+      <c r="AM126" s="3">
+        <v>0.92379999999999995</v>
       </c>
       <c r="AN126" s="3">
         <v>84</v>
@@ -15728,11 +15682,8 @@
       <c r="BE126" s="3">
         <v>0.2</v>
       </c>
-      <c r="BF126" s="3">
-        <v>0.92379999999999995</v>
-      </c>
-    </row>
-    <row r="127" spans="2:58">
+    </row>
+    <row r="127" spans="2:57">
       <c r="B127" s="4">
         <v>1980.25</v>
       </c>
@@ -15844,8 +15795,8 @@
       <c r="AL127" s="10">
         <v>1426.6566</v>
       </c>
-      <c r="AM127" s="12">
-        <v>51</v>
+      <c r="AM127" s="3">
+        <v>0.93500000000000005</v>
       </c>
       <c r="AN127" s="3">
         <v>81</v>
@@ -15898,11 +15849,8 @@
       <c r="BE127" s="3">
         <v>0.3</v>
       </c>
-      <c r="BF127" s="3">
-        <v>0.93500000000000005</v>
-      </c>
-    </row>
-    <row r="128" spans="2:58">
+    </row>
+    <row r="128" spans="2:57">
       <c r="B128" s="4">
         <v>1980.5</v>
       </c>
@@ -16014,8 +15962,8 @@
       <c r="AL128" s="10">
         <v>1428.7605000000001</v>
       </c>
-      <c r="AM128" s="12">
-        <v>63</v>
+      <c r="AM128" s="3">
+        <v>0.8629</v>
       </c>
       <c r="AN128" s="3">
         <v>108</v>
@@ -16068,11 +16016,8 @@
       <c r="BE128" s="3">
         <v>0.3</v>
       </c>
-      <c r="BF128" s="3">
-        <v>0.8629</v>
-      </c>
-    </row>
-    <row r="129" spans="2:58">
+    </row>
+    <row r="129" spans="2:57">
       <c r="B129" s="4">
         <v>1980.75</v>
       </c>
@@ -16184,8 +16129,8 @@
       <c r="AL129" s="10">
         <v>1458.0844</v>
       </c>
-      <c r="AM129" s="12">
-        <v>83</v>
+      <c r="AM129" s="3">
+        <v>0.98980000000000001</v>
       </c>
       <c r="AN129" s="3">
         <v>117</v>
@@ -16238,11 +16183,8 @@
       <c r="BE129" s="3">
         <v>0.2</v>
       </c>
-      <c r="BF129" s="3">
-        <v>0.98980000000000001</v>
-      </c>
-    </row>
-    <row r="130" spans="2:58">
+    </row>
+    <row r="130" spans="2:57">
       <c r="B130" s="4">
         <v>1981</v>
       </c>
@@ -16354,8 +16296,8 @@
       <c r="AL130" s="10">
         <v>1534.4213</v>
       </c>
-      <c r="AM130" s="12">
-        <v>76</v>
+      <c r="AM130" s="3">
+        <v>0.96340000000000003</v>
       </c>
       <c r="AN130" s="3">
         <v>119</v>
@@ -16408,11 +16350,8 @@
       <c r="BE130" s="3">
         <v>0.3</v>
       </c>
-      <c r="BF130" s="3">
-        <v>0.96340000000000003</v>
-      </c>
-    </row>
-    <row r="131" spans="2:58">
+    </row>
+    <row r="131" spans="2:57">
       <c r="B131" s="4">
         <v>1981.25</v>
       </c>
@@ -16524,8 +16463,8 @@
       <c r="AL131" s="10">
         <v>1559.7711999999999</v>
       </c>
-      <c r="AM131" s="12">
-        <v>79</v>
+      <c r="AM131" s="3">
+        <v>1.1214999999999999</v>
       </c>
       <c r="AN131" s="3">
         <v>116</v>
@@ -16578,11 +16517,8 @@
       <c r="BE131" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="BF131" s="3">
-        <v>1.1214999999999999</v>
-      </c>
-    </row>
-    <row r="132" spans="2:58">
+    </row>
+    <row r="132" spans="2:57">
       <c r="B132" s="4">
         <v>1981.5</v>
       </c>
@@ -16694,8 +16630,8 @@
       <c r="AL132" s="10">
         <v>1555.2666999999999</v>
       </c>
-      <c r="AM132" s="12">
-        <v>74</v>
+      <c r="AM132" s="3">
+        <v>1.1418999999999999</v>
       </c>
       <c r="AN132" s="3">
         <v>116</v>
@@ -16748,11 +16684,8 @@
       <c r="BE132" s="3">
         <v>0.21</v>
       </c>
-      <c r="BF132" s="3">
-        <v>1.1418999999999999</v>
-      </c>
-    </row>
-    <row r="133" spans="2:58">
+    </row>
+    <row r="133" spans="2:57">
       <c r="B133" s="4">
         <v>1981.75</v>
       </c>
@@ -16864,8 +16797,8 @@
       <c r="AL133" s="10">
         <v>1537.3171</v>
       </c>
-      <c r="AM133" s="12">
-        <v>62</v>
+      <c r="AM133" s="3">
+        <v>1.4448000000000001</v>
       </c>
       <c r="AN133" s="3">
         <v>103</v>
@@ -16918,11 +16851,8 @@
       <c r="BE133" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="BF133" s="3">
-        <v>1.4448000000000001</v>
-      </c>
-    </row>
-    <row r="134" spans="2:58">
+    </row>
+    <row r="134" spans="2:57">
       <c r="B134" s="4">
         <v>1982</v>
       </c>
@@ -17034,8 +16964,8 @@
       <c r="AL134" s="10">
         <v>1542.5172</v>
       </c>
-      <c r="AM134" s="12">
-        <v>65</v>
+      <c r="AM134" s="3">
+        <v>1.5509999999999999</v>
       </c>
       <c r="AN134" s="3">
         <v>107</v>
@@ -17088,11 +17018,8 @@
       <c r="BE134" s="3">
         <v>0.16</v>
       </c>
-      <c r="BF134" s="3">
-        <v>1.5509999999999999</v>
-      </c>
-    </row>
-    <row r="135" spans="2:58">
+    </row>
+    <row r="135" spans="2:57">
       <c r="B135" s="4">
         <v>1982.25</v>
       </c>
@@ -17204,8 +17131,8 @@
       <c r="AL135" s="10">
         <v>1528.325</v>
       </c>
-      <c r="AM135" s="12">
-        <v>69</v>
+      <c r="AM135" s="3">
+        <v>1.5548999999999999</v>
       </c>
       <c r="AN135" s="3">
         <v>111</v>
@@ -17258,11 +17185,8 @@
       <c r="BE135" s="3">
         <v>0.185</v>
       </c>
-      <c r="BF135" s="3">
-        <v>1.5548999999999999</v>
-      </c>
-    </row>
-    <row r="136" spans="2:58">
+    </row>
+    <row r="136" spans="2:57">
       <c r="B136" s="4">
         <v>1982.5</v>
       </c>
@@ -17374,8 +17298,8 @@
       <c r="AL136" s="10">
         <v>1524.8947000000001</v>
       </c>
-      <c r="AM136" s="12">
-        <v>69</v>
+      <c r="AM136" s="3">
+        <v>1.6774</v>
       </c>
       <c r="AN136" s="3">
         <v>111</v>
@@ -17428,11 +17352,8 @@
       <c r="BE136" s="3">
         <v>0.20499999999999999</v>
       </c>
-      <c r="BF136" s="3">
-        <v>1.6774</v>
-      </c>
-    </row>
-    <row r="137" spans="2:58">
+    </row>
+    <row r="137" spans="2:57">
       <c r="B137" s="4">
         <v>1982.75</v>
       </c>
@@ -17544,8 +17465,8 @@
       <c r="AL137" s="10">
         <v>1534.0571</v>
       </c>
-      <c r="AM137" s="12">
-        <v>83</v>
+      <c r="AM137" s="3">
+        <v>1.5542</v>
       </c>
       <c r="AN137" s="3">
         <v>119</v>
@@ -17598,11 +17519,8 @@
       <c r="BE137" s="3">
         <v>0.27500000000000002</v>
       </c>
-      <c r="BF137" s="3">
-        <v>1.5542</v>
-      </c>
-    </row>
-    <row r="138" spans="2:58">
+    </row>
+    <row r="138" spans="2:57">
       <c r="B138" s="4">
         <v>1983</v>
       </c>
@@ -17714,8 +17632,8 @@
       <c r="AL138" s="10">
         <v>1541.3214</v>
       </c>
-      <c r="AM138" s="12">
-        <v>78</v>
+      <c r="AM138" s="3">
+        <v>1.1416999999999999</v>
       </c>
       <c r="AN138" s="3">
         <v>131</v>
@@ -17768,11 +17686,8 @@
       <c r="BE138" s="3">
         <v>0.16</v>
       </c>
-      <c r="BF138" s="3">
-        <v>1.1416999999999999</v>
-      </c>
-    </row>
-    <row r="139" spans="2:58">
+    </row>
+    <row r="139" spans="2:57">
       <c r="B139" s="4">
         <v>1983.25</v>
       </c>
@@ -17884,8 +17799,8 @@
       <c r="AL139" s="10">
         <v>1575.0555999999999</v>
       </c>
-      <c r="AM139" s="12">
-        <v>98</v>
+      <c r="AM139" s="3">
+        <v>0.89</v>
       </c>
       <c r="AN139" s="3">
         <v>146</v>
@@ -17938,11 +17853,8 @@
       <c r="BE139" s="3">
         <v>0.1</v>
       </c>
-      <c r="BF139" s="3">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="140" spans="2:58">
+    </row>
+    <row r="140" spans="2:57">
       <c r="B140" s="4">
         <v>1983.5</v>
       </c>
@@ -18054,8 +17966,8 @@
       <c r="AL140" s="10">
         <v>1606.3333</v>
       </c>
-      <c r="AM140" s="12">
-        <v>99</v>
+      <c r="AM140" s="3">
+        <v>0.88780000000000003</v>
       </c>
       <c r="AN140" s="3">
         <v>138</v>
@@ -18108,11 +18020,8 @@
       <c r="BE140" s="3">
         <v>0.13</v>
       </c>
-      <c r="BF140" s="3">
-        <v>0.88780000000000003</v>
-      </c>
-    </row>
-    <row r="141" spans="2:58">
+    </row>
+    <row r="141" spans="2:57">
       <c r="B141" s="4">
         <v>1983.75</v>
       </c>
@@ -18224,8 +18133,8 @@
       <c r="AL141" s="10">
         <v>1638.9118000000001</v>
       </c>
-      <c r="AM141" s="12">
-        <v>99</v>
+      <c r="AM141" s="3">
+        <v>0.94359999999999999</v>
       </c>
       <c r="AN141" s="3">
         <v>136</v>
@@ -18278,11 +18187,8 @@
       <c r="BE141" s="3">
         <v>0.1</v>
       </c>
-      <c r="BF141" s="3">
-        <v>0.94359999999999999</v>
-      </c>
-    </row>
-    <row r="142" spans="2:58">
+    </row>
+    <row r="142" spans="2:57">
       <c r="B142" s="4">
         <v>1984</v>
       </c>
@@ -18394,8 +18300,8 @@
       <c r="AL142" s="10">
         <v>1650.3333</v>
       </c>
-      <c r="AM142" s="12">
-        <v>109</v>
+      <c r="AM142" s="3">
+        <v>0.95289999999999997</v>
       </c>
       <c r="AN142" s="3">
         <v>130</v>
@@ -18448,11 +18354,8 @@
       <c r="BE142" s="3">
         <v>0.155</v>
       </c>
-      <c r="BF142" s="3">
-        <v>0.95289999999999997</v>
-      </c>
-    </row>
-    <row r="143" spans="2:58">
+    </row>
+    <row r="143" spans="2:57">
       <c r="B143" s="4">
         <v>1984.25</v>
       </c>
@@ -18564,8 +18467,8 @@
       <c r="AL143" s="10">
         <v>1673.9375</v>
       </c>
-      <c r="AM143" s="12">
-        <v>106</v>
+      <c r="AM143" s="3">
+        <v>0.877</v>
       </c>
       <c r="AN143" s="3">
         <v>117</v>
@@ -18618,11 +18521,8 @@
       <c r="BE143" s="3">
         <v>0.13</v>
       </c>
-      <c r="BF143" s="3">
-        <v>0.877</v>
-      </c>
-    </row>
-    <row r="144" spans="2:58">
+    </row>
+    <row r="144" spans="2:57">
       <c r="B144" s="4">
         <v>1984.5</v>
       </c>
@@ -18734,8 +18634,8 @@
       <c r="AL144" s="10">
         <v>1710.4167</v>
       </c>
-      <c r="AM144" s="12">
-        <v>113</v>
+      <c r="AM144" s="3">
+        <v>0.95779999999999998</v>
       </c>
       <c r="AN144" s="3">
         <v>119</v>
@@ -18788,11 +18688,8 @@
       <c r="BE144" s="3">
         <v>0.23</v>
       </c>
-      <c r="BF144" s="3">
-        <v>0.95779999999999998</v>
-      </c>
-    </row>
-    <row r="145" spans="2:58">
+    </row>
+    <row r="145" spans="2:57">
       <c r="B145" s="4">
         <v>1984.75</v>
       </c>
@@ -18904,8 +18801,8 @@
       <c r="AL145" s="10">
         <v>1710.7143000000001</v>
       </c>
-      <c r="AM145" s="12">
-        <v>104</v>
+      <c r="AM145" s="3">
+        <v>0.99639999999999995</v>
       </c>
       <c r="AN145" s="3">
         <v>118</v>
@@ -18958,11 +18855,8 @@
       <c r="BE145" s="3">
         <v>0.3</v>
       </c>
-      <c r="BF145" s="3">
-        <v>0.99639999999999995</v>
-      </c>
-    </row>
-    <row r="146" spans="2:58">
+    </row>
+    <row r="146" spans="2:57">
       <c r="B146" s="4">
         <v>1985</v>
       </c>
@@ -19074,8 +18968,8 @@
       <c r="AL146" s="10">
         <v>1739.25</v>
       </c>
-      <c r="AM146" s="12">
-        <v>99</v>
+      <c r="AM146" s="3">
+        <v>1.0276000000000001</v>
       </c>
       <c r="AN146" s="3">
         <v>115</v>
@@ -19128,11 +19022,8 @@
       <c r="BE146" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="BF146" s="3">
-        <v>1.0276000000000001</v>
-      </c>
-    </row>
-    <row r="147" spans="2:58">
+    </row>
+    <row r="147" spans="2:57">
       <c r="B147" s="4">
         <v>1985.25</v>
       </c>
@@ -19244,8 +19135,8 @@
       <c r="AL147" s="10">
         <v>1736.9231</v>
       </c>
-      <c r="AM147" s="12">
-        <v>99</v>
+      <c r="AM147" s="3">
+        <v>1.1998</v>
       </c>
       <c r="AN147" s="3">
         <v>114</v>
@@ -19298,11 +19189,8 @@
       <c r="BE147" s="3">
         <v>0.23499999999999999</v>
       </c>
-      <c r="BF147" s="3">
-        <v>1.1998</v>
-      </c>
-    </row>
-    <row r="148" spans="2:58">
+    </row>
+    <row r="148" spans="2:57">
       <c r="B148" s="4">
         <v>1985.5</v>
       </c>
@@ -19414,8 +19302,8 @@
       <c r="AL148" s="10">
         <v>1730.2592999999999</v>
       </c>
-      <c r="AM148" s="12">
-        <v>98</v>
+      <c r="AM148" s="3">
+        <v>1.2437</v>
       </c>
       <c r="AN148" s="3">
         <v>110</v>
@@ -19468,11 +19356,8 @@
       <c r="BE148" s="3">
         <v>0.22</v>
       </c>
-      <c r="BF148" s="3">
-        <v>1.2437</v>
-      </c>
-    </row>
-    <row r="149" spans="2:58">
+    </row>
+    <row r="149" spans="2:57">
       <c r="B149" s="4">
         <v>1985.75</v>
       </c>
@@ -19584,8 +19469,8 @@
       <c r="AL149" s="10">
         <v>1744.875</v>
       </c>
-      <c r="AM149" s="12">
-        <v>96</v>
+      <c r="AM149" s="3">
+        <v>1.4291</v>
       </c>
       <c r="AN149" s="3">
         <v>106</v>
@@ -19638,11 +19523,8 @@
       <c r="BE149" s="3">
         <v>0.17</v>
       </c>
-      <c r="BF149" s="3">
-        <v>1.4291</v>
-      </c>
-    </row>
-    <row r="150" spans="2:58">
+    </row>
+    <row r="150" spans="2:57">
       <c r="B150" s="4">
         <v>1986</v>
       </c>
@@ -19754,8 +19636,8 @@
       <c r="AL150" s="10">
         <v>3728.8182000000002</v>
       </c>
-      <c r="AM150" s="12">
-        <v>96</v>
+      <c r="AM150" s="3">
+        <v>1.8412999999999999</v>
       </c>
       <c r="AN150" s="3">
         <v>112</v>
@@ -19811,11 +19693,8 @@
       <c r="BE150" s="3">
         <v>0.11</v>
       </c>
-      <c r="BF150" s="3">
-        <v>1.8412999999999999</v>
-      </c>
-    </row>
-    <row r="151" spans="2:58">
+    </row>
+    <row r="151" spans="2:57">
       <c r="B151" s="4">
         <v>1986.25</v>
       </c>
@@ -19927,8 +19806,8 @@
       <c r="AL151" s="10">
         <v>3755.96</v>
       </c>
-      <c r="AM151" s="12">
-        <v>95</v>
+      <c r="AM151" s="3">
+        <v>1.972</v>
       </c>
       <c r="AN151" s="3">
         <v>112</v>
@@ -19984,11 +19863,8 @@
       <c r="BE151" s="3">
         <v>0.18</v>
       </c>
-      <c r="BF151" s="3">
-        <v>1.972</v>
-      </c>
-    </row>
-    <row r="152" spans="2:58">
+    </row>
+    <row r="152" spans="2:57">
       <c r="B152" s="4">
         <v>1986.5</v>
       </c>
@@ -20100,8 +19976,8 @@
       <c r="AL152" s="10">
         <v>3798.6522</v>
       </c>
-      <c r="AM152" s="12">
-        <v>91</v>
+      <c r="AM152" s="3">
+        <v>2.0950000000000002</v>
       </c>
       <c r="AN152" s="3">
         <v>108</v>
@@ -20157,11 +20033,8 @@
       <c r="BE152" s="3">
         <v>0.16500000000000001</v>
       </c>
-      <c r="BF152" s="3">
-        <v>2.0950000000000002</v>
-      </c>
-    </row>
-    <row r="153" spans="2:58">
+    </row>
+    <row r="153" spans="2:57">
       <c r="B153" s="4">
         <v>1986.75</v>
       </c>
@@ -20273,8 +20146,8 @@
       <c r="AL153" s="10">
         <v>3811.0455000000002</v>
       </c>
-      <c r="AM153" s="12">
-        <v>90</v>
+      <c r="AM153" s="3">
+        <v>1.9807999999999999</v>
       </c>
       <c r="AN153" s="3">
         <v>101</v>
@@ -20330,11 +20203,8 @@
       <c r="BE153" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="BF153" s="3">
-        <v>1.9807999999999999</v>
-      </c>
-    </row>
-    <row r="154" spans="2:58">
+    </row>
+    <row r="154" spans="2:57">
       <c r="B154" s="4">
         <v>1987</v>
       </c>
@@ -20446,8 +20316,8 @@
       <c r="AL154" s="10">
         <v>3823.4211</v>
       </c>
-      <c r="AM154" s="12">
-        <v>84</v>
+      <c r="AM154" s="3">
+        <v>1.8228</v>
       </c>
       <c r="AN154" s="3">
         <v>105</v>
@@ -20503,11 +20373,8 @@
       <c r="BE154" s="3">
         <v>0.11</v>
       </c>
-      <c r="BF154" s="3">
-        <v>1.8228</v>
-      </c>
-    </row>
-    <row r="155" spans="2:58">
+    </row>
+    <row r="155" spans="2:57">
       <c r="B155" s="4">
         <v>1987.25</v>
       </c>
@@ -20619,8 +20486,8 @@
       <c r="AL155" s="10">
         <v>3854.6154000000001</v>
       </c>
-      <c r="AM155" s="12">
-        <v>92</v>
+      <c r="AM155" s="3">
+        <v>1.6871</v>
       </c>
       <c r="AN155" s="3">
         <v>103</v>
@@ -20676,11 +20543,8 @@
       <c r="BE155" s="3">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="BF155" s="3">
-        <v>1.6871</v>
-      </c>
-    </row>
-    <row r="156" spans="2:58">
+    </row>
+    <row r="156" spans="2:57">
       <c r="B156" s="4">
         <v>1987.5</v>
       </c>
@@ -20792,8 +20656,8 @@
       <c r="AL156" s="10">
         <v>3924.8420999999998</v>
       </c>
-      <c r="AM156" s="12">
-        <v>93</v>
+      <c r="AM156" s="3">
+        <v>1.6107</v>
       </c>
       <c r="AN156" s="3">
         <v>109</v>
@@ -20849,11 +20713,8 @@
       <c r="BE156" s="3">
         <v>0.1</v>
       </c>
-      <c r="BF156" s="3">
-        <v>1.6107</v>
-      </c>
-    </row>
-    <row r="157" spans="2:58">
+    </row>
+    <row r="157" spans="2:57">
       <c r="B157" s="4">
         <v>1987.75</v>
       </c>
@@ -20965,8 +20826,8 @@
       <c r="AL157" s="10">
         <v>3930.3683999999998</v>
       </c>
-      <c r="AM157" s="12">
-        <v>86</v>
+      <c r="AM157" s="3">
+        <v>1.5905</v>
       </c>
       <c r="AN157" s="3">
         <v>101</v>
@@ -21022,11 +20883,8 @@
       <c r="BE157" s="3">
         <v>0.1</v>
       </c>
-      <c r="BF157" s="3">
-        <v>1.5905</v>
-      </c>
-    </row>
-    <row r="158" spans="2:58">
+    </row>
+    <row r="158" spans="2:57">
       <c r="B158" s="4">
         <v>1988</v>
       </c>
@@ -21138,8 +20996,8 @@
       <c r="AL158" s="10">
         <v>3959.4117999999999</v>
       </c>
-      <c r="AM158" s="12">
-        <v>90</v>
+      <c r="AM158" s="3">
+        <v>1.593</v>
       </c>
       <c r="AN158" s="3">
         <v>104</v>
@@ -21195,11 +21053,8 @@
       <c r="BE158" s="3">
         <v>0.15</v>
       </c>
-      <c r="BF158" s="3">
-        <v>1.593</v>
-      </c>
-    </row>
-    <row r="159" spans="2:58">
+    </row>
+    <row r="159" spans="2:57">
       <c r="B159" s="4">
         <v>1988.25</v>
       </c>
@@ -21311,8 +21166,8 @@
       <c r="AL159" s="10">
         <v>4018.6471000000001</v>
       </c>
-      <c r="AM159" s="12">
-        <v>94</v>
+      <c r="AM159" s="3">
+        <v>1.4676</v>
       </c>
       <c r="AN159" s="3">
         <v>106</v>
@@ -21368,11 +21223,8 @@
       <c r="BE159" s="3">
         <v>0.1</v>
       </c>
-      <c r="BF159" s="3">
-        <v>1.4676</v>
-      </c>
-    </row>
-    <row r="160" spans="2:58">
+    </row>
+    <row r="160" spans="2:57">
       <c r="B160" s="4">
         <v>1988.5</v>
       </c>
@@ -21484,8 +21336,8 @@
       <c r="AL160" s="10">
         <v>4125.125</v>
       </c>
-      <c r="AM160" s="12">
-        <v>101</v>
+      <c r="AM160" s="3">
+        <v>1.4797</v>
       </c>
       <c r="AN160" s="3">
         <v>109</v>
@@ -21541,11 +21393,8 @@
       <c r="BE160" s="3">
         <v>0.11</v>
       </c>
-      <c r="BF160" s="3">
-        <v>1.4797</v>
-      </c>
-    </row>
-    <row r="161" spans="2:58">
+    </row>
+    <row r="161" spans="2:57">
       <c r="B161" s="4">
         <v>1988.75</v>
       </c>
@@ -21657,8 +21506,8 @@
       <c r="AL161" s="10">
         <v>4136.3571000000002</v>
       </c>
-      <c r="AM161" s="12">
-        <v>97</v>
+      <c r="AM161" s="3">
+        <v>1.524</v>
       </c>
       <c r="AN161" s="3">
         <v>103</v>
@@ -21714,11 +21563,8 @@
       <c r="BE161" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="BF161" s="3">
-        <v>1.524</v>
-      </c>
-    </row>
-    <row r="162" spans="2:58">
+    </row>
+    <row r="162" spans="2:57">
       <c r="B162" s="4">
         <v>1989</v>
       </c>
@@ -21830,8 +21676,8 @@
       <c r="AL162" s="10">
         <v>4138</v>
       </c>
-      <c r="AM162" s="12">
-        <v>100</v>
+      <c r="AM162" s="3">
+        <v>1.5034000000000001</v>
       </c>
       <c r="AN162" s="3">
         <v>106</v>
@@ -21887,11 +21733,8 @@
       <c r="BE162" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="BF162" s="3">
-        <v>1.5034000000000001</v>
-      </c>
-    </row>
-    <row r="163" spans="2:58">
+    </row>
+    <row r="163" spans="2:57">
       <c r="B163" s="4">
         <v>1989.25</v>
       </c>
@@ -22003,8 +21846,8 @@
       <c r="AL163" s="10">
         <v>4177.25</v>
       </c>
-      <c r="AM163" s="12">
-        <v>90</v>
+      <c r="AM163" s="3">
+        <v>1.7632000000000001</v>
       </c>
       <c r="AN163" s="3">
         <v>101</v>
@@ -22060,11 +21903,8 @@
       <c r="BE163" s="3">
         <v>0.1</v>
       </c>
-      <c r="BF163" s="3">
-        <v>1.7632000000000001</v>
-      </c>
-    </row>
-    <row r="164" spans="2:58">
+    </row>
+    <row r="164" spans="2:57">
       <c r="B164" s="4">
         <v>1989.5</v>
       </c>
@@ -22176,8 +22016,8 @@
       <c r="AL164" s="10">
         <v>4231.0267000000003</v>
       </c>
-      <c r="AM164" s="12">
-        <v>95</v>
+      <c r="AM164" s="3">
+        <v>1.7269000000000001</v>
       </c>
       <c r="AN164" s="3">
         <v>103</v>
@@ -22233,11 +22073,8 @@
       <c r="BE164" s="3">
         <v>0.22</v>
       </c>
-      <c r="BF164" s="3">
-        <v>1.7269000000000001</v>
-      </c>
-    </row>
-    <row r="165" spans="2:58">
+    </row>
+    <row r="165" spans="2:57">
       <c r="B165" s="4">
         <v>1989.75</v>
       </c>
@@ -22349,8 +22186,8 @@
       <c r="AL165" s="10">
         <v>4258.0625</v>
       </c>
-      <c r="AM165" s="12">
-        <v>95</v>
+      <c r="AM165" s="3">
+        <v>1.6442000000000001</v>
       </c>
       <c r="AN165" s="3">
         <v>104</v>
@@ -22406,11 +22243,8 @@
       <c r="BE165" s="3">
         <v>0.1</v>
       </c>
-      <c r="BF165" s="3">
-        <v>1.6442000000000001</v>
-      </c>
-    </row>
-    <row r="166" spans="2:58">
+    </row>
+    <row r="166" spans="2:57">
       <c r="B166" s="4">
         <v>1990</v>
       </c>
@@ -22522,8 +22356,8 @@
       <c r="AL166" s="10">
         <v>4278</v>
       </c>
-      <c r="AM166" s="12">
-        <v>92</v>
+      <c r="AM166" s="3">
+        <v>1.4482999999999999</v>
       </c>
       <c r="AN166" s="3">
         <v>102</v>
@@ -22579,11 +22413,8 @@
       <c r="BE166" s="3">
         <v>0.13</v>
       </c>
-      <c r="BF166" s="3">
-        <v>1.4482999999999999</v>
-      </c>
-    </row>
-    <row r="167" spans="2:58">
+    </row>
+    <row r="167" spans="2:57">
       <c r="B167" s="4">
         <v>1990.25</v>
       </c>
@@ -22695,8 +22526,8 @@
       <c r="AL167" s="10">
         <v>4304.6778000000004</v>
       </c>
-      <c r="AM167" s="12">
-        <v>86</v>
+      <c r="AM167" s="3">
+        <v>1.2152000000000001</v>
       </c>
       <c r="AN167" s="3">
         <v>102</v>
@@ -22752,11 +22583,8 @@
       <c r="BE167" s="3">
         <v>0.25</v>
       </c>
-      <c r="BF167" s="3">
-        <v>1.2152000000000001</v>
-      </c>
-    </row>
-    <row r="168" spans="2:58">
+    </row>
+    <row r="168" spans="2:57">
       <c r="B168" s="4">
         <v>1990.5</v>
       </c>
@@ -22868,8 +22696,8 @@
       <c r="AL168" s="10">
         <v>4243.4083000000001</v>
       </c>
-      <c r="AM168" s="12">
-        <v>74</v>
+      <c r="AM168" s="3">
+        <v>1.2535000000000001</v>
       </c>
       <c r="AN168" s="3">
         <v>83</v>
@@ -22925,11 +22753,8 @@
       <c r="BE168" s="3">
         <v>0.1225</v>
       </c>
-      <c r="BF168" s="3">
-        <v>1.2535000000000001</v>
-      </c>
-    </row>
-    <row r="169" spans="2:58">
+    </row>
+    <row r="169" spans="2:57">
       <c r="B169" s="4">
         <v>1990.75</v>
       </c>
@@ -23041,8 +22866,8 @@
       <c r="AL169" s="10">
         <v>4193.8633</v>
       </c>
-      <c r="AM169" s="12">
-        <v>58</v>
+      <c r="AM169" s="3">
+        <v>1.6213</v>
       </c>
       <c r="AN169" s="3">
         <v>75</v>
@@ -23098,11 +22923,8 @@
       <c r="BE169" s="3">
         <v>0.15</v>
       </c>
-      <c r="BF169" s="3">
-        <v>1.6213</v>
-      </c>
-    </row>
-    <row r="170" spans="2:58">
+    </row>
+    <row r="170" spans="2:57">
       <c r="B170" s="4">
         <v>1991</v>
       </c>
@@ -23214,8 +23036,8 @@
       <c r="AL170" s="10">
         <v>4205.16</v>
       </c>
-      <c r="AM170" s="12">
-        <v>75</v>
+      <c r="AM170" s="3">
+        <v>1.5216000000000001</v>
       </c>
       <c r="AN170" s="3">
         <v>107</v>
@@ -23271,11 +23093,8 @@
       <c r="BE170" s="3">
         <v>0.1535</v>
       </c>
-      <c r="BF170" s="3">
-        <v>1.5216000000000001</v>
-      </c>
-    </row>
-    <row r="171" spans="2:58">
+    </row>
+    <row r="171" spans="2:57">
       <c r="B171" s="4">
         <v>1991.25</v>
       </c>
@@ -23387,8 +23206,8 @@
       <c r="AL171" s="10">
         <v>4231.3615</v>
       </c>
-      <c r="AM171" s="12">
-        <v>79</v>
+      <c r="AM171" s="3">
+        <v>1.4752000000000001</v>
       </c>
       <c r="AN171" s="3">
         <v>118</v>
@@ -23444,11 +23263,8 @@
       <c r="BE171" s="3">
         <v>0.12</v>
       </c>
-      <c r="BF171" s="3">
-        <v>1.4752000000000001</v>
-      </c>
-    </row>
-    <row r="172" spans="2:58">
+    </row>
+    <row r="172" spans="2:57">
       <c r="B172" s="4">
         <v>1991.5</v>
       </c>
@@ -23560,8 +23376,8 @@
       <c r="AL172" s="10">
         <v>4274.6832999999997</v>
       </c>
-      <c r="AM172" s="12">
-        <v>83</v>
+      <c r="AM172" s="3">
+        <v>1.4875</v>
       </c>
       <c r="AN172" s="3">
         <v>117</v>
@@ -23617,11 +23433,8 @@
       <c r="BE172" s="3">
         <v>0.1</v>
       </c>
-      <c r="BF172" s="3">
-        <v>1.4875</v>
-      </c>
-    </row>
-    <row r="173" spans="2:58">
+    </row>
+    <row r="173" spans="2:57">
       <c r="B173" s="4">
         <v>1991.75</v>
       </c>
@@ -23733,8 +23546,8 @@
       <c r="AL173" s="10">
         <v>4270.5102999999999</v>
       </c>
-      <c r="AM173" s="12">
-        <v>65</v>
+      <c r="AM173" s="3">
+        <v>1.5107999999999999</v>
       </c>
       <c r="AN173" s="3">
         <v>100</v>
@@ -23790,11 +23603,8 @@
       <c r="BE173" s="3">
         <v>0.16200000000000001</v>
       </c>
-      <c r="BF173" s="3">
-        <v>1.5107999999999999</v>
-      </c>
-    </row>
-    <row r="174" spans="2:58">
+    </row>
+    <row r="174" spans="2:57">
       <c r="B174" s="4">
         <v>1992</v>
       </c>
@@ -23906,8 +23716,8 @@
       <c r="AL174" s="10">
         <v>5015.8607000000002</v>
       </c>
-      <c r="AM174" s="12">
-        <v>68</v>
+      <c r="AM174" s="3">
+        <v>1.3742000000000001</v>
       </c>
       <c r="AN174" s="3">
         <v>107</v>
@@ -23963,11 +23773,8 @@
       <c r="BE174" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="BF174" s="3">
-        <v>1.3742000000000001</v>
-      </c>
-    </row>
-    <row r="175" spans="2:58">
+    </row>
+    <row r="175" spans="2:57">
       <c r="B175" s="4">
         <v>1992.25</v>
       </c>
@@ -24079,8 +23886,8 @@
       <c r="AL175" s="10">
         <v>5081.5339000000004</v>
       </c>
-      <c r="AM175" s="12">
-        <v>69</v>
+      <c r="AM175" s="3">
+        <v>1.3351999999999999</v>
       </c>
       <c r="AN175" s="3">
         <v>116</v>
@@ -24136,11 +23943,8 @@
       <c r="BE175" s="3">
         <v>0.111</v>
       </c>
-      <c r="BF175" s="3">
-        <v>1.3351999999999999</v>
-      </c>
-    </row>
-    <row r="176" spans="2:58">
+    </row>
+    <row r="176" spans="2:57">
       <c r="B176" s="4">
         <v>1992.5</v>
       </c>
@@ -24252,8 +24056,8 @@
       <c r="AL176" s="10">
         <v>5054.8796000000002</v>
       </c>
-      <c r="AM176" s="12">
-        <v>70</v>
+      <c r="AM176" s="3">
+        <v>1.5062</v>
       </c>
       <c r="AN176" s="3">
         <v>112</v>
@@ -24309,11 +24113,8 @@
       <c r="BE176" s="3">
         <v>0.10100000000000001</v>
       </c>
-      <c r="BF176" s="3">
-        <v>1.5062</v>
-      </c>
-    </row>
-    <row r="177" spans="2:58">
+    </row>
+    <row r="177" spans="2:57">
       <c r="B177" s="4">
         <v>1992.75</v>
       </c>
@@ -24425,8 +24226,8 @@
       <c r="AL177" s="10">
         <v>5096.3906999999999</v>
       </c>
-      <c r="AM177" s="12">
-        <v>87</v>
+      <c r="AM177" s="3">
+        <v>1.4388000000000001</v>
       </c>
       <c r="AN177" s="3">
         <v>122</v>
@@ -24482,11 +24283,8 @@
       <c r="BE177" s="3">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="BF177" s="3">
-        <v>1.4388000000000001</v>
-      </c>
-    </row>
-    <row r="178" spans="2:58">
+    </row>
+    <row r="178" spans="2:57">
       <c r="B178" s="4">
         <v>1993</v>
       </c>
@@ -24598,8 +24396,8 @@
       <c r="AL178" s="10">
         <v>5170.8735999999999</v>
       </c>
-      <c r="AM178" s="12">
-        <v>94</v>
+      <c r="AM178" s="3">
+        <v>1.4533</v>
       </c>
       <c r="AN178" s="3">
         <v>122</v>
@@ -24655,11 +24453,8 @@
       <c r="BE178" s="3">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="BF178" s="3">
-        <v>1.4533</v>
-      </c>
-    </row>
-    <row r="179" spans="2:58">
+    </row>
+    <row r="179" spans="2:57">
       <c r="B179" s="4">
         <v>1993.25</v>
       </c>
@@ -24771,8 +24566,8 @@
       <c r="AL179" s="10">
         <v>5204.3662000000004</v>
       </c>
-      <c r="AM179" s="12">
-        <v>81</v>
+      <c r="AM179" s="3">
+        <v>1.4012</v>
       </c>
       <c r="AN179" s="3">
         <v>107</v>
@@ -24828,11 +24623,8 @@
       <c r="BE179" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="BF179" s="3">
-        <v>1.4012</v>
-      </c>
-    </row>
-    <row r="180" spans="2:58">
+    </row>
+    <row r="180" spans="2:57">
       <c r="B180" s="4">
         <v>1993.5</v>
       </c>
@@ -24944,8 +24736,8 @@
       <c r="AL180" s="10">
         <v>5196.6360999999997</v>
       </c>
-      <c r="AM180" s="12">
-        <v>72</v>
+      <c r="AM180" s="3">
+        <v>1.4315</v>
       </c>
       <c r="AN180" s="3">
         <v>98</v>
@@ -25001,11 +24793,8 @@
       <c r="BE180" s="3">
         <v>0.1</v>
       </c>
-      <c r="BF180" s="3">
-        <v>1.4315</v>
-      </c>
-    </row>
-    <row r="181" spans="2:58">
+    </row>
+    <row r="181" spans="2:57">
       <c r="B181" s="4">
         <v>1993.75</v>
       </c>
@@ -25117,8 +24906,8 @@
       <c r="AL181" s="10">
         <v>5329.4335000000001</v>
       </c>
-      <c r="AM181" s="12">
-        <v>80</v>
+      <c r="AM181" s="3">
+        <v>1.3460000000000001</v>
       </c>
       <c r="AN181" s="3">
         <v>103</v>
@@ -25174,11 +24963,8 @@
       <c r="BE181" s="3">
         <v>0.06</v>
       </c>
-      <c r="BF181" s="3">
-        <v>1.3460000000000001</v>
-      </c>
-    </row>
-    <row r="182" spans="2:58">
+    </row>
+    <row r="182" spans="2:57">
       <c r="B182" s="4">
         <v>1994</v>
       </c>
@@ -25290,8 +25076,8 @@
       <c r="AL182" s="10">
         <v>5407.4053000000004</v>
       </c>
-      <c r="AM182" s="12">
-        <v>94</v>
+      <c r="AM182" s="3">
+        <v>1.2428999999999999</v>
       </c>
       <c r="AN182" s="3">
         <v>117</v>
@@ -25347,11 +25133,8 @@
       <c r="BE182" s="3">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="BF182" s="3">
-        <v>1.2428999999999999</v>
-      </c>
-    </row>
-    <row r="183" spans="2:58">
+    </row>
+    <row r="183" spans="2:57">
       <c r="B183" s="4">
         <v>1994.25</v>
       </c>
@@ -25463,8 +25246,8 @@
       <c r="AL183" s="10">
         <v>5460.2984999999999</v>
       </c>
-      <c r="AM183" s="12">
-        <v>93</v>
+      <c r="AM183" s="3">
+        <v>1.2508999999999999</v>
       </c>
       <c r="AN183" s="3">
         <v>109</v>
@@ -25520,11 +25303,8 @@
       <c r="BE183" s="3">
         <v>0.115</v>
       </c>
-      <c r="BF183" s="3">
-        <v>1.2508999999999999</v>
-      </c>
-    </row>
-    <row r="184" spans="2:58">
+    </row>
+    <row r="184" spans="2:57">
       <c r="B184" s="4">
         <v>1994.5</v>
       </c>
@@ -25636,8 +25416,8 @@
       <c r="AL184" s="10">
         <v>5481.3909999999996</v>
       </c>
-      <c r="AM184" s="12">
-        <v>89</v>
+      <c r="AM184" s="3">
+        <v>1.2150000000000001</v>
       </c>
       <c r="AN184" s="3">
         <v>107</v>
@@ -25693,11 +25473,8 @@
       <c r="BE184" s="3">
         <v>0.08</v>
       </c>
-      <c r="BF184" s="3">
-        <v>1.2150000000000001</v>
-      </c>
-    </row>
-    <row r="185" spans="2:58">
+    </row>
+    <row r="185" spans="2:57">
       <c r="B185" s="4">
         <v>1994.75</v>
       </c>
@@ -25809,8 +25586,8 @@
       <c r="AL185" s="10">
         <v>5550.6143000000002</v>
       </c>
-      <c r="AM185" s="12">
-        <v>99</v>
+      <c r="AM185" s="3">
+        <v>1.2815000000000001</v>
       </c>
       <c r="AN185" s="3">
         <v>112</v>
@@ -25866,11 +25643,8 @@
       <c r="BE185" s="3">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="BF185" s="3">
-        <v>1.2815000000000001</v>
-      </c>
-    </row>
-    <row r="186" spans="2:58">
+    </row>
+    <row r="186" spans="2:57">
       <c r="B186" s="4">
         <v>1995</v>
       </c>
@@ -25982,8 +25756,8 @@
       <c r="AL186" s="10">
         <v>5602.8140999999996</v>
       </c>
-      <c r="AM186" s="12">
-        <v>98</v>
+      <c r="AM186" s="3">
+        <v>1.2770999999999999</v>
       </c>
       <c r="AN186" s="3">
         <v>112</v>
@@ -26039,11 +25813,8 @@
       <c r="BE186" s="3">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="BF186" s="3">
-        <v>1.2770999999999999</v>
-      </c>
-    </row>
-    <row r="187" spans="2:58">
+    </row>
+    <row r="187" spans="2:57">
       <c r="B187" s="4">
         <v>1995.25</v>
       </c>
@@ -26155,8 +25926,8 @@
       <c r="AL187" s="10">
         <v>5633.4938000000002</v>
       </c>
-      <c r="AM187" s="12">
-        <v>92</v>
+      <c r="AM187" s="3">
+        <v>1.3073999999999999</v>
       </c>
       <c r="AN187" s="3">
         <v>103</v>
@@ -26212,11 +25983,8 @@
       <c r="BE187" s="3">
         <v>0.12</v>
       </c>
-      <c r="BF187" s="3">
-        <v>1.3073999999999999</v>
-      </c>
-    </row>
-    <row r="188" spans="2:58">
+    </row>
+    <row r="188" spans="2:57">
       <c r="B188" s="4">
         <v>1995.5</v>
       </c>
@@ -26328,8 +26096,8 @@
       <c r="AL188" s="10">
         <v>5658.4949999999999</v>
       </c>
-      <c r="AM188" s="12">
-        <v>95</v>
+      <c r="AM188" s="3">
+        <v>1.3132999999999999</v>
       </c>
       <c r="AN188" s="3">
         <v>108</v>
@@ -26385,11 +26153,8 @@
       <c r="BE188" s="3">
         <v>0.09</v>
       </c>
-      <c r="BF188" s="3">
-        <v>1.3132999999999999</v>
-      </c>
-    </row>
-    <row r="189" spans="2:58">
+    </row>
+    <row r="189" spans="2:57">
       <c r="B189" s="4">
         <v>1995.75</v>
       </c>
@@ -26501,8 +26266,8 @@
       <c r="AL189" s="10">
         <v>5719.8359</v>
       </c>
-      <c r="AM189" s="12">
-        <v>90</v>
+      <c r="AM189" s="3">
+        <v>1.4167000000000001</v>
       </c>
       <c r="AN189" s="3">
         <v>104</v>
@@ -26558,11 +26323,8 @@
       <c r="BE189" s="3">
         <v>0.08</v>
       </c>
-      <c r="BF189" s="3">
-        <v>1.4167000000000001</v>
-      </c>
-    </row>
-    <row r="190" spans="2:58">
+    </row>
+    <row r="190" spans="2:57">
       <c r="B190" s="4">
         <v>1996</v>
       </c>
@@ -26674,8 +26436,8 @@
       <c r="AL190" s="10">
         <v>6972.8486999999996</v>
       </c>
-      <c r="AM190" s="12">
-        <v>84</v>
+      <c r="AM190" s="3">
+        <v>1.3314999999999999</v>
       </c>
       <c r="AN190" s="3">
         <v>103</v>
@@ -26731,11 +26493,8 @@
       <c r="BE190" s="3">
         <v>0.09</v>
       </c>
-      <c r="BF190" s="3">
-        <v>1.3314999999999999</v>
-      </c>
-    </row>
-    <row r="191" spans="2:58">
+    </row>
+    <row r="191" spans="2:57">
       <c r="B191" s="4">
         <v>1996.25</v>
       </c>
@@ -26847,8 +26606,8 @@
       <c r="AL191" s="10">
         <v>7015.8933999999999</v>
       </c>
-      <c r="AM191" s="12">
-        <v>89</v>
+      <c r="AM191" s="3">
+        <v>1.2784</v>
       </c>
       <c r="AN191" s="3">
         <v>104</v>
@@ -26904,11 +26663,8 @@
       <c r="BE191" s="3">
         <v>0.11</v>
       </c>
-      <c r="BF191" s="3">
-        <v>1.2784</v>
-      </c>
-    </row>
-    <row r="192" spans="2:58">
+    </row>
+    <row r="192" spans="2:57">
       <c r="B192" s="4">
         <v>1996.5</v>
       </c>
@@ -27020,8 +26776,8 @@
       <c r="AL192" s="10">
         <v>7072.2407999999996</v>
       </c>
-      <c r="AM192" s="12">
-        <v>101</v>
+      <c r="AM192" s="3">
+        <v>1.2848999999999999</v>
       </c>
       <c r="AN192" s="3">
         <v>108</v>
@@ -27077,11 +26833,8 @@
       <c r="BE192" s="3">
         <v>0.1</v>
       </c>
-      <c r="BF192" s="3">
-        <v>1.2848999999999999</v>
-      </c>
-    </row>
-    <row r="193" spans="2:58">
+    </row>
+    <row r="193" spans="2:57">
       <c r="B193" s="4">
         <v>1996.75</v>
       </c>
@@ -27193,8 +26946,8 @@
       <c r="AL193" s="10">
         <v>7114.8063000000002</v>
       </c>
-      <c r="AM193" s="12">
-        <v>106</v>
+      <c r="AM193" s="3">
+        <v>1.3058000000000001</v>
       </c>
       <c r="AN193" s="3">
         <v>112</v>
@@ -27250,11 +27003,8 @@
       <c r="BE193" s="3">
         <v>7.5499999999999998E-2</v>
       </c>
-      <c r="BF193" s="3">
-        <v>1.3058000000000001</v>
-      </c>
-    </row>
-    <row r="194" spans="2:58">
+    </row>
+    <row r="194" spans="2:57">
       <c r="B194" s="4">
         <v>1997</v>
       </c>
@@ -27366,8 +27116,8 @@
       <c r="AL194" s="10">
         <v>7204.6731</v>
       </c>
-      <c r="AM194" s="12">
-        <v>107</v>
+      <c r="AM194" s="3">
+        <v>1.2424999999999999</v>
       </c>
       <c r="AN194" s="3">
         <v>112</v>
@@ -27423,11 +27173,8 @@
       <c r="BE194" s="3">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="BF194" s="3">
-        <v>1.2424999999999999</v>
-      </c>
-    </row>
-    <row r="195" spans="2:58">
+    </row>
+    <row r="195" spans="2:57">
       <c r="B195" s="4">
         <v>1997.25</v>
       </c>
@@ -27539,8 +27286,8 @@
       <c r="AL195" s="10">
         <v>7293.8343999999997</v>
       </c>
-      <c r="AM195" s="12">
-        <v>114</v>
+      <c r="AM195" s="3">
+        <v>1.1975</v>
       </c>
       <c r="AN195" s="3">
         <v>109</v>
@@ -27596,11 +27343,8 @@
       <c r="BE195" s="3">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="BF195" s="3">
-        <v>1.1975</v>
-      </c>
-    </row>
-    <row r="196" spans="2:58">
+    </row>
+    <row r="196" spans="2:57">
       <c r="B196" s="4">
         <v>1997.5</v>
       </c>
@@ -27712,8 +27456,8 @@
       <c r="AL196" s="10">
         <v>7361.4951000000001</v>
       </c>
-      <c r="AM196" s="12">
-        <v>122</v>
+      <c r="AM196" s="3">
+        <v>1.2225999999999999</v>
       </c>
       <c r="AN196" s="3">
         <v>118</v>
@@ -27769,11 +27513,8 @@
       <c r="BE196" s="3">
         <v>0.1</v>
       </c>
-      <c r="BF196" s="3">
-        <v>1.2225999999999999</v>
-      </c>
-    </row>
-    <row r="197" spans="2:58">
+    </row>
+    <row r="197" spans="2:57">
       <c r="B197" s="4">
         <v>1997.75</v>
       </c>
@@ -27885,8 +27626,8 @@
       <c r="AL197" s="10">
         <v>7441.924</v>
       </c>
-      <c r="AM197" s="12">
-        <v>119</v>
+      <c r="AM197" s="3">
+        <v>1.3562000000000001</v>
       </c>
       <c r="AN197" s="3">
         <v>114</v>
@@ -27942,11 +27683,8 @@
       <c r="BE197" s="3">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="BF197" s="3">
-        <v>1.3562000000000001</v>
-      </c>
-    </row>
-    <row r="198" spans="2:58">
+    </row>
+    <row r="198" spans="2:57">
       <c r="B198" s="4">
         <v>1998</v>
       </c>
@@ -28058,8 +27796,8 @@
       <c r="AL198" s="10">
         <v>7509.5862999999999</v>
       </c>
-      <c r="AM198" s="12">
-        <v>121</v>
+      <c r="AM198" s="3">
+        <v>1.3443000000000001</v>
       </c>
       <c r="AN198" s="3">
         <v>117</v>
@@ -28115,11 +27853,8 @@
       <c r="BE198" s="3">
         <v>0.11600000000000001</v>
       </c>
-      <c r="BF198" s="3">
-        <v>1.3443000000000001</v>
-      </c>
-    </row>
-    <row r="199" spans="2:58">
+    </row>
+    <row r="199" spans="2:57">
       <c r="B199" s="4">
         <v>1998.25</v>
       </c>
@@ -28231,8 +27966,8 @@
       <c r="AL199" s="10">
         <v>7582.7902000000004</v>
       </c>
-      <c r="AM199" s="12">
-        <v>118</v>
+      <c r="AM199" s="3">
+        <v>1.3249</v>
       </c>
       <c r="AN199" s="3">
         <v>114</v>
@@ -28288,11 +28023,8 @@
       <c r="BE199" s="3">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="BF199" s="3">
-        <v>1.3249</v>
-      </c>
-    </row>
-    <row r="200" spans="2:58">
+    </row>
+    <row r="200" spans="2:57">
       <c r="B200" s="4">
         <v>1998.5</v>
       </c>
@@ -28404,8 +28136,8 @@
       <c r="AL200" s="10">
         <v>7725.884</v>
       </c>
-      <c r="AM200" s="12">
-        <v>116</v>
+      <c r="AM200" s="3">
+        <v>2.0169000000000001</v>
       </c>
       <c r="AN200" s="3">
         <v>110</v>
@@ -28461,11 +28193,8 @@
       <c r="BE200" s="3">
         <v>0.1265</v>
       </c>
-      <c r="BF200" s="3">
-        <v>2.0169000000000001</v>
-      </c>
-    </row>
-    <row r="201" spans="2:58">
+    </row>
+    <row r="201" spans="2:57">
       <c r="B201" s="4">
         <v>1998.75</v>
       </c>
@@ -28577,8 +28306,8 @@
       <c r="AL201" s="10">
         <v>7756.8599000000004</v>
       </c>
-      <c r="AM201" s="12">
-        <v>107</v>
+      <c r="AM201" s="3">
+        <v>2.1269</v>
       </c>
       <c r="AN201" s="3">
         <v>103</v>
@@ -28634,11 +28363,8 @@
       <c r="BE201" s="3">
         <v>0.09</v>
       </c>
-      <c r="BF201" s="3">
-        <v>2.1269</v>
-      </c>
-    </row>
-    <row r="202" spans="2:58">
+    </row>
+    <row r="202" spans="2:57">
       <c r="B202" s="4">
         <v>1999</v>
       </c>
@@ -28750,8 +28476,8 @@
       <c r="AL202" s="10">
         <v>7904.7511000000004</v>
       </c>
-      <c r="AM202" s="12">
-        <v>120</v>
+      <c r="AM202" s="3">
+        <v>1.833</v>
       </c>
       <c r="AN202" s="3">
         <v>107</v>
@@ -28807,11 +28533,8 @@
       <c r="BE202" s="3">
         <v>0.113</v>
       </c>
-      <c r="BF202" s="3">
-        <v>1.833</v>
-      </c>
-    </row>
-    <row r="203" spans="2:58">
+    </row>
+    <row r="203" spans="2:57">
       <c r="B203" s="4">
         <v>1999.25</v>
       </c>
@@ -28923,8 +28646,8 @@
       <c r="AL203" s="10">
         <v>8020.2395999999999</v>
       </c>
-      <c r="AM203" s="12">
-        <v>117</v>
+      <c r="AM203" s="3">
+        <v>1.7621</v>
       </c>
       <c r="AN203" s="3">
         <v>110</v>
@@ -28980,11 +28703,8 @@
       <c r="BE203" s="3">
         <v>0.152</v>
       </c>
-      <c r="BF203" s="3">
-        <v>1.7621</v>
-      </c>
-    </row>
-    <row r="204" spans="2:58">
+    </row>
+    <row r="204" spans="2:57">
       <c r="B204" s="4">
         <v>1999.5</v>
       </c>
@@ -29096,8 +28816,8 @@
       <c r="AL204" s="10">
         <v>8075.5977000000003</v>
       </c>
-      <c r="AM204" s="12">
-        <v>120</v>
+      <c r="AM204" s="3">
+        <v>2.0268999999999999</v>
       </c>
       <c r="AN204" s="3">
         <v>108</v>
@@ -29153,11 +28873,8 @@
       <c r="BE204" s="3">
         <v>0.105</v>
       </c>
-      <c r="BF204" s="3">
-        <v>2.0268999999999999</v>
-      </c>
-    </row>
-    <row r="205" spans="2:58">
+    </row>
+    <row r="205" spans="2:57">
       <c r="B205" s="4">
         <v>1999.75</v>
       </c>
@@ -29269,8 +28986,8 @@
       <c r="AL205" s="10">
         <v>9227.3778000000002</v>
       </c>
-      <c r="AM205" s="12">
-        <v>122</v>
+      <c r="AM205" s="3">
+        <v>2.0446</v>
       </c>
       <c r="AN205" s="3">
         <v>110</v>
@@ -29326,11 +29043,8 @@
       <c r="BE205" s="3">
         <v>0.09</v>
       </c>
-      <c r="BF205" s="3">
-        <v>2.0446</v>
-      </c>
-    </row>
-    <row r="206" spans="2:58">
+    </row>
+    <row r="206" spans="2:57">
       <c r="B206" s="4">
         <v>2000</v>
       </c>
@@ -29442,8 +29156,8 @@
       <c r="AL206" s="10">
         <v>9367.4786999999997</v>
       </c>
-      <c r="AM206" s="12">
-        <v>132</v>
+      <c r="AM206" s="3">
+        <v>2.3315999999999999</v>
       </c>
       <c r="AN206" s="3">
         <v>117</v>
@@ -29499,11 +29213,8 @@
       <c r="BE206" s="3">
         <v>0.112</v>
       </c>
-      <c r="BF206" s="3">
-        <v>2.3315999999999999</v>
-      </c>
-    </row>
-    <row r="207" spans="2:58">
+    </row>
+    <row r="207" spans="2:57">
       <c r="B207" s="4">
         <v>2000.25</v>
       </c>
@@ -29615,8 +29326,8 @@
       <c r="AL207" s="10">
         <v>9559.0841999999993</v>
       </c>
-      <c r="AM207" s="12">
-        <v>129</v>
+      <c r="AM207" s="3">
+        <v>2.835</v>
       </c>
       <c r="AN207" s="3">
         <v>113</v>
@@ -29672,11 +29383,8 @@
       <c r="BE207" s="3">
         <v>0.11749999999999999</v>
       </c>
-      <c r="BF207" s="3">
-        <v>2.835</v>
-      </c>
-    </row>
-    <row r="208" spans="2:58">
+    </row>
+    <row r="208" spans="2:57">
       <c r="B208" s="4">
         <v>2000.5</v>
       </c>
@@ -29788,8 +29496,8 @@
       <c r="AL208" s="10">
         <v>9679.2191999999995</v>
       </c>
-      <c r="AM208" s="12">
-        <v>134</v>
+      <c r="AM208" s="3">
+        <v>3.2391999999999999</v>
       </c>
       <c r="AN208" s="3">
         <v>112</v>
@@ -29845,11 +29553,8 @@
       <c r="BE208" s="3">
         <v>0.113</v>
       </c>
-      <c r="BF208" s="3">
-        <v>3.2391999999999999</v>
-      </c>
-    </row>
-    <row r="209" spans="2:58">
+    </row>
+    <row r="209" spans="2:57">
       <c r="B209" s="4">
         <v>2000.75</v>
       </c>
@@ -29961,8 +29666,8 @@
       <c r="AL209" s="10">
         <v>9763.1823999999997</v>
       </c>
-      <c r="AM209" s="12">
-        <v>125</v>
+      <c r="AM209" s="3">
+        <v>3.6334</v>
       </c>
       <c r="AN209" s="3">
         <v>109</v>
@@ -30018,11 +29723,8 @@
       <c r="BE209" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="BF209" s="3">
-        <v>3.6334</v>
-      </c>
-    </row>
-    <row r="210" spans="2:58">
+    </row>
+    <row r="210" spans="2:57">
       <c r="B210" s="4">
         <v>2001</v>
       </c>
@@ -30134,8 +29836,8 @@
       <c r="AL210" s="10">
         <v>9712.6553000000004</v>
       </c>
-      <c r="AM210" s="12">
-        <v>109</v>
+      <c r="AM210" s="3">
+        <v>3.2886000000000002</v>
       </c>
       <c r="AN210" s="3">
         <v>102</v>
@@ -30191,11 +29893,8 @@
       <c r="BE210" s="3">
         <v>0.09</v>
       </c>
-      <c r="BF210" s="3">
-        <v>3.2886000000000002</v>
-      </c>
-    </row>
-    <row r="211" spans="2:58">
+    </row>
+    <row r="211" spans="2:57">
       <c r="B211" s="4">
         <v>2001.25</v>
       </c>
@@ -30307,8 +30006,8 @@
       <c r="AL211" s="10">
         <v>9738.5184000000008</v>
       </c>
-      <c r="AM211" s="12">
-        <v>109</v>
+      <c r="AM211" s="3">
+        <v>3.1236000000000002</v>
       </c>
       <c r="AN211" s="3">
         <v>107</v>
@@ -30364,11 +30063,8 @@
       <c r="BE211" s="3">
         <v>0.10299999999999999</v>
       </c>
-      <c r="BF211" s="3">
-        <v>3.1236000000000002</v>
-      </c>
-    </row>
-    <row r="212" spans="2:58">
+    </row>
+    <row r="212" spans="2:57">
       <c r="B212" s="4">
         <v>2001.5</v>
       </c>
@@ -30480,8 +30176,8 @@
       <c r="AL212" s="10">
         <v>9654.2819999999992</v>
       </c>
-      <c r="AM212" s="12">
-        <v>105</v>
+      <c r="AM212" s="3">
+        <v>3.3347000000000002</v>
       </c>
       <c r="AN212" s="3">
         <v>108</v>
@@ -30537,11 +30233,8 @@
       <c r="BE212" s="3">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="BF212" s="3">
-        <v>3.3347000000000002</v>
-      </c>
-    </row>
-    <row r="213" spans="2:58">
+    </row>
+    <row r="213" spans="2:57">
       <c r="B213" s="4">
         <v>2001.75</v>
       </c>
@@ -30653,8 +30346,8 @@
       <c r="AL213" s="10">
         <v>9517.2214000000004</v>
       </c>
-      <c r="AM213" s="12">
-        <v>100</v>
+      <c r="AM213" s="3">
+        <v>3.0945</v>
       </c>
       <c r="AN213" s="3">
         <v>124</v>
@@ -30710,11 +30403,8 @@
       <c r="BE213" s="3">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="BF213" s="3">
-        <v>3.0945</v>
-      </c>
-    </row>
-    <row r="214" spans="2:58">
+    </row>
+    <row r="214" spans="2:57">
       <c r="B214" s="4">
         <v>2002</v>
       </c>
@@ -30826,8 +30516,8 @@
       <c r="AL214" s="10">
         <v>9644.9868000000006</v>
       </c>
-      <c r="AM214" s="12">
-        <v>113</v>
+      <c r="AM214" s="3">
+        <v>2.7568000000000001</v>
       </c>
       <c r="AN214" s="3">
         <v>140</v>
@@ -30883,11 +30573,8 @@
       <c r="BE214" s="3">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="BF214" s="3">
-        <v>2.7568000000000001</v>
-      </c>
-    </row>
-    <row r="215" spans="2:58">
+    </row>
+    <row r="215" spans="2:57">
       <c r="B215" s="4">
         <v>2002.25</v>
       </c>
@@ -30999,8 +30686,8 @@
       <c r="AL215" s="10">
         <v>9858.2685999999994</v>
       </c>
-      <c r="AM215" s="12">
-        <v>109</v>
+      <c r="AM215" s="3">
+        <v>3.1526999999999998</v>
       </c>
       <c r="AN215" s="3">
         <v>130</v>
@@ -31056,11 +30743,8 @@
       <c r="BE215" s="3">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="BF215" s="3">
-        <v>3.1526999999999998</v>
-      </c>
-    </row>
-    <row r="216" spans="2:58">
+    </row>
+    <row r="216" spans="2:57">
       <c r="B216" s="4">
         <v>2002.5</v>
       </c>
@@ -31172,8 +30856,8 @@
       <c r="AL216" s="10">
         <v>9757.9624999999996</v>
       </c>
-      <c r="AM216" s="12">
-        <v>96</v>
+      <c r="AM216" s="3">
+        <v>4.1440999999999999</v>
       </c>
       <c r="AN216" s="3">
         <v>121</v>
@@ -31229,11 +30913,8 @@
       <c r="BE216" s="3">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="BF216" s="3">
-        <v>4.1440999999999999</v>
-      </c>
-    </row>
-    <row r="217" spans="2:58">
+    </row>
+    <row r="217" spans="2:57">
       <c r="B217" s="4">
         <v>2002.75</v>
       </c>
@@ -31345,8 +31026,8 @@
       <c r="AL217" s="10">
         <v>9805.7348999999995</v>
       </c>
-      <c r="AM217" s="12">
-        <v>92</v>
+      <c r="AM217" s="3">
+        <v>3.87</v>
       </c>
       <c r="AN217" s="3">
         <v>115</v>
@@ -31402,11 +31083,8 @@
       <c r="BE217" s="3">
         <v>0.1</v>
       </c>
-      <c r="BF217" s="3">
-        <v>3.87</v>
-      </c>
-    </row>
-    <row r="218" spans="2:58">
+    </row>
+    <row r="218" spans="2:57">
       <c r="B218" s="4">
         <v>2003</v>
       </c>
@@ -31518,8 +31196,8 @@
       <c r="AL218" s="10">
         <v>9876.2742999999991</v>
       </c>
-      <c r="AM218" s="12">
-        <v>86</v>
+      <c r="AM218" s="3">
+        <v>3.2366999999999999</v>
       </c>
       <c r="AN218" s="3">
         <v>103</v>
@@ -31575,11 +31253,8 @@
       <c r="BE218" s="3">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="BF218" s="3">
-        <v>3.2366999999999999</v>
-      </c>
-    </row>
-    <row r="219" spans="2:58">
+    </row>
+    <row r="219" spans="2:57">
       <c r="B219" s="4">
         <v>2003.25</v>
       </c>
@@ -31691,8 +31366,8 @@
       <c r="AL219" s="10">
         <v>9931.6479999999992</v>
       </c>
-      <c r="AM219" s="12">
-        <v>103</v>
+      <c r="AM219" s="3">
+        <v>2.6349999999999998</v>
       </c>
       <c r="AN219" s="3">
         <v>126</v>
@@ -31748,11 +31423,8 @@
       <c r="BE219" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="BF219" s="3">
-        <v>2.6349999999999998</v>
-      </c>
-    </row>
-    <row r="220" spans="2:58">
+    </row>
+    <row r="220" spans="2:57">
       <c r="B220" s="4">
         <v>2003.5</v>
       </c>
@@ -31864,8 +31536,8 @@
       <c r="AL220" s="10">
         <v>10058.7102</v>
       </c>
-      <c r="AM220" s="12">
-        <v>95</v>
+      <c r="AM220" s="3">
+        <v>2.359</v>
       </c>
       <c r="AN220" s="3">
         <v>120</v>
@@ -31921,11 +31593,8 @@
       <c r="BE220" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="BF220" s="3">
-        <v>2.359</v>
-      </c>
-    </row>
-    <row r="221" spans="2:58">
+    </row>
+    <row r="221" spans="2:57">
       <c r="B221" s="4">
         <v>2003.75</v>
       </c>
@@ -32037,8 +31706,8 @@
       <c r="AL221" s="10">
         <v>10284.9851</v>
       </c>
-      <c r="AM221" s="12">
-        <v>105</v>
+      <c r="AM221" s="3">
+        <v>1.982</v>
       </c>
       <c r="AN221" s="3">
         <v>124</v>
@@ -32094,11 +31763,8 @@
       <c r="BE221" s="3">
         <v>0.12</v>
       </c>
-      <c r="BF221" s="3">
-        <v>1.982</v>
-      </c>
-    </row>
-    <row r="222" spans="2:58">
+    </row>
+    <row r="222" spans="2:57">
       <c r="B222" s="4">
         <v>2004</v>
       </c>
@@ -32210,8 +31876,8 @@
       <c r="AL222" s="10">
         <v>11141.102999999999</v>
       </c>
-      <c r="AM222" s="12">
-        <v>114</v>
+      <c r="AM222" s="3">
+        <v>1.8884000000000001</v>
       </c>
       <c r="AN222" s="3">
         <v>127</v>
@@ -32267,11 +31933,8 @@
       <c r="BE222" s="3">
         <v>0.17499999999999999</v>
       </c>
-      <c r="BF222" s="3">
-        <v>1.8884000000000001</v>
-      </c>
-    </row>
-    <row r="223" spans="2:58">
+    </row>
+    <row r="223" spans="2:57">
       <c r="B223" s="4">
         <v>2004.25</v>
       </c>
@@ -32383,8 +32046,8 @@
       <c r="AL223" s="10">
         <v>11245.808000000001</v>
       </c>
-      <c r="AM223" s="12">
-        <v>103</v>
+      <c r="AM223" s="3">
+        <v>1.8445</v>
       </c>
       <c r="AN223" s="3">
         <v>119</v>
@@ -32440,11 +32103,8 @@
       <c r="BE223" s="3">
         <v>0.115</v>
       </c>
-      <c r="BF223" s="3">
-        <v>1.8445</v>
-      </c>
-    </row>
-    <row r="224" spans="2:58">
+    </row>
+    <row r="224" spans="2:57">
       <c r="B224" s="4">
         <v>2004.5</v>
       </c>
@@ -32556,8 +32216,8 @@
       <c r="AL224" s="10">
         <v>11267.0409</v>
       </c>
-      <c r="AM224" s="12">
-        <v>109</v>
+      <c r="AM224" s="3">
+        <v>1.8208</v>
       </c>
       <c r="AN224" s="3">
         <v>124</v>
@@ -32613,11 +32273,8 @@
       <c r="BE224" s="3">
         <v>0.11</v>
       </c>
-      <c r="BF224" s="3">
-        <v>1.8208</v>
-      </c>
-    </row>
-    <row r="225" spans="2:58">
+    </row>
+    <row r="225" spans="2:57">
       <c r="B225" s="4">
         <v>2004.75</v>
       </c>
@@ -32729,8 +32386,8 @@
       <c r="AL225" s="10">
         <v>11366.8073</v>
       </c>
-      <c r="AM225" s="12">
-        <v>105</v>
+      <c r="AM225" s="3">
+        <v>1.6519999999999999</v>
       </c>
       <c r="AN225" s="3">
         <v>119</v>
@@ -32786,11 +32443,8 @@
       <c r="BE225" s="3">
         <v>0.13600000000000001</v>
       </c>
-      <c r="BF225" s="3">
-        <v>1.6519999999999999</v>
-      </c>
-    </row>
-    <row r="226" spans="2:58">
+    </row>
+    <row r="226" spans="2:57">
       <c r="B226" s="4">
         <v>2005</v>
       </c>
@@ -32902,8 +32556,8 @@
       <c r="AL226" s="10">
         <v>11473.721299999999</v>
       </c>
-      <c r="AM226" s="12">
-        <v>97</v>
+      <c r="AM226" s="3">
+        <v>1.8519000000000001</v>
       </c>
       <c r="AN226" s="3">
         <v>110</v>
@@ -32959,11 +32613,8 @@
       <c r="BE226" s="3">
         <v>0.13300000000000001</v>
       </c>
-      <c r="BF226" s="3">
-        <v>1.8519000000000001</v>
-      </c>
-    </row>
-    <row r="227" spans="2:58">
+    </row>
+    <row r="227" spans="2:57">
       <c r="B227" s="4">
         <v>2005.25</v>
       </c>
@@ -33075,8 +32726,8 @@
       <c r="AL227" s="10">
         <v>11533.703299999999</v>
       </c>
-      <c r="AM227" s="12">
-        <v>93</v>
+      <c r="AM227" s="3">
+        <v>1.9699</v>
       </c>
       <c r="AN227" s="3">
         <v>100</v>
@@ -33132,11 +32783,8 @@
       <c r="BE227" s="3">
         <v>0.15</v>
       </c>
-      <c r="BF227" s="3">
-        <v>1.9699</v>
-      </c>
-    </row>
-    <row r="228" spans="2:58">
+    </row>
+    <row r="228" spans="2:57">
       <c r="B228" s="4">
         <v>2005.5</v>
       </c>
@@ -33248,8 +32896,8 @@
       <c r="AL228" s="10">
         <v>11573.257100000001</v>
       </c>
-      <c r="AM228" s="12">
-        <v>86</v>
+      <c r="AM228" s="3">
+        <v>1.7806999999999999</v>
       </c>
       <c r="AN228" s="3">
         <v>94</v>
@@ -33305,11 +32953,8 @@
       <c r="BE228" s="3">
         <v>0.1555</v>
       </c>
-      <c r="BF228" s="3">
-        <v>1.7806999999999999</v>
-      </c>
-    </row>
-    <row r="229" spans="2:58">
+    </row>
+    <row r="229" spans="2:57">
       <c r="B229" s="4">
         <v>2005.75</v>
       </c>
@@ -33421,8 +33066,8 @@
       <c r="AL229" s="10">
         <v>11652.688599999999</v>
       </c>
-      <c r="AM229" s="12">
-        <v>80</v>
+      <c r="AM229" s="3">
+        <v>1.8502000000000001</v>
       </c>
       <c r="AN229" s="3">
         <v>96</v>
@@ -33478,11 +33123,8 @@
       <c r="BE229" s="3">
         <v>0.14699999999999999</v>
       </c>
-      <c r="BF229" s="3">
-        <v>1.8502000000000001</v>
-      </c>
-    </row>
-    <row r="230" spans="2:58">
+    </row>
+    <row r="230" spans="2:57">
       <c r="B230" s="4">
         <v>2006</v>
       </c>
@@ -33594,8 +33236,8 @@
       <c r="AL230" s="10">
         <v>11703.1333</v>
       </c>
-      <c r="AM230" s="12">
-        <v>86</v>
+      <c r="AM230" s="3">
+        <v>1.6903999999999999</v>
       </c>
       <c r="AN230" s="3">
         <v>98</v>
@@ -33651,11 +33293,8 @@
       <c r="BE230" s="3">
         <v>0.14799999999999999</v>
       </c>
-      <c r="BF230" s="3">
-        <v>1.6903999999999999</v>
-      </c>
-    </row>
-    <row r="231" spans="2:58">
+    </row>
+    <row r="231" spans="2:57">
       <c r="B231" s="4">
         <v>2006.25</v>
       </c>
@@ -33767,8 +33406,8 @@
       <c r="AL231" s="10">
         <v>11813.453100000001</v>
       </c>
-      <c r="AM231" s="12">
-        <v>81</v>
+      <c r="AM231" s="3">
+        <v>1.6846000000000001</v>
       </c>
       <c r="AN231" s="3">
         <v>86</v>
@@ -33824,11 +33463,8 @@
       <c r="BE231" s="3">
         <v>0.18</v>
       </c>
-      <c r="BF231" s="3">
-        <v>1.6846000000000001</v>
-      </c>
-    </row>
-    <row r="232" spans="2:58">
+    </row>
+    <row r="232" spans="2:57">
       <c r="B232" s="4">
         <v>2006.5</v>
       </c>
@@ -33940,8 +33576,8 @@
       <c r="AL232" s="10">
         <v>11781.614</v>
       </c>
-      <c r="AM232" s="12">
-        <v>86</v>
+      <c r="AM232" s="3">
+        <v>1.772</v>
       </c>
       <c r="AN232" s="3">
         <v>89</v>
@@ -33997,11 +33633,8 @@
       <c r="BE232" s="3">
         <v>0.14099999999999999</v>
       </c>
-      <c r="BF232" s="3">
-        <v>1.772</v>
-      </c>
-    </row>
-    <row r="233" spans="2:58">
+    </row>
+    <row r="233" spans="2:57">
       <c r="B233" s="4">
         <v>2006.75</v>
       </c>
@@ -34113,8 +33746,8 @@
       <c r="AL233" s="10">
         <v>11818.911</v>
       </c>
-      <c r="AM233" s="12">
-        <v>97</v>
+      <c r="AM233" s="3">
+        <v>1.6173999999999999</v>
       </c>
       <c r="AN233" s="3">
         <v>102</v>
@@ -34170,11 +33803,8 @@
       <c r="BE233" s="3">
         <v>0.13880000000000001</v>
       </c>
-      <c r="BF233" s="3">
-        <v>1.6173999999999999</v>
-      </c>
-    </row>
-    <row r="234" spans="2:58">
+    </row>
+    <row r="234" spans="2:57">
       <c r="B234" s="4">
         <v>2007</v>
       </c>
@@ -34286,8 +33916,8 @@
       <c r="AL234" s="10">
         <v>11951.517400000001</v>
       </c>
-      <c r="AM234" s="12">
-        <v>100</v>
+      <c r="AM234" s="3">
+        <v>1.5329999999999999</v>
       </c>
       <c r="AN234" s="3">
         <v>101</v>
@@ -34343,11 +33973,8 @@
       <c r="BE234" s="3">
         <v>0.1232</v>
       </c>
-      <c r="BF234" s="3">
-        <v>1.5329999999999999</v>
-      </c>
-    </row>
-    <row r="235" spans="2:58">
+    </row>
+    <row r="235" spans="2:57">
       <c r="B235" s="4">
         <v>2007.25</v>
       </c>
@@ -34459,8 +34086,8 @@
       <c r="AL235" s="10">
         <v>11945.093000000001</v>
       </c>
-      <c r="AM235" s="12">
-        <v>89</v>
+      <c r="AM235" s="3">
+        <v>1.6978</v>
       </c>
       <c r="AN235" s="3">
         <v>93</v>
@@ -34516,11 +34143,8 @@
       <c r="BE235" s="3">
         <v>9.4E-2</v>
       </c>
-      <c r="BF235" s="3">
-        <v>1.6978</v>
-      </c>
-    </row>
-    <row r="236" spans="2:58">
+    </row>
+    <row r="236" spans="2:57">
       <c r="B236" s="4">
         <v>2007.5</v>
       </c>
@@ -34632,8 +34256,8 @@
       <c r="AL236" s="10">
         <v>11888.040800000001</v>
       </c>
-      <c r="AM236" s="12">
-        <v>93</v>
+      <c r="AM236" s="3">
+        <v>2.2343999999999999</v>
       </c>
       <c r="AN236" s="3">
         <v>93</v>
@@ -34689,11 +34313,8 @@
       <c r="BE236" s="3">
         <v>0.13400000000000001</v>
       </c>
-      <c r="BF236" s="3">
-        <v>2.2343999999999999</v>
-      </c>
-    </row>
-    <row r="237" spans="2:58">
+    </row>
+    <row r="237" spans="2:57">
       <c r="B237" s="4">
         <v>2007.75</v>
       </c>
@@ -34805,8 +34426,8 @@
       <c r="AL237" s="10">
         <v>11965.8781</v>
       </c>
-      <c r="AM237" s="12">
-        <v>80</v>
+      <c r="AM237" s="3">
+        <v>2.7972999999999999</v>
       </c>
       <c r="AN237" s="3">
         <v>87</v>
@@ -34862,11 +34483,8 @@
       <c r="BE237" s="3">
         <v>0.1971</v>
       </c>
-      <c r="BF237" s="3">
-        <v>2.7972999999999999</v>
-      </c>
-    </row>
-    <row r="238" spans="2:58">
+    </row>
+    <row r="238" spans="2:57">
       <c r="B238" s="4">
         <v>2008</v>
       </c>
@@ -34978,8 +34596,8 @@
       <c r="AL238" s="10">
         <v>11979.1163</v>
       </c>
-      <c r="AM238" s="12">
-        <v>84</v>
+      <c r="AM238" s="3">
+        <v>3.5019999999999998</v>
       </c>
       <c r="AN238" s="3">
         <v>92</v>
@@ -35035,11 +34653,8 @@
       <c r="BE238" s="3">
         <v>0.20100000000000001</v>
       </c>
-      <c r="BF238" s="3">
-        <v>3.5019999999999998</v>
-      </c>
-    </row>
-    <row r="239" spans="2:58">
+    </row>
+    <row r="239" spans="2:57">
       <c r="B239" s="4">
         <v>2008.25</v>
       </c>
@@ -35151,8 +34766,8 @@
       <c r="AL239" s="10">
         <v>11936.965700000001</v>
       </c>
-      <c r="AM239" s="12">
-        <v>66</v>
+      <c r="AM239" s="3">
+        <v>3.4013</v>
       </c>
       <c r="AN239" s="3">
         <v>78</v>
@@ -35208,11 +34823,8 @@
       <c r="BE239" s="3">
         <v>0.1076</v>
       </c>
-      <c r="BF239" s="3">
-        <v>3.4013</v>
-      </c>
-    </row>
-    <row r="240" spans="2:58">
+    </row>
+    <row r="240" spans="2:57">
       <c r="B240" s="4">
         <v>2008.5</v>
       </c>
@@ -35324,8 +34936,8 @@
       <c r="AL240" s="10">
         <v>11931.8172</v>
       </c>
-      <c r="AM240" s="12">
-        <v>74</v>
+      <c r="AM240" s="3">
+        <v>4.8465999999999996</v>
       </c>
       <c r="AN240" s="3">
         <v>93</v>
@@ -35381,11 +34993,8 @@
       <c r="BE240" s="3">
         <v>0.22</v>
       </c>
-      <c r="BF240" s="3">
-        <v>4.8465999999999996</v>
-      </c>
-    </row>
-    <row r="241" spans="2:58">
+    </row>
+    <row r="241" spans="2:57">
       <c r="B241" s="4">
         <v>2008.75</v>
       </c>
@@ -35497,8 +35106,8 @@
       <c r="AL241" s="10">
         <v>11735.748600000001</v>
       </c>
-      <c r="AM241" s="12">
-        <v>67</v>
+      <c r="AM241" s="3">
+        <v>7.2518000000000002</v>
       </c>
       <c r="AN241" s="3">
         <v>100</v>
@@ -35554,11 +35163,8 @@
       <c r="BE241" s="3">
         <v>0.17</v>
       </c>
-      <c r="BF241" s="3">
-        <v>7.2518000000000002</v>
-      </c>
-    </row>
-    <row r="242" spans="2:58">
+    </row>
+    <row r="242" spans="2:57">
       <c r="B242" s="4">
         <v>2009</v>
       </c>
@@ -35670,8 +35276,8 @@
       <c r="AL242" s="10">
         <v>11550.893599999999</v>
       </c>
-      <c r="AM242" s="12">
-        <v>66</v>
+      <c r="AM242" s="3">
+        <v>6.0926</v>
       </c>
       <c r="AN242" s="3">
         <v>102</v>
@@ -35727,11 +35333,8 @@
       <c r="BE242" s="3">
         <v>0.16830000000000001</v>
       </c>
-      <c r="BF242" s="3">
-        <v>6.0926</v>
-      </c>
-    </row>
-    <row r="243" spans="2:58">
+    </row>
+    <row r="243" spans="2:57">
       <c r="B243" s="4">
         <v>2009.25</v>
       </c>
@@ -35843,8 +35446,8 @@
       <c r="AL243" s="10">
         <v>11502.073399999999</v>
       </c>
-      <c r="AM243" s="12">
-        <v>85</v>
+      <c r="AM243" s="3">
+        <v>4.5029000000000003</v>
       </c>
       <c r="AN243" s="3">
         <v>119</v>
@@ -35900,11 +35503,8 @@
       <c r="BE243" s="3">
         <v>0.22670000000000001</v>
       </c>
-      <c r="BF243" s="3">
-        <v>4.5029000000000003</v>
-      </c>
-    </row>
-    <row r="244" spans="2:58">
+    </row>
+    <row r="244" spans="2:57">
       <c r="B244" s="4">
         <v>2009.5</v>
       </c>
@@ -36016,8 +35616,8 @@
       <c r="AL244" s="10">
         <v>13302.1441</v>
       </c>
-      <c r="AM244" s="12">
-        <v>81</v>
+      <c r="AM244" s="3">
+        <v>3.1901999999999999</v>
       </c>
       <c r="AN244" s="3">
         <v>119</v>
@@ -36073,11 +35673,8 @@
       <c r="BE244" s="3">
         <v>0.19900000000000001</v>
       </c>
-      <c r="BF244" s="3">
-        <v>3.1901999999999999</v>
-      </c>
-    </row>
-    <row r="245" spans="2:58">
+    </row>
+    <row r="245" spans="2:57">
       <c r="B245" s="4">
         <v>2009.75</v>
       </c>
@@ -36189,8 +35786,8 @@
       <c r="AL245" s="10">
         <v>13464.8354</v>
       </c>
-      <c r="AM245" s="12">
-        <v>80</v>
+      <c r="AM245" s="3">
+        <v>2.6547999999999998</v>
       </c>
       <c r="AN245" s="3">
         <v>116</v>
@@ -36246,11 +35843,8 @@
       <c r="BE245" s="3">
         <v>0.13350000000000001</v>
       </c>
-      <c r="BF245" s="3">
-        <v>2.6547999999999998</v>
-      </c>
-    </row>
-    <row r="246" spans="2:58">
+    </row>
+    <row r="246" spans="2:57">
       <c r="B246" s="4">
         <v>2010</v>
       </c>
@@ -36362,8 +35956,8 @@
       <c r="AL246" s="10">
         <v>13624.8172</v>
       </c>
-      <c r="AM246" s="12">
-        <v>84</v>
+      <c r="AM246" s="3">
+        <v>2.3338000000000001</v>
       </c>
       <c r="AN246" s="3">
         <v>120</v>
@@ -36419,11 +36013,8 @@
       <c r="BE246" s="3">
         <v>0.24</v>
       </c>
-      <c r="BF246" s="3">
-        <v>2.3338000000000001</v>
-      </c>
-    </row>
-    <row r="247" spans="2:58">
+    </row>
+    <row r="247" spans="2:57">
       <c r="B247" s="4">
         <v>2010.25</v>
       </c>
@@ -36535,8 +36126,8 @@
       <c r="AL247" s="10">
         <v>13770.6744</v>
       </c>
-      <c r="AM247" s="12">
-        <v>81</v>
+      <c r="AM247" s="3">
+        <v>2.5171999999999999</v>
       </c>
       <c r="AN247" s="3">
         <v>114</v>
@@ -36592,11 +36183,8 @@
       <c r="BE247" s="3">
         <v>0.22800000000000001</v>
       </c>
-      <c r="BF247" s="3">
-        <v>2.5171999999999999</v>
-      </c>
-    </row>
-    <row r="248" spans="2:58">
+    </row>
+    <row r="248" spans="2:57">
       <c r="B248" s="4">
         <v>2010.5</v>
       </c>
@@ -36708,8 +36296,8 @@
       <c r="AL248" s="10">
         <v>13676.7464</v>
       </c>
-      <c r="AM248" s="12">
-        <v>74</v>
+      <c r="AM248" s="3">
+        <v>2.5743</v>
       </c>
       <c r="AN248" s="3">
         <v>103</v>
@@ -36765,11 +36353,8 @@
       <c r="BE248" s="3">
         <v>0.19700000000000001</v>
       </c>
-      <c r="BF248" s="3">
-        <v>2.5743</v>
-      </c>
-    </row>
-    <row r="249" spans="2:58">
+    </row>
+    <row r="249" spans="2:57">
       <c r="B249" s="4">
         <v>2010.75</v>
       </c>
@@ -36881,8 +36466,8 @@
       <c r="AL249" s="10">
         <v>13715.589099999999</v>
       </c>
-      <c r="AM249" s="12">
-        <v>75</v>
+      <c r="AM249" s="3">
+        <v>2.3157999999999999</v>
       </c>
       <c r="AN249" s="3">
         <v>114</v>
@@ -36938,11 +36523,8 @@
       <c r="BE249" s="3">
         <v>0.17199999999999999</v>
       </c>
-      <c r="BF249" s="3">
-        <v>2.3157999999999999</v>
-      </c>
-    </row>
-    <row r="250" spans="2:58">
+    </row>
+    <row r="250" spans="2:57">
       <c r="B250" s="4">
         <v>2011</v>
       </c>
@@ -37054,8 +36636,8 @@
       <c r="AL250" s="10">
         <v>13951.4679</v>
       </c>
-      <c r="AM250" s="12">
-        <v>78</v>
+      <c r="AM250" s="3">
+        <v>2.0299</v>
       </c>
       <c r="AN250" s="3">
         <v>112</v>
@@ -37111,11 +36693,8 @@
       <c r="BE250" s="3">
         <v>0.19500000000000001</v>
       </c>
-      <c r="BF250" s="3">
-        <v>2.0299</v>
-      </c>
-    </row>
-    <row r="251" spans="2:58">
+    </row>
+    <row r="251" spans="2:57">
       <c r="B251" s="4">
         <v>2011.25</v>
       </c>
@@ -37227,8 +36806,8 @@
       <c r="AL251" s="10">
         <v>13980.0453</v>
       </c>
-      <c r="AM251" s="12">
-        <v>78</v>
+      <c r="AM251" s="3">
+        <v>2.1107</v>
       </c>
       <c r="AN251" s="3">
         <v>108</v>
@@ -37284,11 +36863,8 @@
       <c r="BE251" s="3">
         <v>0.17499999999999999</v>
       </c>
-      <c r="BF251" s="3">
-        <v>2.1107</v>
-      </c>
-    </row>
-    <row r="252" spans="2:58">
+    </row>
+    <row r="252" spans="2:57">
       <c r="B252" s="4">
         <v>2011.5</v>
       </c>
@@ -37400,8 +36976,8 @@
       <c r="AL252" s="10">
         <v>13685.0682</v>
       </c>
-      <c r="AM252" s="12">
-        <v>55</v>
+      <c r="AM252" s="3">
+        <v>2.7482000000000002</v>
       </c>
       <c r="AN252" s="3">
         <v>91</v>
@@ -37457,11 +37033,8 @@
       <c r="BE252" s="3">
         <v>0.123</v>
       </c>
-      <c r="BF252" s="3">
-        <v>2.7482000000000002</v>
-      </c>
-    </row>
-    <row r="253" spans="2:58">
+    </row>
+    <row r="253" spans="2:57">
       <c r="B253" s="4">
         <v>2011.75</v>
       </c>
@@ -37549,8 +37122,8 @@
       <c r="AL253" s="10">
         <v>13770.545700000001</v>
       </c>
-      <c r="AM253" s="12">
-        <v>64</v>
+      <c r="AM253" s="3">
+        <v>2.8654000000000002</v>
       </c>
       <c r="AN253" s="3">
         <v>98</v>
@@ -37606,11 +37179,8 @@
       <c r="BE253" s="3">
         <v>8.9499999999999996E-2</v>
       </c>
-      <c r="BF253" s="3">
-        <v>2.8654000000000002</v>
-      </c>
-    </row>
-    <row r="254" spans="2:58">
+    </row>
+    <row r="254" spans="2:57">
       <c r="B254" s="4">
         <v>2012</v>
       </c>
@@ -37698,8 +37268,8 @@
       <c r="AL254" s="10">
         <v>13850.800800000001</v>
       </c>
-      <c r="AM254" s="12">
-        <v>87</v>
+      <c r="AM254" s="3">
+        <v>2.5446</v>
       </c>
       <c r="AN254" s="3">
         <v>116</v>
@@ -37755,11 +37325,8 @@
       <c r="BE254" s="3">
         <v>0.1132</v>
       </c>
-      <c r="BF254" s="3">
-        <v>2.5446</v>
-      </c>
-    </row>
-    <row r="255" spans="2:58">
+    </row>
+    <row r="255" spans="2:57">
       <c r="B255" s="4">
         <v>2012.25</v>
       </c>
@@ -37847,8 +37414,8 @@
       <c r="AL255" s="10">
         <v>13935.9372</v>
       </c>
-      <c r="AM255" s="12">
-        <v>89</v>
+      <c r="AM255" s="3">
+        <v>2.6608999999999998</v>
       </c>
       <c r="AN255" s="3">
         <v>116</v>
@@ -37904,11 +37471,8 @@
       <c r="BE255" s="3">
         <v>0.12870000000000001</v>
       </c>
-      <c r="BF255" s="3">
-        <v>2.6608999999999998</v>
-      </c>
-    </row>
-    <row r="256" spans="2:58">
+    </row>
+    <row r="256" spans="2:57">
       <c r="B256" s="4">
         <v>2012.5</v>
       </c>
@@ -37996,8 +37560,8 @@
       <c r="AL256" s="10">
         <v>13891.9807</v>
       </c>
-      <c r="AM256" s="12">
-        <v>84</v>
+      <c r="AM256" s="3">
+        <v>2.4359999999999999</v>
       </c>
       <c r="AN256" s="3">
         <v>114</v>
@@ -38053,11 +37617,8 @@
       <c r="BE256" s="3">
         <v>0.1411</v>
       </c>
-      <c r="BF256" s="3">
-        <v>2.4359999999999999</v>
-      </c>
-    </row>
-    <row r="257" spans="2:58">
+    </row>
+    <row r="257" spans="2:57">
       <c r="B257" s="4">
         <v>2012.75</v>
       </c>
@@ -38145,8 +37706,8 @@
       <c r="AL257" s="10">
         <v>13997.2996</v>
       </c>
-      <c r="AM257" s="12">
-        <v>93</v>
+      <c r="AM257" s="3">
+        <v>2.2204999999999999</v>
       </c>
       <c r="AN257" s="3">
         <v>115</v>
@@ -38202,11 +37763,8 @@
       <c r="BE257" s="3">
         <v>0.12429999999999999</v>
       </c>
-      <c r="BF257" s="3">
-        <v>2.2204999999999999</v>
-      </c>
-    </row>
-    <row r="258" spans="2:58">
+    </row>
+    <row r="258" spans="2:57">
       <c r="B258" s="4">
         <v>2013</v>
       </c>
@@ -38294,8 +37852,8 @@
       <c r="AL258" s="10">
         <v>14083.2801</v>
       </c>
-      <c r="AM258" s="12">
-        <v>83</v>
+      <c r="AM258" s="3">
+        <v>2.1053999999999999</v>
       </c>
       <c r="AN258" s="3">
         <v>107</v>
@@ -38351,11 +37909,8 @@
       <c r="BE258" s="3">
         <v>0.1489</v>
       </c>
-      <c r="BF258" s="3">
-        <v>2.1053999999999999</v>
-      </c>
-    </row>
-    <row r="259" spans="2:58">
+    </row>
+    <row r="259" spans="2:57">
       <c r="B259" s="4">
         <v>2013.25</v>
       </c>
@@ -38443,8 +37998,8 @@
       <c r="AL259" s="10">
         <v>14191.8524</v>
       </c>
-      <c r="AM259" s="12">
-        <v>87</v>
+      <c r="AM259" s="3">
+        <v>2.0493000000000001</v>
       </c>
       <c r="AN259" s="3">
         <v>110</v>
@@ -38500,11 +38055,8 @@
       <c r="BE259" s="3">
         <v>0.14580000000000001</v>
       </c>
-      <c r="BF259" s="3">
-        <v>2.0493000000000001</v>
-      </c>
-    </row>
-    <row r="260" spans="2:58">
+    </row>
+    <row r="260" spans="2:57">
       <c r="B260" s="4">
         <v>2013.5</v>
       </c>
@@ -38592,8 +38144,8 @@
       <c r="AL260" s="10">
         <v>16168.933000000001</v>
       </c>
-      <c r="AM260" s="12">
-        <v>82</v>
+      <c r="AM260" s="3">
+        <v>2.0004</v>
       </c>
       <c r="AN260" s="3">
         <v>101</v>
@@ -38649,11 +38201,8 @@
       <c r="BE260" s="3">
         <v>0.192</v>
       </c>
-      <c r="BF260" s="3">
-        <v>2.0004</v>
-      </c>
-    </row>
-    <row r="261" spans="2:58">
+    </row>
+    <row r="261" spans="2:57">
       <c r="B261" s="4">
         <v>2013.75</v>
       </c>
@@ -38741,8 +38290,8 @@
       <c r="AL261" s="10">
         <v>16298.6389</v>
       </c>
-      <c r="AM261" s="12">
-        <v>81</v>
+      <c r="AM261" s="3">
+        <v>1.8586</v>
       </c>
       <c r="AN261" s="3">
         <v>96</v>
@@ -38798,11 +38347,8 @@
       <c r="BE261" s="3">
         <v>0.22819999999999999</v>
       </c>
-      <c r="BF261" s="3">
-        <v>1.8586</v>
-      </c>
-    </row>
-    <row r="262" spans="2:58">
+    </row>
+    <row r="262" spans="2:57">
       <c r="B262" s="4">
         <v>2014</v>
       </c>
@@ -38890,8 +38436,8 @@
       <c r="AL262" s="10">
         <v>16517.545999999998</v>
       </c>
-      <c r="AM262" s="12">
-        <v>78</v>
+      <c r="AM262" s="3">
+        <v>1.6918</v>
       </c>
       <c r="AN262" s="3">
         <v>100</v>
@@ -38947,11 +38493,8 @@
       <c r="BE262" s="3">
         <v>0.1656</v>
       </c>
-      <c r="BF262" s="3">
-        <v>1.6918</v>
-      </c>
-    </row>
-    <row r="263" spans="2:58">
+    </row>
+    <row r="263" spans="2:57">
       <c r="B263" s="4">
         <v>2014.25</v>
       </c>
@@ -39039,8 +38582,8 @@
       <c r="AL263" s="10">
         <v>16556.617200000001</v>
       </c>
-      <c r="AM263" s="12">
-        <v>85</v>
+      <c r="AM263" s="3">
+        <v>1.5889</v>
       </c>
       <c r="AN263" s="3">
         <v>103</v>
@@ -39096,11 +38639,8 @@
       <c r="BE263" s="3">
         <v>0.18690000000000001</v>
       </c>
-      <c r="BF263" s="3">
-        <v>1.5889</v>
-      </c>
-    </row>
-    <row r="264" spans="2:58">
+    </row>
+    <row r="264" spans="2:57">
       <c r="B264" s="4">
         <v>2014.5</v>
       </c>
@@ -39188,8 +38728,8 @@
       <c r="AL264" s="10">
         <v>16588.095700000002</v>
       </c>
-      <c r="AM264" s="12">
-        <v>84</v>
+      <c r="AM264" s="3">
+        <v>1.6941999999999999</v>
       </c>
       <c r="AN264" s="3">
         <v>97</v>
@@ -39245,11 +38785,8 @@
       <c r="BE264" s="3">
         <v>0.1744</v>
       </c>
-      <c r="BF264" s="3">
-        <v>1.6941999999999999</v>
-      </c>
-    </row>
-    <row r="265" spans="2:58">
+    </row>
+    <row r="265" spans="2:57">
       <c r="B265" s="4">
         <v>2014.75</v>
       </c>
@@ -39337,8 +38874,8 @@
       <c r="AL265" s="10">
         <v>16735.5494</v>
       </c>
-      <c r="AM265" s="12">
-        <v>99</v>
+      <c r="AM265" s="3">
+        <v>1.9925999999999999</v>
       </c>
       <c r="AN265" s="3">
         <v>110</v>
@@ -39394,11 +38931,8 @@
       <c r="BE265" s="3">
         <v>0.16969999999999999</v>
       </c>
-      <c r="BF265" s="3">
-        <v>1.9925999999999999</v>
-      </c>
-    </row>
-    <row r="266" spans="2:58">
+    </row>
+    <row r="266" spans="2:57">
       <c r="B266" s="4">
         <v>2015</v>
       </c>
@@ -39486,8 +39020,8 @@
       <c r="AL266" s="10">
         <v>16894.113000000001</v>
       </c>
-      <c r="AM266" s="12">
-        <v>109</v>
+      <c r="AM266" s="3">
+        <v>2.0068999999999999</v>
       </c>
       <c r="AN266" s="3">
         <v>115</v>
@@ -39543,11 +39077,8 @@
       <c r="BE266" s="3">
         <v>0.1177</v>
       </c>
-      <c r="BF266" s="3">
-        <v>2.0068999999999999</v>
-      </c>
-    </row>
-    <row r="267" spans="2:58">
+    </row>
+    <row r="267" spans="2:57">
       <c r="B267" s="4">
         <v>2015.25</v>
       </c>
@@ -39635,8 +39166,8 @@
       <c r="AL267" s="10">
         <v>16872.451700000001</v>
       </c>
-      <c r="AM267" s="12">
-        <v>105</v>
+      <c r="AM267" s="3">
+        <v>2.0863999999999998</v>
       </c>
       <c r="AN267" s="3">
         <v>113</v>
@@ -39692,11 +39223,8 @@
       <c r="BE267" s="3">
         <v>0.17499999999999999</v>
       </c>
-      <c r="BF267" s="3">
-        <v>2.0863999999999998</v>
-      </c>
-    </row>
-    <row r="268" spans="2:58">
+    </row>
+    <row r="268" spans="2:57">
       <c r="B268" s="4">
         <v>2015.5</v>
       </c>
@@ -39784,8 +39312,8 @@
       <c r="AL268" s="10">
         <v>16843.275699999998</v>
       </c>
-      <c r="AM268" s="12">
-        <v>98</v>
+      <c r="AM268" s="3">
+        <v>2.3969999999999998</v>
       </c>
       <c r="AN268" s="3">
         <v>102</v>
@@ -39841,11 +39369,8 @@
       <c r="BE268" s="3">
         <v>0.121</v>
       </c>
-      <c r="BF268" s="3">
-        <v>2.3969999999999998</v>
-      </c>
-    </row>
-    <row r="269" spans="2:58">
+    </row>
+    <row r="269" spans="2:57">
       <c r="B269" s="4">
         <v>2015.75</v>
       </c>
@@ -39933,8 +39458,8 @@
       <c r="AL269" s="10">
         <v>16943.550200000001</v>
       </c>
-      <c r="AM269" s="12">
-        <v>104</v>
+      <c r="AM269" s="3">
+        <v>2.6116000000000001</v>
       </c>
       <c r="AN269" s="3">
         <v>102</v>
@@ -39990,11 +39515,8 @@
       <c r="BE269" s="3">
         <v>9.5200000000000007E-2</v>
       </c>
-      <c r="BF269" s="3">
-        <v>2.6116000000000001</v>
-      </c>
-    </row>
-    <row r="270" spans="2:58">
+    </row>
+    <row r="270" spans="2:57">
       <c r="B270" s="4">
         <v>2016</v>
       </c>
@@ -40082,8 +39604,8 @@
       <c r="AL270" s="10">
         <v>16928.802299999999</v>
       </c>
-      <c r="AM270" s="12">
-        <v>102</v>
+      <c r="AM270" s="3">
+        <v>2.6930000000000001</v>
       </c>
       <c r="AN270" s="3">
         <v>104</v>
@@ -40139,11 +39661,8 @@
       <c r="BE270" s="3">
         <v>0.13</v>
       </c>
-      <c r="BF270" s="3">
-        <v>2.6930000000000001</v>
-      </c>
-    </row>
-    <row r="271" spans="2:58">
+    </row>
+    <row r="271" spans="2:57">
       <c r="B271" s="4">
         <v>2016.25</v>
       </c>
@@ -40231,8 +39750,8 @@
       <c r="AL271" s="10">
         <v>16973.336599999999</v>
       </c>
-      <c r="AM271" s="12">
-        <v>101</v>
+      <c r="AM271" s="3">
+        <v>2.0855000000000001</v>
       </c>
       <c r="AN271" s="3">
         <v>102</v>
@@ -40288,11 +39807,8 @@
       <c r="BE271" s="3">
         <v>0.14080000000000001</v>
       </c>
-      <c r="BF271" s="3">
-        <v>2.0855000000000001</v>
-      </c>
-    </row>
-    <row r="272" spans="2:58">
+    </row>
+    <row r="272" spans="2:57">
       <c r="B272" s="4">
         <v>2016.5</v>
       </c>
@@ -40380,9 +39896,6 @@
       <c r="AL272" s="10">
         <v>17066.220099999999</v>
       </c>
-      <c r="AM272" s="12">
-        <v>98</v>
-      </c>
       <c r="AN272" s="3">
         <v>104</v>
       </c>
@@ -40526,9 +40039,6 @@
       <c r="AL273" s="10">
         <v>17176.599699999999</v>
       </c>
-      <c r="AM273" s="12">
-        <v>103</v>
-      </c>
       <c r="AN273" s="3">
         <v>110</v>
       </c>
@@ -40672,9 +40182,6 @@
       <c r="AL274" s="10">
         <v>17305.7156</v>
       </c>
-      <c r="AM274" s="12">
-        <v>109</v>
-      </c>
       <c r="AN274" s="3">
         <v>117</v>
       </c>
@@ -40818,9 +40325,6 @@
       <c r="AL275" s="10">
         <v>17398.7997</v>
       </c>
-      <c r="AM275" s="12">
-        <v>102</v>
-      </c>
       <c r="AN275" s="3">
         <v>114</v>
       </c>
@@ -40964,9 +40468,6 @@
       <c r="AL276" s="10">
         <v>17536.6898</v>
       </c>
-      <c r="AM276" s="3">
-        <v>95</v>
-      </c>
       <c r="AN276" s="3">
         <v>106</v>
       </c>
@@ -41107,9 +40608,6 @@
       <c r="AL277" s="10">
         <v>17684.021700000001</v>
       </c>
-      <c r="AM277" s="3">
-        <v>102</v>
-      </c>
       <c r="AN277" s="3">
         <v>111</v>
       </c>
@@ -41250,9 +40748,6 @@
       <c r="AL278" s="10">
         <v>17865.490399999999</v>
       </c>
-      <c r="AM278" s="3">
-        <v>102</v>
-      </c>
       <c r="AN278" s="3">
         <v>113</v>
       </c>
@@ -41386,9 +40881,6 @@
       </c>
       <c r="AL279" s="10">
         <v>17994.831900000001</v>
-      </c>
-      <c r="AM279" s="3">
-        <v>107</v>
       </c>
       <c r="AN279" s="3">
         <v>107</v>

</xml_diff>

<commit_message>
summarixed a paper di laura veldkamp
</commit_message>
<xml_diff>
--- a/Code/Data/Quarterly.xlsx
+++ b/Code/Data/Quarterly.xlsx
@@ -968,10 +968,10 @@
   <dimension ref="A1:BK937"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="AJ6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="AM138" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AL279" sqref="AL279"/>
+      <selection pane="bottomRight" activeCell="AT150" sqref="AT150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
adjusting an error in aggregating cash
</commit_message>
<xml_diff>
--- a/Code/Data/Quarterly.xlsx
+++ b/Code/Data/Quarterly.xlsx
@@ -1485,10 +1485,10 @@
   <dimension ref="A1:CG937"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="BG99" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="BB43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="BH117" sqref="BH117"/>
+      <selection pane="bottomRight" activeCell="BE59" sqref="BE59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -7873,13 +7873,13 @@
       </c>
       <c r="BC51" s="10"/>
       <c r="BD51" s="3">
-        <v>0.16032957997673</v>
+        <v>0.18395308305876101</v>
       </c>
       <c r="BE51" s="12">
-        <v>66.130305091841507</v>
+        <v>1.1350672458004101</v>
       </c>
       <c r="BF51" s="12">
-        <v>194.92119215686299</v>
+        <v>3.3456470588235301</v>
       </c>
       <c r="BJ51" s="10"/>
       <c r="BK51" s="10"/>
@@ -8047,13 +8047,13 @@
       </c>
       <c r="BC52" s="10"/>
       <c r="BD52" s="3">
-        <v>0.134193896120715</v>
+        <v>0.21431705424608599</v>
       </c>
       <c r="BE52" s="12">
-        <v>2.9888991194249801</v>
+        <v>2.4328999422451099</v>
       </c>
       <c r="BF52" s="12">
-        <v>1151.32122285175</v>
+        <v>461.71548914069899</v>
       </c>
       <c r="BJ52" s="10"/>
       <c r="BK52" s="10"/>
@@ -8221,13 +8221,13 @@
       </c>
       <c r="BC53" s="10"/>
       <c r="BD53" s="3">
-        <v>0.115565961516143</v>
+        <v>0.214676514203817</v>
       </c>
       <c r="BE53" s="12">
-        <v>1.5737911481126501</v>
+        <v>2.5031918857672402</v>
       </c>
       <c r="BF53" s="12">
-        <v>3694.3911680831002</v>
+        <v>2896.93538432483</v>
       </c>
       <c r="BJ53" s="10"/>
       <c r="BK53" s="10"/>
@@ -8397,13 +8397,13 @@
       </c>
       <c r="BC54" s="10"/>
       <c r="BD54" s="3">
-        <v>0.10097218987803</v>
+        <v>0.21058559949037201</v>
       </c>
       <c r="BE54" s="12">
-        <v>1.2522422226676899</v>
+        <v>2.4736095001870599</v>
       </c>
       <c r="BF54" s="12">
-        <v>6405.7554220000002</v>
+        <v>6406.7570040000001</v>
       </c>
       <c r="BJ54" s="10"/>
       <c r="BK54" s="10"/>
@@ -8573,13 +8573,13 @@
       </c>
       <c r="BC55" s="10"/>
       <c r="BD55" s="3">
-        <v>9.0838952087527999E-2</v>
+        <v>0.211247890874146</v>
       </c>
       <c r="BE55" s="12">
-        <v>1.08375741983241</v>
+        <v>2.4821098820077401</v>
       </c>
       <c r="BF55" s="12">
-        <v>8161.545196</v>
+        <v>10887.469755</v>
       </c>
       <c r="BJ55" s="10"/>
       <c r="BK55" s="10"/>
@@ -8749,13 +8749,13 @@
       </c>
       <c r="BC56" s="10"/>
       <c r="BD56" s="3">
-        <v>8.8177053113015005E-2</v>
+        <v>0.21685276532526601</v>
       </c>
       <c r="BE56" s="12">
-        <v>1.05645664061773</v>
+        <v>2.5520350779013601</v>
       </c>
       <c r="BF56" s="12">
-        <v>8679.7340550000008</v>
+        <v>14014.523961000001</v>
       </c>
       <c r="BJ56" s="10"/>
       <c r="BK56" s="10"/>
@@ -8925,13 +8925,13 @@
       </c>
       <c r="BC57" s="10"/>
       <c r="BD57" s="3">
-        <v>9.0163245138825995E-2</v>
+        <v>0.224402191455818</v>
       </c>
       <c r="BE57" s="12">
-        <v>1.1126183819394599</v>
+        <v>2.6644106528336899</v>
       </c>
       <c r="BF57" s="12">
-        <v>9017.8445250000004</v>
+        <v>15659.73115</v>
       </c>
       <c r="BJ57" s="10"/>
       <c r="BK57" s="10"/>
@@ -9101,13 +9101,13 @@
       </c>
       <c r="BC58" s="10"/>
       <c r="BD58" s="3">
-        <v>9.4265438635059998E-2</v>
+        <v>0.22652813597295099</v>
       </c>
       <c r="BE58" s="12">
-        <v>1.16218786910587</v>
+        <v>2.73425737450702</v>
       </c>
       <c r="BF58" s="12">
-        <v>9578.2388510000001</v>
+        <v>17066.471086000001</v>
       </c>
       <c r="BJ58" s="10"/>
       <c r="BK58" s="10"/>
@@ -9277,13 +9277,13 @@
       </c>
       <c r="BC59" s="10"/>
       <c r="BD59" s="3">
-        <v>9.3969534378454997E-2</v>
+        <v>0.22225501864844099</v>
       </c>
       <c r="BE59" s="12">
-        <v>1.16804670413914</v>
+        <v>2.7349513981878899</v>
       </c>
       <c r="BF59" s="12">
-        <v>9928.1467229999998</v>
+        <v>18237.540069999999</v>
       </c>
       <c r="BJ59" s="10"/>
       <c r="BK59" s="10"/>
@@ -9453,13 +9453,13 @@
       </c>
       <c r="BC60" s="10"/>
       <c r="BD60" s="3">
-        <v>9.5497745075803997E-2</v>
+        <v>0.22065819892628899</v>
       </c>
       <c r="BE60" s="12">
-        <v>1.1993092535238099</v>
+        <v>2.75342958910145</v>
       </c>
       <c r="BF60" s="12">
-        <v>10206.201419999999</v>
+        <v>19935.458175</v>
       </c>
       <c r="BJ60" s="10"/>
       <c r="BK60" s="10"/>
@@ -9629,13 +9629,13 @@
       </c>
       <c r="BC61" s="10"/>
       <c r="BD61" s="3">
-        <v>0.10040830097504901</v>
+        <v>0.22220106771381101</v>
       </c>
       <c r="BE61" s="12">
-        <v>1.2816918989427699</v>
+        <v>2.7979125569024701</v>
       </c>
       <c r="BF61" s="12">
-        <v>11316.279884</v>
+        <v>22527.119385999998</v>
       </c>
       <c r="BJ61" s="10"/>
       <c r="BK61" s="10"/>
@@ -9805,13 +9805,13 @@
       </c>
       <c r="BC62" s="10"/>
       <c r="BD62" s="3">
-        <v>0.107240480811264</v>
+        <v>0.220416672948541</v>
       </c>
       <c r="BE62" s="12">
-        <v>1.3605019263617</v>
+        <v>2.7893281221450201</v>
       </c>
       <c r="BF62" s="12">
-        <v>12148.334021000001</v>
+        <v>23605.118263</v>
       </c>
       <c r="BJ62" s="10"/>
       <c r="BK62" s="10"/>
@@ -9981,13 +9981,13 @@
       </c>
       <c r="BC63" s="10"/>
       <c r="BD63" s="3">
-        <v>0.109086987248376</v>
+        <v>0.21222366695985501</v>
       </c>
       <c r="BE63" s="12">
-        <v>1.3862068241931</v>
+        <v>2.7311931740625499</v>
       </c>
       <c r="BF63" s="12">
-        <v>12795.064544000001</v>
+        <v>23279.539059999999</v>
       </c>
       <c r="BJ63" s="10"/>
       <c r="BK63" s="10"/>
@@ -10157,13 +10157,13 @@
       </c>
       <c r="BC64" s="10"/>
       <c r="BD64" s="3">
-        <v>0.10992048903540701</v>
+        <v>0.202033375322796</v>
       </c>
       <c r="BE64" s="12">
-        <v>1.4073019362182</v>
+        <v>2.6712027361707502</v>
       </c>
       <c r="BF64" s="12">
-        <v>13050.950564999999</v>
+        <v>21961.637146000001</v>
       </c>
       <c r="BJ64" s="10"/>
       <c r="BK64" s="10"/>
@@ -10333,13 +10333,13 @@
       </c>
       <c r="BC65" s="10"/>
       <c r="BD65" s="3">
-        <v>0.108569635119353</v>
+        <v>0.19626530779151399</v>
       </c>
       <c r="BE65" s="12">
-        <v>1.42101409449759</v>
+        <v>2.6818381891679102</v>
       </c>
       <c r="BF65" s="12">
-        <v>13624.119966</v>
+        <v>21508.910209999998</v>
       </c>
       <c r="BJ65" s="10"/>
       <c r="BK65" s="10"/>
@@ -10509,13 +10509,13 @@
       </c>
       <c r="BC66" s="10"/>
       <c r="BD66" s="3">
-        <v>0.109429839383941</v>
+        <v>0.19685110918749599</v>
       </c>
       <c r="BE66" s="12">
-        <v>1.4475368623226501</v>
+        <v>2.7033116887371502</v>
       </c>
       <c r="BF66" s="12">
-        <v>14026.902797000001</v>
+        <v>21905.949237000001</v>
       </c>
       <c r="BJ66" s="10"/>
       <c r="BK66" s="10"/>
@@ -10685,13 +10685,13 @@
       </c>
       <c r="BC67" s="10"/>
       <c r="BD67" s="3">
-        <v>0.105939501956014</v>
+        <v>0.197763196556617</v>
       </c>
       <c r="BE67" s="12">
-        <v>1.4202431131492099</v>
+        <v>2.6831059210978498</v>
       </c>
       <c r="BF67" s="12">
-        <v>14002.196726</v>
+        <v>22068.659030999999</v>
       </c>
       <c r="BJ67" s="10"/>
       <c r="BK67" s="10"/>
@@ -10861,13 +10861,13 @@
       </c>
       <c r="BC68" s="10"/>
       <c r="BD68" s="3">
-        <v>0.10659847102208</v>
+        <v>0.19509113858910901</v>
       </c>
       <c r="BE68" s="12">
-        <v>1.4527486450376701</v>
+        <v>2.6985907240999198</v>
       </c>
       <c r="BF68" s="12">
-        <v>14633.148728</v>
+        <v>23842.575108000001</v>
       </c>
       <c r="BJ68" s="10"/>
       <c r="BK68" s="10"/>
@@ -11037,13 +11037,13 @@
       </c>
       <c r="BC69" s="10"/>
       <c r="BD69" s="3">
-        <v>0.11436198331777001</v>
+        <v>0.19054944596516701</v>
       </c>
       <c r="BE69" s="12">
-        <v>1.60002739482517</v>
+        <v>2.7564186094706198</v>
       </c>
       <c r="BF69" s="12">
-        <v>17465.215011</v>
+        <v>30081.989637999999</v>
       </c>
       <c r="BJ69" s="10"/>
       <c r="BK69" s="10"/>
@@ -11213,13 +11213,13 @@
       </c>
       <c r="BC70" s="10"/>
       <c r="BD70" s="3">
-        <v>0.12338824141526</v>
+        <v>0.188492269692042</v>
       </c>
       <c r="BE70" s="12">
-        <v>1.7399497258177601</v>
+        <v>2.8089363855383902</v>
       </c>
       <c r="BF70" s="12">
-        <v>20606.452324000002</v>
+        <v>38324.946337000001</v>
       </c>
       <c r="BJ70" s="10"/>
       <c r="BK70" s="10"/>
@@ -11389,13 +11389,13 @@
       </c>
       <c r="BC71" s="10"/>
       <c r="BD71" s="3">
-        <v>0.12771887128985199</v>
+        <v>0.19109408754649401</v>
       </c>
       <c r="BE71" s="12">
-        <v>1.75413346832168</v>
+        <v>2.8896050183827802</v>
       </c>
       <c r="BF71" s="12">
-        <v>22969.034446999998</v>
+        <v>45865.930613999997</v>
       </c>
       <c r="BJ71" s="10"/>
       <c r="BK71" s="10"/>
@@ -11565,13 +11565,13 @@
       </c>
       <c r="BC72" s="10"/>
       <c r="BD72" s="3">
-        <v>0.134476458410239</v>
+        <v>0.19522851825149201</v>
       </c>
       <c r="BE72" s="12">
-        <v>1.78759068781505</v>
+        <v>2.95964168849261</v>
       </c>
       <c r="BF72" s="12">
-        <v>24564.056002000001</v>
+        <v>49356.900307000004</v>
       </c>
       <c r="BJ72" s="10"/>
       <c r="BK72" s="10"/>
@@ -11741,13 +11741,13 @@
       </c>
       <c r="BC73" s="10"/>
       <c r="BD73" s="3">
-        <v>0.14961454480077399</v>
+        <v>0.19593241082207299</v>
       </c>
       <c r="BE73" s="12">
-        <v>1.99210147705425</v>
+        <v>2.9459099452771</v>
       </c>
       <c r="BF73" s="12">
-        <v>27954.516005000001</v>
+        <v>51154.233952000002</v>
       </c>
       <c r="BJ73" s="10"/>
       <c r="BK73" s="10"/>
@@ -11919,13 +11919,13 @@
       </c>
       <c r="BC74" s="15"/>
       <c r="BD74" s="3">
-        <v>0.169655646904941</v>
+        <v>0.19216739328146801</v>
       </c>
       <c r="BE74" s="12">
-        <v>2.32922229123692</v>
+        <v>2.8493347932026398</v>
       </c>
       <c r="BF74" s="12">
-        <v>32197.633185999999</v>
+        <v>54468.192789000001</v>
       </c>
       <c r="BJ74" s="10"/>
       <c r="BK74" s="10"/>
@@ -12097,13 +12097,13 @@
       </c>
       <c r="BC75" s="15"/>
       <c r="BD75" s="3">
-        <v>0.18564299779198501</v>
+        <v>0.19113420284204</v>
       </c>
       <c r="BE75" s="12">
-        <v>2.5317573910081199</v>
+        <v>2.8278149719922898</v>
       </c>
       <c r="BF75" s="12">
-        <v>36756.836259999996</v>
+        <v>60875.546679999999</v>
       </c>
       <c r="BJ75" s="10"/>
       <c r="BK75" s="10"/>
@@ -12275,13 +12275,13 @@
       </c>
       <c r="BC76" s="15"/>
       <c r="BD76" s="3">
-        <v>0.19351326184517001</v>
+        <v>0.194304464164962</v>
       </c>
       <c r="BE76" s="12">
-        <v>2.5510139399859399</v>
+        <v>2.9135684452680501</v>
       </c>
       <c r="BF76" s="12">
-        <v>39780.309372999996</v>
+        <v>67701.801149000006</v>
       </c>
       <c r="BJ76" s="10"/>
       <c r="BK76" s="10"/>
@@ -12453,13 +12453,13 @@
       </c>
       <c r="BC77" s="15"/>
       <c r="BD77" s="3">
-        <v>0.196930368944814</v>
+        <v>0.198084276937917</v>
       </c>
       <c r="BE77" s="12">
-        <v>2.59322717744607</v>
+        <v>3.0208377988512098</v>
       </c>
       <c r="BF77" s="12">
-        <v>42077.073275000002</v>
+        <v>72243.360237999994</v>
       </c>
       <c r="BJ77" s="10"/>
       <c r="BK77" s="10"/>
@@ -12647,13 +12647,13 @@
       </c>
       <c r="BC78" s="15"/>
       <c r="BD78" s="3">
-        <v>0.201104691276107</v>
+        <v>0.19961358822905301</v>
       </c>
       <c r="BE78" s="12">
-        <v>2.9998665594048202</v>
+        <v>3.06136993392552</v>
       </c>
       <c r="BF78" s="12">
-        <v>44029.589678999997</v>
+        <v>74788.344693999999</v>
       </c>
       <c r="BJ78" s="10"/>
       <c r="BK78" s="10"/>
@@ -12841,13 +12841,13 @@
       </c>
       <c r="BC79" s="15"/>
       <c r="BD79" s="3">
-        <v>0.203186973702043</v>
+        <v>0.19994983642300099</v>
       </c>
       <c r="BE79" s="12">
-        <v>2.5457969511816501</v>
+        <v>3.0917145272156699</v>
       </c>
       <c r="BF79" s="12">
-        <v>46561.779836000002</v>
+        <v>79810.865441999995</v>
       </c>
       <c r="BJ79" s="10"/>
       <c r="BK79" s="10"/>
@@ -13035,13 +13035,13 @@
       </c>
       <c r="BC80" s="15"/>
       <c r="BD80" s="3">
-        <v>0.20210479354375799</v>
+        <v>0.199136719424099</v>
       </c>
       <c r="BE80" s="12">
-        <v>1.9441953837433199</v>
+        <v>3.1299940073067098</v>
       </c>
       <c r="BF80" s="12">
-        <v>48728.648090000002</v>
+        <v>85916.428727000006</v>
       </c>
       <c r="BJ80" s="10"/>
       <c r="BK80" s="10"/>
@@ -13231,13 +13231,13 @@
       </c>
       <c r="BC81" s="15"/>
       <c r="BD81" s="3">
-        <v>0.20290218625787801</v>
+        <v>0.19790500557698401</v>
       </c>
       <c r="BE81" s="12">
-        <v>1.7124599510754701</v>
+        <v>3.1728909380363102</v>
       </c>
       <c r="BF81" s="12">
-        <v>51651.455464999999</v>
+        <v>90710.357766000001</v>
       </c>
       <c r="BJ81" s="10"/>
       <c r="BK81" s="10"/>
@@ -13452,13 +13452,13 @@
       </c>
       <c r="BC82" s="15"/>
       <c r="BD82" s="3">
-        <v>0.20639905022382901</v>
+        <v>0.19826153991477499</v>
       </c>
       <c r="BE82" s="12">
-        <v>2.9742643904089401</v>
+        <v>3.2234935565117402</v>
       </c>
       <c r="BF82" s="12">
-        <v>53738.598953000001</v>
+        <v>95392.355555999995</v>
       </c>
       <c r="BJ82" s="10"/>
       <c r="BK82" s="10"/>
@@ -13673,13 +13673,13 @@
       </c>
       <c r="BC83" s="15"/>
       <c r="BD83" s="3">
-        <v>0.21235020802788501</v>
+        <v>0.20207354153700099</v>
       </c>
       <c r="BE83" s="12">
-        <v>1.21266206148936</v>
+        <v>3.3067687913250401</v>
       </c>
       <c r="BF83" s="12">
-        <v>56563.884555999997</v>
+        <v>101781.89273399999</v>
       </c>
       <c r="BJ83" s="10"/>
       <c r="BK83" s="10"/>
@@ -13894,13 +13894,13 @@
       </c>
       <c r="BC84" s="15"/>
       <c r="BD84" s="3">
-        <v>0.21934888301598199</v>
+        <v>0.209675761304668</v>
       </c>
       <c r="BE84" s="12">
-        <v>0.58918622671420395</v>
+        <v>3.44438287088265</v>
       </c>
       <c r="BF84" s="12">
-        <v>60306.887798999996</v>
+        <v>108910.595671</v>
       </c>
       <c r="BJ84" s="10"/>
       <c r="BK84" s="10"/>
@@ -14114,13 +14114,13 @@
       </c>
       <c r="BC85" s="15"/>
       <c r="BD85" s="3">
-        <v>0.224405232336539</v>
+        <v>0.218199312822905</v>
       </c>
       <c r="BE85" s="12">
-        <v>0.48441290156333</v>
+        <v>3.5807839518354201</v>
       </c>
       <c r="BF85" s="12">
-        <v>64588.255320999997</v>
+        <v>114202.32832299999</v>
       </c>
       <c r="BJ85" s="10"/>
       <c r="BK85" s="10"/>
@@ -14335,13 +14335,13 @@
       </c>
       <c r="BC86" s="15"/>
       <c r="BD86" s="3">
-        <v>0.23178053591287601</v>
+        <v>0.224891045022825</v>
       </c>
       <c r="BE86" s="12">
-        <v>0.71462038225532099</v>
+        <v>3.6833538127252199</v>
       </c>
       <c r="BF86" s="12">
-        <v>67746.785942999995</v>
+        <v>119861.69362400001</v>
       </c>
       <c r="BJ86" s="10"/>
       <c r="BK86" s="10"/>
@@ -14555,13 +14555,13 @@
       </c>
       <c r="BC87" s="15"/>
       <c r="BD87" s="3">
-        <v>0.22487302211140101</v>
+        <v>0.22838661915453101</v>
       </c>
       <c r="BE87" s="12">
-        <v>0.90466200865110802</v>
+        <v>3.7724849757482799</v>
       </c>
       <c r="BF87" s="12">
-        <v>70188.954505999995</v>
+        <v>127605.8217</v>
       </c>
       <c r="BJ87" s="10"/>
       <c r="BK87" s="10"/>
@@ -14783,13 +14783,13 @@
       </c>
       <c r="BC88" s="15"/>
       <c r="BD88" s="3">
-        <v>0.20905991619912601</v>
+        <v>0.22848069886821301</v>
       </c>
       <c r="BE88" s="12">
-        <v>0.56086625451513705</v>
+        <v>3.9222347988955599</v>
       </c>
       <c r="BF88" s="12">
-        <v>72095.313829000006</v>
+        <v>133362.447782</v>
       </c>
       <c r="BJ88" s="10"/>
       <c r="BK88" s="10"/>
@@ -15011,13 +15011,13 @@
       </c>
       <c r="BC89" s="15"/>
       <c r="BD89" s="3">
-        <v>0.19563797934706401</v>
+        <v>0.228123380777429</v>
       </c>
       <c r="BE89" s="12">
-        <v>0.37176935211166201</v>
+        <v>3.9753448788877201</v>
       </c>
       <c r="BF89" s="12">
-        <v>76129.857784000007</v>
+        <v>134289.669165</v>
       </c>
       <c r="BJ89" s="10"/>
       <c r="BK89" s="10"/>
@@ -15239,13 +15239,13 @@
       </c>
       <c r="BC90" s="15"/>
       <c r="BD90" s="3">
-        <v>0.19964867565307301</v>
+        <v>0.23825450175270901</v>
       </c>
       <c r="BE90" s="12">
-        <v>0.39101396876626598</v>
+        <v>5.8642664394608497</v>
       </c>
       <c r="BF90" s="12">
-        <v>79726.353902999996</v>
+        <v>136426.999438</v>
       </c>
       <c r="BJ90" s="10"/>
       <c r="BK90" s="10"/>
@@ -15467,13 +15467,13 @@
       </c>
       <c r="BC91" s="15"/>
       <c r="BD91" s="3">
-        <v>0.17544923993405401</v>
+        <v>0.222701338549218</v>
       </c>
       <c r="BE91" s="12">
-        <v>0.46796428102858201</v>
+        <v>2.4828640864920701</v>
       </c>
       <c r="BF91" s="12">
-        <v>91528.095899999898</v>
+        <v>145299.82114499999</v>
       </c>
       <c r="BJ91" s="10"/>
       <c r="BK91" s="10"/>
@@ -15695,13 +15695,13 @@
       </c>
       <c r="BC92" s="15"/>
       <c r="BD92" s="3">
-        <v>0.14691079134858401</v>
+        <v>0.18748705416641701</v>
       </c>
       <c r="BE92" s="12">
-        <v>0.42461838877411401</v>
+        <v>1.06621762555745</v>
       </c>
       <c r="BF92" s="12">
-        <v>103599.56255800001</v>
+        <v>155594.71455899999</v>
       </c>
       <c r="BJ92" s="10"/>
       <c r="BK92" s="10"/>
@@ -15923,13 +15923,13 @@
       </c>
       <c r="BC93" s="15"/>
       <c r="BD93" s="3">
-        <v>0.13437455606952001</v>
+        <v>0.16380273321433</v>
       </c>
       <c r="BE93" s="12">
-        <v>0.31547267990528999</v>
+        <v>0.72338360354564601</v>
       </c>
       <c r="BF93" s="12">
-        <v>107637.98129</v>
+        <v>158044.96051199999</v>
       </c>
       <c r="BJ93" s="10"/>
       <c r="BK93" s="10"/>
@@ -16151,13 +16151,13 @@
       </c>
       <c r="BC94" s="15"/>
       <c r="BD94" s="3">
-        <v>0.144845706952345</v>
+        <v>0.16549832707328199</v>
       </c>
       <c r="BE94" s="3">
-        <v>0.25626121554180398</v>
+        <v>0.77147877908300599</v>
       </c>
       <c r="BF94" s="3">
-        <v>100176.740091</v>
+        <v>154104.80900800001</v>
       </c>
       <c r="BJ94" s="10"/>
       <c r="BK94" s="10"/>
@@ -16379,13 +16379,13 @@
       </c>
       <c r="BC95" s="15"/>
       <c r="BD95" s="3">
-        <v>0.15734428635838199</v>
+        <v>0.17847906905460001</v>
       </c>
       <c r="BE95" s="3">
-        <v>0.25356187763398103</v>
+        <v>0.978559643183049</v>
       </c>
       <c r="BF95" s="3">
-        <v>102385.10507000001</v>
+        <v>157901.31834200001</v>
       </c>
       <c r="BJ95" s="10"/>
       <c r="BK95" s="10"/>
@@ -16607,13 +16607,13 @@
       </c>
       <c r="BC96" s="15"/>
       <c r="BD96" s="3">
-        <v>0.153743480736414</v>
+        <v>0.181073564949289</v>
       </c>
       <c r="BE96" s="3">
-        <v>0.28796908845514002</v>
+        <v>0.97348522498830103</v>
       </c>
       <c r="BF96" s="3">
-        <v>119259.877028</v>
+        <v>181605.31529200001</v>
       </c>
       <c r="BJ96" s="10"/>
       <c r="BK96" s="10"/>
@@ -16835,13 +16835,13 @@
       </c>
       <c r="BC97" s="15"/>
       <c r="BD97" s="3">
-        <v>0.14610373089856099</v>
+        <v>0.175168991036662</v>
       </c>
       <c r="BE97" s="3">
-        <v>0.305496536627062</v>
+        <v>0.84647142690989996</v>
       </c>
       <c r="BF97" s="3">
-        <v>135539.31767600001</v>
+        <v>215392.73313800001</v>
       </c>
       <c r="BJ97" s="10"/>
       <c r="BK97" s="10"/>
@@ -17065,13 +17065,13 @@
         <v>-6.1175000000000007E-2</v>
       </c>
       <c r="BD98" s="3">
-        <v>0.15728655276043699</v>
+        <v>0.18399356255579299</v>
       </c>
       <c r="BE98" s="3">
-        <v>0.28162311297524101</v>
+        <v>0.99543742173133998</v>
       </c>
       <c r="BF98" s="3">
-        <v>130059.53139400001</v>
+        <v>237232.76045500001</v>
       </c>
       <c r="BG98" s="3">
         <v>1.026</v>
@@ -17298,13 +17298,13 @@
         <v>-0.1303</v>
       </c>
       <c r="BD99" s="3">
-        <v>0.16577010577126</v>
+        <v>0.19358471872635599</v>
       </c>
       <c r="BE99" s="3">
-        <v>0.276553043636516</v>
+        <v>1.22066941562113</v>
       </c>
       <c r="BF99" s="3">
-        <v>132346.682118</v>
+        <v>246025.60365199999</v>
       </c>
       <c r="BG99" s="3">
         <v>1.0113000000000001</v>
@@ -17531,13 +17531,13 @@
         <v>-0.19322500000000001</v>
       </c>
       <c r="BD100" s="3">
-        <v>0.15815140810877201</v>
+        <v>0.18960394688801299</v>
       </c>
       <c r="BE100" s="3">
-        <v>0.30042617316040299</v>
+        <v>1.1100212108274099</v>
       </c>
       <c r="BF100" s="3">
-        <v>149935.13651899999</v>
+        <v>248832.60437399999</v>
       </c>
       <c r="BG100" s="3">
         <v>0.97560000000000002</v>
@@ -17764,13 +17764,13 @@
         <v>2.0800000000000003E-2</v>
       </c>
       <c r="BD101" s="3">
-        <v>0.15304436293265</v>
+        <v>0.180474194655494</v>
       </c>
       <c r="BE101" s="3">
-        <v>0.32990879077447599</v>
+        <v>0.896280892947519</v>
       </c>
       <c r="BF101" s="3">
-        <v>171688.17733800001</v>
+        <v>254946.35239399999</v>
       </c>
       <c r="BG101" s="3">
         <v>1.2197</v>
@@ -17997,13 +17997,13 @@
         <v>-9.2499999999999701E-4</v>
       </c>
       <c r="BD102" s="3">
-        <v>0.16877901328775699</v>
+        <v>0.19085365996436299</v>
       </c>
       <c r="BE102" s="3">
-        <v>0.32252055232586202</v>
+        <v>1.0378989329034001</v>
       </c>
       <c r="BF102" s="3">
-        <v>170013.72888000001</v>
+        <v>260675.82152900001</v>
       </c>
       <c r="BG102" s="3">
         <v>1.1686000000000001</v>
@@ -18230,13 +18230,13 @@
         <v>0.44482499999999997</v>
       </c>
       <c r="BD103" s="3">
-        <v>0.17856703778911501</v>
+        <v>0.20394014386424</v>
       </c>
       <c r="BE103" s="3">
-        <v>0.31067075639800601</v>
+        <v>1.38835540597116</v>
       </c>
       <c r="BF103" s="3">
-        <v>165858.997703</v>
+        <v>266825.44107499998</v>
       </c>
       <c r="BG103" s="3">
         <v>1.6315</v>
@@ -18464,13 +18464,13 @@
         <v>0.83892500000000003</v>
       </c>
       <c r="BD104" s="3">
-        <v>0.153392018208275</v>
+        <v>0.18839191267326499</v>
       </c>
       <c r="BE104" s="3">
-        <v>0.31676623764374201</v>
+        <v>1.1702789470216599</v>
       </c>
       <c r="BF104" s="3">
-        <v>173988.77579099999</v>
+        <v>272777.59204000002</v>
       </c>
       <c r="BG104" s="3">
         <v>2.1772</v>
@@ -18697,13 +18697,13 @@
         <v>0.7399</v>
       </c>
       <c r="BD105" s="3">
-        <v>0.124453650527158</v>
+        <v>0.15687543677497701</v>
       </c>
       <c r="BE105" s="3">
-        <v>0.33875147175141601</v>
+        <v>0.72777562559151499</v>
       </c>
       <c r="BF105" s="3">
-        <v>191917.47080800001</v>
+        <v>277215.59786400001</v>
       </c>
       <c r="BG105" s="3">
         <v>2.1158999999999999</v>
@@ -18930,13 +18930,13 @@
         <v>0.34040000000000004</v>
       </c>
       <c r="BD106" s="3">
-        <v>0.111240753358216</v>
+        <v>0.13957029244587299</v>
       </c>
       <c r="BE106" s="3">
-        <v>0.34343707032229798</v>
+        <v>0.56287280603171497</v>
       </c>
       <c r="BF106" s="3">
-        <v>195941.16817200001</v>
+        <v>279686.73942200001</v>
       </c>
       <c r="BG106" s="3">
         <v>1.5933999999999999</v>
@@ -19163,13 +19163,13 @@
         <v>0.249975</v>
       </c>
       <c r="BD107" s="3">
-        <v>0.108376174732987</v>
+        <v>0.136502169078354</v>
       </c>
       <c r="BE107" s="3">
-        <v>0.34452778152562102</v>
+        <v>0.52784529536886604</v>
       </c>
       <c r="BF107" s="3">
-        <v>199461.298962</v>
+        <v>285122.78755000001</v>
       </c>
       <c r="BG107" s="3">
         <v>1.4368000000000001</v>
@@ -19396,13 +19396,13 @@
         <v>0.213725</v>
       </c>
       <c r="BD108" s="3">
-        <v>0.10974023803825</v>
+        <v>0.13889420851436099</v>
       </c>
       <c r="BE108" s="3">
-        <v>0.354752272471407</v>
+        <v>0.52803870991618795</v>
       </c>
       <c r="BF108" s="3">
-        <v>210936.96853099999</v>
+        <v>289986.84016800002</v>
       </c>
       <c r="BG108" s="3">
         <v>1.3525</v>
@@ -19629,13 +19629,13 @@
         <v>-4.9750000000000003E-3</v>
       </c>
       <c r="BD109" s="3">
-        <v>0.1098987214824</v>
+        <v>0.13837206753720399</v>
       </c>
       <c r="BE109" s="3">
-        <v>0.37748801829532602</v>
+        <v>0.50798326737312305</v>
       </c>
       <c r="BF109" s="3">
-        <v>229825.462302</v>
+        <v>289758.43168500002</v>
       </c>
       <c r="BG109" s="3">
         <v>1.1652</v>
@@ -19862,13 +19862,13 @@
         <v>-8.7049999999999988E-2</v>
       </c>
       <c r="BD110" s="3">
-        <v>0.10833218633861</v>
+        <v>0.13560704452264999</v>
       </c>
       <c r="BE110" s="3">
-        <v>0.39132803677058903</v>
+        <v>0.48470937223272498</v>
       </c>
       <c r="BF110" s="3">
-        <v>237793.80991499999</v>
+        <v>278124.18306000001</v>
       </c>
       <c r="BG110" s="3">
         <v>1.0137</v>
@@ -20095,13 +20095,13 @@
         <v>-7.4124999999999996E-2</v>
       </c>
       <c r="BD111" s="3">
-        <v>0.107698836669813</v>
+        <v>0.13421165875969901</v>
       </c>
       <c r="BE111" s="3">
-        <v>0.39458778102885</v>
+        <v>0.47204809840214701</v>
       </c>
       <c r="BF111" s="3">
-        <v>243005.42312200001</v>
+        <v>270245.75417899998</v>
       </c>
       <c r="BG111" s="3">
         <v>0.99609999999999999</v>
@@ -20328,13 +20328,13 @@
         <v>-0.13437499999999999</v>
       </c>
       <c r="BD112" s="3">
-        <v>0.108671845817465</v>
+        <v>0.13176377263712299</v>
       </c>
       <c r="BE112" s="3">
-        <v>0.391679367401498</v>
+        <v>0.45762813629803201</v>
       </c>
       <c r="BF112" s="3">
-        <v>252291.192668</v>
+        <v>272648.61108</v>
       </c>
       <c r="BG112" s="3">
         <v>0.89380000000000004</v>
@@ -20561,13 +20561,13 @@
         <v>-0.19112499999999999</v>
       </c>
       <c r="BD113" s="3">
-        <v>0.110469437882341</v>
+        <v>0.126927924018883</v>
       </c>
       <c r="BE113" s="3">
-        <v>0.394439474929969</v>
+        <v>0.43844670291879001</v>
       </c>
       <c r="BF113" s="3">
-        <v>267490.18715999997</v>
+        <v>279468.70235899999</v>
       </c>
       <c r="BG113" s="3">
         <v>0.95240000000000002</v>
@@ -20794,13 +20794,13 @@
         <v>-0.214475</v>
       </c>
       <c r="BD114" s="3">
-        <v>0.110525551398639</v>
+        <v>0.12131145566312899</v>
       </c>
       <c r="BE114" s="3">
-        <v>0.39992797611277497</v>
+        <v>0.42287207150232597</v>
       </c>
       <c r="BF114" s="3">
-        <v>276493.12016799999</v>
+        <v>283770.24865700002</v>
       </c>
       <c r="BG114" s="3">
         <v>0.90690000000000004</v>
@@ -21027,13 +21027,13 @@
         <v>-0.20880000000000001</v>
       </c>
       <c r="BD115" s="3">
-        <v>0.109990512447944</v>
+        <v>0.117486412141215</v>
       </c>
       <c r="BE115" s="3">
-        <v>0.40229704348744799</v>
+        <v>0.41407832381601001</v>
       </c>
       <c r="BF115" s="3">
-        <v>283744.87874100002</v>
+        <v>287814.903406</v>
       </c>
       <c r="BG115" s="3">
         <v>0.84830000000000005</v>
@@ -21260,13 +21260,13 @@
         <v>-0.14255000000000001</v>
       </c>
       <c r="BD116" s="3">
-        <v>0.11052398255283299</v>
+        <v>0.11729020461293101</v>
       </c>
       <c r="BE116" s="3">
-        <v>0.40458508200450499</v>
+        <v>0.41741822679584201</v>
       </c>
       <c r="BF116" s="3">
-        <v>294722.40779500001</v>
+        <v>298882.85821600002</v>
       </c>
       <c r="BG116" s="3">
         <v>0.96399999999999997</v>
@@ -21493,13 +21493,13 @@
         <v>-0.24445</v>
       </c>
       <c r="BD117" s="3">
-        <v>0.112772461378488</v>
+        <v>0.120071935792574</v>
       </c>
       <c r="BE117" s="3">
-        <v>0.41293081350142402</v>
+        <v>0.43220797890319002</v>
       </c>
       <c r="BF117" s="3">
-        <v>311065.97813900001</v>
+        <v>318264.95408199902</v>
       </c>
       <c r="BG117" s="3">
         <v>0.88529999999999998</v>
@@ -21727,13 +21727,13 @@
         <v>-0.35142500000000004</v>
       </c>
       <c r="BD118" s="3">
-        <v>0.113211548714078</v>
+        <v>0.120937348838443</v>
       </c>
       <c r="BE118" s="3">
-        <v>0.42125921300791203</v>
+        <v>0.44070936026665403</v>
       </c>
       <c r="BF118" s="3">
-        <v>320213.18320899899</v>
+        <v>329827.82807099901</v>
       </c>
       <c r="BG118" s="3">
         <v>0.74839999999999995</v>
@@ -21963,13 +21963,13 @@
         <v>-0.35807500000000003</v>
       </c>
       <c r="BD119" s="3">
-        <v>0.112228146616504</v>
+        <v>0.120155005060994</v>
       </c>
       <c r="BE119" s="3">
-        <v>0.42247296280958002</v>
+        <v>0.44045168898072601</v>
       </c>
       <c r="BF119" s="3">
-        <v>326827.28383099998</v>
+        <v>337842.56680500001</v>
       </c>
       <c r="BG119" s="3">
         <v>0.69720000000000004</v>
@@ -22199,13 +22199,13 @@
         <v>-0.41002500000000003</v>
       </c>
       <c r="BD120" s="3">
-        <v>0.111526786969188</v>
+        <v>0.119281548617363</v>
       </c>
       <c r="BE120" s="3">
-        <v>0.41896653649468202</v>
+        <v>0.43678677510234498</v>
       </c>
       <c r="BF120" s="3">
-        <v>336955.91786699998</v>
+        <v>349170.77591199998</v>
       </c>
       <c r="BG120" s="3">
         <v>0.61029999999999995</v>
@@ -22435,13 +22435,13 @@
         <v>-0.39570000000000005</v>
       </c>
       <c r="BD121" s="3">
-        <v>0.112339716848848</v>
+        <v>0.120008517187491</v>
       </c>
       <c r="BE121" s="3">
-        <v>0.419816604072828</v>
+        <v>0.43974075280974501</v>
       </c>
       <c r="BF121" s="3">
-        <v>351993.59345300001</v>
+        <v>364656.33336500003</v>
       </c>
       <c r="BG121" s="3">
         <v>0.63759999999999994</v>
@@ -22671,13 +22671,13 @@
         <v>-0.27247499999999997</v>
       </c>
       <c r="BD122" s="3">
-        <v>0.11344490231458799</v>
+        <v>0.12159185717446901</v>
       </c>
       <c r="BE122" s="3">
-        <v>0.42944137766544899</v>
+        <v>0.45097600168323898</v>
       </c>
       <c r="BF122" s="3">
-        <v>364709.21085500001</v>
+        <v>377378.47096599999</v>
       </c>
       <c r="BG122" s="3">
         <v>0.66539999999999999</v>
@@ -22907,13 +22907,13 @@
         <v>-0.25080000000000002</v>
       </c>
       <c r="BD123" s="3">
-        <v>0.113122476918026</v>
+        <v>0.120975013521594</v>
       </c>
       <c r="BE123" s="3">
-        <v>0.43326866733564101</v>
+        <v>0.45408997581057797</v>
       </c>
       <c r="BF123" s="3">
-        <v>376526.35007399903</v>
+        <v>387265.42195899901</v>
       </c>
       <c r="BG123" s="3">
         <v>0.69</v>
@@ -23143,13 +23143,13 @@
         <v>-0.40362499999999996</v>
       </c>
       <c r="BD124" s="3">
-        <v>0.111015560894342</v>
+        <v>0.118059053279676</v>
       </c>
       <c r="BE124" s="3">
-        <v>0.42621934630059899</v>
+        <v>0.44599421558664398</v>
       </c>
       <c r="BF124" s="3">
-        <v>385842.07025099901</v>
+        <v>396601.65957499901</v>
       </c>
       <c r="BG124" s="3">
         <v>0.65900000000000003</v>
@@ -23379,13 +23379,13 @@
         <v>-0.24897499999999997</v>
       </c>
       <c r="BD125" s="3">
-        <v>0.10926164970783001</v>
+        <v>0.115959492371777</v>
       </c>
       <c r="BE125" s="3">
-        <v>0.41959523469816001</v>
+        <v>0.44017810886301101</v>
       </c>
       <c r="BF125" s="3">
-        <v>393826.64285699901</v>
+        <v>406641.391165999</v>
       </c>
       <c r="BG125" s="3">
         <v>0.77180000000000004</v>
@@ -23615,13 +23615,13 @@
         <v>-0.2445</v>
       </c>
       <c r="BD126" s="3">
-        <v>0.107959548216346</v>
+        <v>0.115344517316773</v>
       </c>
       <c r="BE126" s="3">
-        <v>0.41985561579880498</v>
+        <v>0.44017242405594298</v>
       </c>
       <c r="BF126" s="3">
-        <v>394857.39814100001</v>
+        <v>409772.73260400002</v>
       </c>
       <c r="BG126" s="3">
         <v>0.92379999999999995</v>
@@ -23851,13 +23851,13 @@
         <v>-0.18429999999999996</v>
       </c>
       <c r="BD127" s="3">
-        <v>0.10694164813798999</v>
+        <v>0.114478402728767</v>
       </c>
       <c r="BE127" s="3">
-        <v>0.41797066565456198</v>
+        <v>0.436133293219024</v>
       </c>
       <c r="BF127" s="3">
-        <v>399343.04122700001</v>
+        <v>408843.91354600003</v>
       </c>
       <c r="BG127" s="3">
         <v>0.93500000000000005</v>
@@ -24087,13 +24087,13 @@
         <v>-7.8300000000000008E-2</v>
       </c>
       <c r="BD128" s="3">
-        <v>0.105829768669653</v>
+        <v>0.11358443197394399</v>
       </c>
       <c r="BE128" s="3">
-        <v>0.40955356175851398</v>
+        <v>0.43314550748632202</v>
       </c>
       <c r="BF128" s="3">
-        <v>412189.93431899999</v>
+        <v>432400.53721400001</v>
       </c>
       <c r="BG128" s="3">
         <v>0.8629</v>
@@ -24323,13 +24323,13 @@
         <v>9.3750000000000014E-2</v>
       </c>
       <c r="BD129" s="3">
-        <v>0.104772153143371</v>
+        <v>0.112343659928306</v>
       </c>
       <c r="BE129" s="3">
-        <v>0.40122962820854902</v>
+        <v>0.43306847195491199</v>
       </c>
       <c r="BF129" s="3">
-        <v>427658.57303099998</v>
+        <v>487395.12177099998</v>
       </c>
       <c r="BG129" s="3">
         <v>0.98980000000000001</v>
@@ -24559,13 +24559,13 @@
         <v>0.22002499999999997</v>
       </c>
       <c r="BD130" s="3">
-        <v>0.104044294173496</v>
+        <v>0.11229246756839301</v>
       </c>
       <c r="BE130" s="3">
-        <v>0.40238398113603002</v>
+        <v>0.44132950050429198</v>
       </c>
       <c r="BF130" s="3">
-        <v>432015.24177800003</v>
+        <v>554451.86956799997</v>
       </c>
       <c r="BG130" s="3">
         <v>0.96340000000000003</v>
@@ -24795,13 +24795,13 @@
         <v>0.41004999999999997</v>
       </c>
       <c r="BD131" s="3">
-        <v>0.102199904922189</v>
+        <v>0.110552919601796</v>
       </c>
       <c r="BE131" s="3">
-        <v>0.400000637245298</v>
+        <v>0.43537919152896198</v>
       </c>
       <c r="BF131" s="3">
-        <v>436754.45563699998</v>
+        <v>596600.89863500104</v>
       </c>
       <c r="BG131" s="3">
         <v>1.1214999999999999</v>
@@ -25031,13 +25031,13 @@
         <v>0.40697499999999998</v>
       </c>
       <c r="BD132" s="3">
-        <v>9.7541452685181995E-2</v>
+        <v>0.105691496443963</v>
       </c>
       <c r="BE132" s="3">
-        <v>0.381808262197677</v>
+        <v>0.410589171874857</v>
       </c>
       <c r="BF132" s="3">
-        <v>445404.41354799899</v>
+        <v>599295.38989300095</v>
       </c>
       <c r="BG132" s="3">
         <v>1.1418999999999999</v>
@@ -25267,13 +25267,13 @@
         <v>0.55515000000000003</v>
       </c>
       <c r="BD133" s="3">
-        <v>9.1867858468742E-2</v>
+        <v>0.10012167146045101</v>
       </c>
       <c r="BE133" s="3">
-        <v>0.35696394259852898</v>
+        <v>0.384402539649708</v>
       </c>
       <c r="BF133" s="3">
-        <v>452814.92828199902</v>
+        <v>579323.12285400101</v>
       </c>
       <c r="BG133" s="3">
         <v>1.4448000000000001</v>
@@ -25503,13 +25503,13 @@
         <v>0.77115</v>
       </c>
       <c r="BD134" s="3">
-        <v>8.6812205492627997E-2</v>
+        <v>9.61926048953715E-2</v>
       </c>
       <c r="BE134" s="3">
-        <v>0.33784489435479798</v>
+        <v>0.36836914907128798</v>
       </c>
       <c r="BF134" s="3">
-        <v>444973.96526499902</v>
+        <v>554166.88142600004</v>
       </c>
       <c r="BG134" s="3">
         <v>1.5509999999999999</v>
@@ -25739,13 +25739,13 @@
         <v>0.74307499999999993</v>
       </c>
       <c r="BD135" s="3">
-        <v>8.5776670972133998E-2</v>
+        <v>9.4628113639360495E-2</v>
       </c>
       <c r="BE135" s="3">
-        <v>0.337008921355331</v>
+        <v>0.36457571558924201</v>
       </c>
       <c r="BF135" s="3">
-        <v>448925.314931</v>
+        <v>539062.61877700104</v>
       </c>
       <c r="BG135" s="3">
         <v>1.5548999999999999</v>
@@ -25975,13 +25975,13 @@
         <v>0.36220000000000002</v>
       </c>
       <c r="BD136" s="3">
-        <v>8.8185292030966006E-2</v>
+        <v>9.5802855610275794E-2</v>
       </c>
       <c r="BE136" s="3">
-        <v>0.34955643711067602</v>
+        <v>0.37245064232967401</v>
       </c>
       <c r="BF136" s="3">
-        <v>475401.90082600003</v>
+        <v>548182.92000800103</v>
       </c>
       <c r="BG136" s="3">
         <v>1.6774</v>
@@ -26211,13 +26211,13 @@
         <v>0.48142499999999999</v>
       </c>
       <c r="BD137" s="3">
-        <v>9.0982171880596999E-2</v>
+        <v>9.8197534498659603E-2</v>
       </c>
       <c r="BE137" s="3">
-        <v>0.360694054933131</v>
+        <v>0.38504293582951099</v>
       </c>
       <c r="BF137" s="3">
-        <v>509585.037717</v>
+        <v>575247.58849000104</v>
       </c>
       <c r="BG137" s="3">
         <v>1.5542</v>
@@ -26447,13 +26447,13 @@
         <v>0.2656</v>
       </c>
       <c r="BD138" s="3">
-        <v>9.1000206091229996E-2</v>
+        <v>9.9332393209383293E-2</v>
       </c>
       <c r="BE138" s="3">
-        <v>0.35993805700138698</v>
+        <v>0.39037054489607398</v>
       </c>
       <c r="BF138" s="3">
-        <v>514859.24478000001</v>
+        <v>595950.53228900104</v>
       </c>
       <c r="BG138" s="3">
         <v>1.1416999999999999</v>
@@ -26685,13 +26685,13 @@
         <v>-5.4499999999999965E-3</v>
       </c>
       <c r="BD139" s="3">
-        <v>9.0753859900629993E-2</v>
+        <v>9.8431541290753599E-2</v>
       </c>
       <c r="BE139" s="3">
-        <v>0.356663737640182</v>
+        <v>0.38228243770440901</v>
       </c>
       <c r="BF139" s="3">
-        <v>517288.66819599998</v>
+        <v>604404.23213200003</v>
       </c>
       <c r="BG139" s="3">
         <v>0.89</v>
@@ -26923,13 +26923,13 @@
         <v>-9.8674999999999999E-2</v>
       </c>
       <c r="BD140" s="3">
-        <v>9.1686384503664994E-2</v>
+        <v>9.63454278994757E-2</v>
       </c>
       <c r="BE140" s="3">
-        <v>0.35923179806250299</v>
+        <v>0.36705215763836102</v>
       </c>
       <c r="BF140" s="3">
-        <v>539596.43202299904</v>
+        <v>606079.12960700004</v>
       </c>
       <c r="BG140" s="3">
         <v>0.88780000000000003</v>
@@ -27161,13 +27161,13 @@
         <v>3.9625E-2</v>
       </c>
       <c r="BD141" s="3">
-        <v>9.2507046533527995E-2</v>
+        <v>9.4772382842493494E-2</v>
       </c>
       <c r="BE141" s="3">
-        <v>0.365376874528691</v>
+        <v>0.35779248415542297</v>
       </c>
       <c r="BF141" s="3">
-        <v>569839.51083899895</v>
+        <v>604684.02785800002</v>
       </c>
       <c r="BG141" s="3">
         <v>0.94359999999999999</v>
@@ -27399,13 +27399,13 @@
         <v>3.5875000000000004E-2</v>
       </c>
       <c r="BD142" s="3">
-        <v>8.8952937407489996E-2</v>
+        <v>9.1903066120946703E-2</v>
       </c>
       <c r="BE142" s="3">
-        <v>0.35755347955380201</v>
+        <v>0.34649923951664602</v>
       </c>
       <c r="BF142" s="3">
-        <v>558238.840814</v>
+        <v>575499.71504799998</v>
       </c>
       <c r="BG142" s="3">
         <v>0.95289999999999997</v>
@@ -27637,13 +27637,13 @@
         <v>-7.7149999999999996E-2</v>
       </c>
       <c r="BD143" s="3">
-        <v>8.5076896434250995E-2</v>
+        <v>8.9126766499728505E-2</v>
       </c>
       <c r="BE143" s="3">
-        <v>0.34806969644597402</v>
+        <v>0.34071617181951303</v>
       </c>
       <c r="BF143" s="3">
-        <v>539527.66899599996</v>
+        <v>554376.87906399998</v>
       </c>
       <c r="BG143" s="3">
         <v>0.877</v>
@@ -27875,13 +27875,13 @@
         <v>-4.9800000000000004E-2</v>
       </c>
       <c r="BD144" s="3">
-        <v>8.3723845152155002E-2</v>
+        <v>8.7805938617518994E-2</v>
       </c>
       <c r="BE144" s="3">
-        <v>0.34683893183866898</v>
+        <v>0.342299824722607</v>
       </c>
       <c r="BF144" s="3">
-        <v>544309.38919300097</v>
+        <v>559597.44567600102</v>
       </c>
       <c r="BG144" s="3">
         <v>0.95779999999999998</v>
@@ -28113,13 +28113,13 @@
         <v>-0.100975</v>
       </c>
       <c r="BD145" s="3">
-        <v>8.4642999668490995E-2</v>
+        <v>8.8231655305638104E-2</v>
       </c>
       <c r="BE145" s="3">
-        <v>0.354446259058664</v>
+        <v>0.34814606714966201</v>
       </c>
       <c r="BF145" s="3">
-        <v>571384.567821</v>
+        <v>583731.24020200095</v>
       </c>
       <c r="BG145" s="3">
         <v>0.99639999999999995</v>
@@ -28351,13 +28351,13 @@
         <v>-2.2450000000000001E-2</v>
       </c>
       <c r="BD146" s="3">
-        <v>8.3350445187202998E-2</v>
+        <v>8.7373494784597897E-2</v>
       </c>
       <c r="BE146" s="3">
-        <v>0.35433942075258401</v>
+        <v>0.34427772496258602</v>
       </c>
       <c r="BF146" s="3">
-        <v>572747.85307799897</v>
+        <v>584154.66466999904</v>
       </c>
       <c r="BG146" s="3">
         <v>1.0276000000000001</v>
@@ -28589,13 +28589,13 @@
         <v>3.7799999999999993E-2</v>
       </c>
       <c r="BD147" s="3">
-        <v>8.2545211719847994E-2</v>
+        <v>8.7096922869808996E-2</v>
       </c>
       <c r="BE147" s="3">
-        <v>0.357560714241553</v>
+        <v>0.346725595722431</v>
       </c>
       <c r="BF147" s="3">
-        <v>578854.59837099805</v>
+        <v>592391.35166999802</v>
       </c>
       <c r="BG147" s="3">
         <v>1.1998</v>
@@ -28827,13 +28827,13 @@
         <v>0.21395</v>
       </c>
       <c r="BD148" s="3">
-        <v>8.3100940554145006E-2</v>
+        <v>8.7347311038133799E-2</v>
       </c>
       <c r="BE148" s="3">
-        <v>0.36519778828713401</v>
+        <v>0.35613226940426601</v>
       </c>
       <c r="BF148" s="3">
-        <v>605220.62265799905</v>
+        <v>620251.97499699797</v>
       </c>
       <c r="BG148" s="3">
         <v>1.2437</v>
@@ -29065,13 +29065,13 @@
         <v>0.22452499999999997</v>
       </c>
       <c r="BD149" s="3">
-        <v>8.4882595590634005E-2</v>
+        <v>8.8599207862926702E-2</v>
       </c>
       <c r="BE149" s="3">
-        <v>0.37589276283496897</v>
+        <v>0.36994871612716901</v>
       </c>
       <c r="BF149" s="3">
-        <v>646480.26452099998</v>
+        <v>668454.10531999904</v>
       </c>
       <c r="BG149" s="3">
         <v>1.4291</v>
@@ -29303,13 +29303,13 @@
         <v>0.261075</v>
       </c>
       <c r="BD150" s="3">
-        <v>8.3739719689330999E-2</v>
+        <v>8.8152311126601005E-2</v>
       </c>
       <c r="BE150" s="3">
-        <v>0.37367858475329901</v>
+        <v>0.37084312377696599</v>
       </c>
       <c r="BF150" s="3">
-        <v>652963.24330300104</v>
+        <v>684205.32857400004</v>
       </c>
       <c r="BG150" s="3">
         <v>1.8412999999999999</v>
@@ -29546,13 +29546,13 @@
         <v>0.265625</v>
       </c>
       <c r="BD151" s="3">
-        <v>8.3885983875489997E-2</v>
+        <v>8.8971682961072204E-2</v>
       </c>
       <c r="BE151" s="3">
-        <v>0.37871700597491198</v>
+        <v>0.37778449550932203</v>
       </c>
       <c r="BF151" s="3">
-        <v>670961.53617700096</v>
+        <v>704042.39160500094</v>
       </c>
       <c r="BG151" s="3">
         <v>1.972</v>
@@ -29789,13 +29789,13 @@
         <v>0.47762499999999997</v>
       </c>
       <c r="BD152" s="3">
-        <v>8.6234366133703E-2</v>
+        <v>9.10237290275447E-2</v>
       </c>
       <c r="BE152" s="3">
-        <v>0.39512507919832801</v>
+        <v>0.39252842529805998</v>
       </c>
       <c r="BF152" s="3">
-        <v>719383.185201001</v>
+        <v>741476.79032100202</v>
       </c>
       <c r="BG152" s="3">
         <v>2.0950000000000002</v>
@@ -30032,13 +30032,13 @@
         <v>0.48585</v>
       </c>
       <c r="BD153" s="3">
-        <v>8.8059394820539996E-2</v>
+        <v>9.2284885043628903E-2</v>
       </c>
       <c r="BE153" s="3">
-        <v>0.40968025916748602</v>
+        <v>0.40288171341023599</v>
       </c>
       <c r="BF153" s="3">
-        <v>764820.32628000097</v>
+        <v>777450.36399800098</v>
       </c>
       <c r="BG153" s="3">
         <v>1.9807999999999999</v>
@@ -30275,13 +30275,13 @@
         <v>0.16820000000000002</v>
       </c>
       <c r="BD154" s="3">
-        <v>8.5869919429733002E-2</v>
+        <v>9.1224099377405596E-2</v>
       </c>
       <c r="BE154" s="3">
-        <v>0.40686360779719399</v>
+        <v>0.398514027836253</v>
       </c>
       <c r="BF154" s="3">
-        <v>753679.60455299995</v>
+        <v>769947.22196700005</v>
       </c>
       <c r="BG154" s="3">
         <v>1.8228</v>
@@ -30518,13 +30518,13 @@
         <v>-2.0299999999999999E-2</v>
       </c>
       <c r="BD155" s="3">
-        <v>8.4747383383226002E-2</v>
+        <v>9.1485735578219901E-2</v>
       </c>
       <c r="BE155" s="3">
-        <v>0.40740080249020499</v>
+        <v>0.401063132345579</v>
       </c>
       <c r="BF155" s="3">
-        <v>750805.117111</v>
+        <v>776975.590845</v>
       </c>
       <c r="BG155" s="3">
         <v>1.6871</v>
@@ -30761,13 +30761,13 @@
         <v>-3.9900000000000019E-2</v>
       </c>
       <c r="BD156" s="3">
-        <v>8.6937409265431004E-2</v>
+        <v>9.3389492671592605E-2</v>
       </c>
       <c r="BE156" s="3">
-        <v>0.42268343408800901</v>
+        <v>0.41654830440637802</v>
       </c>
       <c r="BF156" s="3">
-        <v>800187.44256400003</v>
+        <v>825967.21187899995</v>
       </c>
       <c r="BG156" s="3">
         <v>1.6107</v>
@@ -31004,13 +31004,13 @@
         <v>-0.35852500000000004</v>
       </c>
       <c r="BD157" s="3">
-        <v>8.8416142300110995E-2</v>
+        <v>9.4849643448382107E-2</v>
       </c>
       <c r="BE157" s="3">
-        <v>0.43515432801062898</v>
+        <v>0.43436518910064997</v>
       </c>
       <c r="BF157" s="3">
-        <v>855971.31530100002</v>
+        <v>886237.21618700004</v>
       </c>
       <c r="BG157" s="3">
         <v>1.5905</v>
@@ -31247,13 +31247,13 @@
         <v>-0.17615</v>
       </c>
       <c r="BD158" s="3">
-        <v>8.4729078005526995E-2</v>
+        <v>9.2673566022909701E-2</v>
       </c>
       <c r="BE158" s="3">
-        <v>0.42276394115192001</v>
+        <v>0.430154309651547</v>
       </c>
       <c r="BF158" s="3">
-        <v>836074.36494</v>
+        <v>882615.18565600005</v>
       </c>
       <c r="BG158" s="3">
         <v>1.593</v>
@@ -31490,13 +31490,13 @@
         <v>-0.12994999999999998</v>
       </c>
       <c r="BD159" s="3">
-        <v>8.0248352776047999E-2</v>
+        <v>8.8907961464829405E-2</v>
       </c>
       <c r="BE159" s="3">
-        <v>0.40513732323438001</v>
+        <v>0.41579188779742798</v>
       </c>
       <c r="BF159" s="3">
-        <v>796075.61965699994</v>
+        <v>853433.63927199901</v>
       </c>
       <c r="BG159" s="3">
         <v>1.4676</v>
@@ -31733,13 +31733,13 @@
         <v>-4.8099999999999997E-2</v>
       </c>
       <c r="BD160" s="3">
-        <v>8.1718250850916996E-2</v>
+        <v>8.8476818976236604E-2</v>
       </c>
       <c r="BE160" s="3">
-        <v>0.41536908536806699</v>
+        <v>0.41598292619168298</v>
       </c>
       <c r="BF160" s="3">
-        <v>830582.27102699899</v>
+        <v>875993.30236299895</v>
       </c>
       <c r="BG160" s="3">
         <v>1.4797</v>
@@ -31976,13 +31976,13 @@
         <v>9.9725000000000008E-2</v>
       </c>
       <c r="BD161" s="3">
-        <v>8.6497241071109995E-2</v>
+        <v>9.1788093273054094E-2</v>
       </c>
       <c r="BE161" s="3">
-        <v>0.44362968944108999</v>
+        <v>0.43598039196781202</v>
       </c>
       <c r="BF161" s="3">
-        <v>912372.99968699901</v>
+        <v>951115.27888899902</v>
       </c>
       <c r="BG161" s="3">
         <v>1.524</v>
@@ -32219,13 +32219,13 @@
         <v>0.19262499999999999</v>
       </c>
       <c r="BD162" s="3">
-        <v>8.8863053571093004E-2</v>
+        <v>9.5969352362422697E-2</v>
       </c>
       <c r="BE162" s="3">
-        <v>0.46681034025423301</v>
+        <v>0.46526361432306201</v>
       </c>
       <c r="BF162" s="3">
-        <v>959335.87584399898</v>
+        <v>1014619.1955950001</v>
       </c>
       <c r="BG162" s="3">
         <v>1.5034000000000001</v>
@@ -32462,13 +32462,13 @@
         <v>0.439025</v>
       </c>
       <c r="BD163" s="3">
-        <v>8.8476823852007003E-2</v>
+        <v>9.7481357448031103E-2</v>
       </c>
       <c r="BE163" s="3">
-        <v>0.47455922040375098</v>
+        <v>0.48475995089219898</v>
       </c>
       <c r="BF163" s="3">
-        <v>966770.18469799997</v>
+        <v>1041815.1880570001</v>
       </c>
       <c r="BG163" s="3">
         <v>1.7632000000000001</v>
@@ -32705,13 +32705,13 @@
         <v>0.47524999999999995</v>
       </c>
       <c r="BD164" s="3">
-        <v>8.8451213810080004E-2</v>
+        <v>9.5848009146308102E-2</v>
       </c>
       <c r="BE164" s="3">
-        <v>0.47472258515393001</v>
+        <v>0.48391276797447702</v>
       </c>
       <c r="BF164" s="3">
-        <v>984170.76196900196</v>
+        <v>1051064.1223319999</v>
       </c>
       <c r="BG164" s="3">
         <v>1.7269000000000001</v>
@@ -32948,13 +32948,13 @@
         <v>0.455675</v>
       </c>
       <c r="BD165" s="3">
-        <v>8.7989992423445004E-2</v>
+        <v>9.2987632155279498E-2</v>
       </c>
       <c r="BE165" s="3">
-        <v>0.46945747545170402</v>
+        <v>0.472024525039697</v>
       </c>
       <c r="BF165" s="3">
-        <v>1005244.212053</v>
+        <v>1048292.986383</v>
       </c>
       <c r="BG165" s="3">
         <v>1.6442000000000001</v>
@@ -33191,13 +33191,13 @@
         <v>0.26757500000000001</v>
       </c>
       <c r="BD166" s="3">
-        <v>8.6583195760755002E-2</v>
+        <v>9.1903579477757499E-2</v>
       </c>
       <c r="BE166" s="3">
-        <v>0.46491958079231499</v>
+        <v>0.46692677602039001</v>
       </c>
       <c r="BF166" s="3">
-        <v>1005743.163708</v>
+        <v>1043393.937817</v>
       </c>
       <c r="BG166" s="3">
         <v>1.4482999999999999</v>
@@ -33434,13 +33434,13 @@
         <v>8.0625000000000002E-2</v>
       </c>
       <c r="BD167" s="3">
-        <v>8.5105764655282995E-2</v>
+        <v>9.1700148715228205E-2</v>
       </c>
       <c r="BE167" s="3">
-        <v>0.46143260614345399</v>
+        <v>0.46808400013568502</v>
       </c>
       <c r="BF167" s="3">
-        <v>1004114.421647</v>
+        <v>1052799.2064439999</v>
       </c>
       <c r="BG167" s="3">
         <v>1.2152000000000001</v>
@@ -33677,13 +33677,13 @@
         <v>6.08E-2</v>
       </c>
       <c r="BD168" s="3">
-        <v>8.6125718418775005E-2</v>
+        <v>9.1720680229395002E-2</v>
       </c>
       <c r="BE168" s="3">
-        <v>0.46607366836560399</v>
+        <v>0.46857339113407198</v>
       </c>
       <c r="BF168" s="3">
-        <v>1036397.270263</v>
+        <v>1086534.195416</v>
       </c>
       <c r="BG168" s="3">
         <v>1.2535000000000001</v>
@@ -33920,13 +33920,13 @@
         <v>0.34792500000000004</v>
       </c>
       <c r="BD169" s="3">
-        <v>8.6504011312098006E-2</v>
+        <v>9.1227397678685901E-2</v>
       </c>
       <c r="BE169" s="3">
-        <v>0.46344286210748098</v>
+        <v>0.46492377592838902</v>
       </c>
       <c r="BF169" s="3">
-        <v>1052834.475412</v>
+        <v>1113729.103593</v>
       </c>
       <c r="BG169" s="3">
         <v>1.6213</v>
@@ -34163,13 +34163,13 @@
         <v>0.28492499999999998</v>
       </c>
       <c r="BD170" s="3">
-        <v>8.6354588903019003E-2</v>
+        <v>9.2351021839123901E-2</v>
       </c>
       <c r="BE170" s="3">
-        <v>0.46396991771948398</v>
+        <v>0.47301467679493098</v>
       </c>
       <c r="BF170" s="3">
-        <v>1047787.382448</v>
+        <v>1128938.1245820001</v>
       </c>
       <c r="BG170" s="3">
         <v>1.5216000000000001</v>
@@ -34406,13 +34406,13 @@
         <v>0.20732499999999998</v>
       </c>
       <c r="BD171" s="3">
-        <v>8.7355054852066003E-2</v>
+        <v>9.4969761704192607E-2</v>
       </c>
       <c r="BE171" s="3">
-        <v>0.47278427334548701</v>
+        <v>0.49256118708894298</v>
       </c>
       <c r="BF171" s="3">
-        <v>1063344.288308</v>
+        <v>1172130.6602479999</v>
       </c>
       <c r="BG171" s="3">
         <v>1.4752000000000001</v>
@@ -34649,13 +34649,13 @@
         <v>0.20484999999999998</v>
       </c>
       <c r="BD172" s="3">
-        <v>9.0502114983782994E-2</v>
+        <v>9.7208709081763003E-2</v>
       </c>
       <c r="BE172" s="3">
-        <v>0.48642626914901399</v>
+        <v>0.50607480717238096</v>
       </c>
       <c r="BF172" s="3">
-        <v>1119161.411882</v>
+        <v>1235839.9295930001</v>
       </c>
       <c r="BG172" s="3">
         <v>1.4875</v>
@@ -34892,13 +34892,13 @@
         <v>0.18975</v>
       </c>
       <c r="BD173" s="3">
-        <v>9.1931480710982005E-2</v>
+        <v>9.7010891729449794E-2</v>
       </c>
       <c r="BE173" s="3">
-        <v>0.48795015834571598</v>
+        <v>0.49997155703822599</v>
       </c>
       <c r="BF173" s="3">
-        <v>1158109.0792410001</v>
+        <v>1263137.6316579999</v>
       </c>
       <c r="BG173" s="3">
         <v>1.5107999999999999</v>
@@ -35135,13 +35135,13 @@
         <v>0.12354999999999999</v>
       </c>
       <c r="BD174" s="3">
-        <v>9.0118829904766995E-2</v>
+        <v>9.6824940225198206E-2</v>
       </c>
       <c r="BE174" s="3">
-        <v>0.47825119993639298</v>
+        <v>0.49303890050215199</v>
       </c>
       <c r="BF174" s="3">
-        <v>1144914.921572</v>
+        <v>1257073.9782410001</v>
       </c>
       <c r="BG174" s="3">
         <v>1.3742000000000001</v>
@@ -35378,13 +35378,13 @@
         <v>4.6975000000000003E-2</v>
       </c>
       <c r="BD175" s="3">
-        <v>8.8879966643726993E-2</v>
+        <v>9.7997031239655294E-2</v>
       </c>
       <c r="BE175" s="3">
-        <v>0.47562836766065097</v>
+        <v>0.49960535578270598</v>
       </c>
       <c r="BF175" s="3">
-        <v>1140101.155398</v>
+        <v>1267389.4143099999</v>
       </c>
       <c r="BG175" s="3">
         <v>1.3351999999999999</v>
@@ -35621,13 +35621,13 @@
         <v>0.12515000000000001</v>
       </c>
       <c r="BD176" s="3">
-        <v>9.1476244892242001E-2</v>
+        <v>0.100195826219834</v>
       </c>
       <c r="BE176" s="3">
-        <v>0.493924847601379</v>
+        <v>0.51646638452765004</v>
       </c>
       <c r="BF176" s="3">
-        <v>1201238.4962249999</v>
+        <v>1329431.5372609999</v>
       </c>
       <c r="BG176" s="3">
         <v>1.5062</v>
@@ -35864,13 +35864,13 @@
         <v>0.13067500000000001</v>
       </c>
       <c r="BD177" s="3">
-        <v>9.3556159960108007E-2</v>
+        <v>9.9708888561341399E-2</v>
       </c>
       <c r="BE177" s="3">
-        <v>0.508704812263854</v>
+        <v>0.51969344773535298</v>
       </c>
       <c r="BF177" s="3">
-        <v>1261131.684564</v>
+        <v>1373624.804581</v>
       </c>
       <c r="BG177" s="3">
         <v>1.4388000000000001</v>
@@ -36107,13 +36107,13 @@
         <v>7.1899999999999992E-2</v>
       </c>
       <c r="BD178" s="3">
-        <v>9.3347976519483997E-2</v>
+        <v>9.8007302548250103E-2</v>
       </c>
       <c r="BE178" s="3">
-        <v>0.51362588314105195</v>
+        <v>0.51288000216504104</v>
       </c>
       <c r="BF178" s="3">
-        <v>1271120.861152</v>
+        <v>1354747.9522820001</v>
       </c>
       <c r="BG178" s="3">
         <v>1.4533</v>
@@ -36350,13 +36350,13 @@
         <v>1.7750000000000005E-3</v>
       </c>
       <c r="BD179" s="3">
-        <v>9.1519476421853999E-2</v>
+        <v>9.6091235624672006E-2</v>
       </c>
       <c r="BE179" s="3">
-        <v>0.51278398558041505</v>
+        <v>0.50889703477466097</v>
       </c>
       <c r="BF179" s="3">
-        <v>1271050.393833</v>
+        <v>1339364.4774720001</v>
       </c>
       <c r="BG179" s="3">
         <v>1.4012</v>
@@ -36593,13 +36593,13 @@
         <v>-2.4625000000000001E-2</v>
       </c>
       <c r="BD180" s="3">
-        <v>9.0382151282107998E-2</v>
+        <v>9.4754266721934002E-2</v>
       </c>
       <c r="BE180" s="3">
-        <v>0.512417283364901</v>
+        <v>0.51392834619212002</v>
       </c>
       <c r="BF180" s="3">
-        <v>1308328.5930880001</v>
+        <v>1379822.7631969999</v>
       </c>
       <c r="BG180" s="3">
         <v>1.4315</v>
@@ -36836,13 +36836,13 @@
         <v>-0.12909999999999999</v>
       </c>
       <c r="BD181" s="3">
-        <v>8.9287828367637004E-2</v>
+        <v>9.2505791037579804E-2</v>
       </c>
       <c r="BE181" s="3">
-        <v>0.50725774903656795</v>
+        <v>0.51096760296174304</v>
       </c>
       <c r="BF181" s="3">
-        <v>1350991.667019</v>
+        <v>1426684.376039</v>
       </c>
       <c r="BG181" s="3">
         <v>1.3460000000000001</v>
@@ -37079,13 +37079,13 @@
         <v>-0.32047499999999995</v>
       </c>
       <c r="BD182" s="3">
-        <v>8.6260685919720997E-2</v>
+        <v>8.95188896643693E-2</v>
       </c>
       <c r="BE182" s="3">
-        <v>0.48343075648276801</v>
+        <v>0.493087375225501</v>
       </c>
       <c r="BF182" s="3">
-        <v>1313322.3218759999</v>
+        <v>1402545.1649239999</v>
       </c>
       <c r="BG182" s="3">
         <v>1.2428999999999999</v>
@@ -37322,13 +37322,13 @@
         <v>-0.30645</v>
       </c>
       <c r="BD183" s="3">
-        <v>8.3960786272857996E-2</v>
+        <v>8.7360526230093494E-2</v>
       </c>
       <c r="BE183" s="3">
-        <v>0.46360117816438801</v>
+        <v>0.47639479392581002</v>
       </c>
       <c r="BF183" s="3">
-        <v>1266909.634199</v>
+        <v>1356254.48377</v>
       </c>
       <c r="BG183" s="3">
         <v>1.2508999999999999</v>
@@ -37565,13 +37565,13 @@
         <v>-0.31940000000000002</v>
       </c>
       <c r="BD184" s="3">
-        <v>8.3883037642049005E-2</v>
+        <v>8.6936153557970505E-2</v>
       </c>
       <c r="BE184" s="3">
-        <v>0.45751906171116302</v>
+        <v>0.46768546200406302</v>
       </c>
       <c r="BF184" s="3">
-        <v>1284483.932756</v>
+        <v>1365085.6788910001</v>
       </c>
       <c r="BG184" s="3">
         <v>1.2150000000000001</v>
@@ -37808,13 +37808,13 @@
         <v>-0.25207499999999999</v>
       </c>
       <c r="BD185" s="3">
-        <v>8.2638251029754001E-2</v>
+        <v>8.4476952260826702E-2</v>
       </c>
       <c r="BE185" s="3">
-        <v>0.45175479220239001</v>
+        <v>0.45304482796592699</v>
       </c>
       <c r="BF185" s="3">
-        <v>1313293.3809720001</v>
+        <v>1373790.446738</v>
       </c>
       <c r="BG185" s="3">
         <v>1.2815000000000001</v>
@@ -38051,13 +38051,13 @@
         <v>-0.259575</v>
       </c>
       <c r="BD186" s="3">
-        <v>7.9438197147320005E-2</v>
+        <v>8.0002704411172396E-2</v>
       </c>
       <c r="BE186" s="3">
-        <v>0.43402941835218101</v>
+        <v>0.42419702397794001</v>
       </c>
       <c r="BF186" s="3">
-        <v>1273488.4809079999</v>
+        <v>1306116.3662459999</v>
       </c>
       <c r="BG186" s="3">
         <v>1.2770999999999999</v>
@@ -38294,13 +38294,13 @@
         <v>-0.26277499999999998</v>
       </c>
       <c r="BD187" s="3">
-        <v>7.7680585894412998E-2</v>
+        <v>7.7551042355454805E-2</v>
       </c>
       <c r="BE187" s="3">
-        <v>0.42659370842218203</v>
+        <v>0.41028480184389499</v>
       </c>
       <c r="BF187" s="3">
-        <v>1253120.415242</v>
+        <v>1267650.525997</v>
       </c>
       <c r="BG187" s="3">
         <v>1.3073999999999999</v>
@@ -38537,13 +38537,13 @@
         <v>-0.2112</v>
       </c>
       <c r="BD188" s="3">
-        <v>7.9507563331361997E-2</v>
+        <v>7.9991704142931205E-2</v>
       </c>
       <c r="BE188" s="3">
-        <v>0.437431581092531</v>
+        <v>0.42726953031528803</v>
       </c>
       <c r="BF188" s="3">
-        <v>1315307.7961850001</v>
+        <v>1346071.0409599999</v>
       </c>
       <c r="BG188" s="3">
         <v>1.3132999999999999</v>
@@ -38780,13 +38780,13 @@
         <v>-9.1175000000000006E-2</v>
       </c>
       <c r="BD189" s="3">
-        <v>8.1645503759540994E-2</v>
+        <v>8.2873271568599402E-2</v>
       </c>
       <c r="BE189" s="3">
-        <v>0.44995153777067998</v>
+        <v>0.44900507808502099</v>
       </c>
       <c r="BF189" s="3">
-        <v>1401810.431655</v>
+        <v>1463473.877817</v>
       </c>
       <c r="BG189" s="3">
         <v>1.4167000000000001</v>
@@ -39023,13 +39023,13 @@
         <v>-0.27934999999999999</v>
       </c>
       <c r="BD190" s="3">
-        <v>7.9907681235962993E-2</v>
+        <v>8.2180385316430404E-2</v>
       </c>
       <c r="BE190" s="3">
-        <v>0.437230802543981</v>
+        <v>0.44248097117239898</v>
       </c>
       <c r="BF190" s="3">
-        <v>1369229.4134509999</v>
+        <v>1454889.054151</v>
       </c>
       <c r="BG190" s="3">
         <v>1.3314999999999999</v>
@@ -39266,13 +39266,13 @@
         <v>-0.31377500000000003</v>
       </c>
       <c r="BD191" s="3">
-        <v>7.7931653320703995E-2</v>
+        <v>8.0111699622274296E-2</v>
       </c>
       <c r="BE191" s="3">
-        <v>0.42640228820349502</v>
+        <v>0.426690089252725</v>
       </c>
       <c r="BF191" s="3">
-        <v>1332472.3659930001</v>
+        <v>1405601.3965419999</v>
       </c>
       <c r="BG191" s="3">
         <v>1.2784</v>
@@ -39509,13 +39509,13 @@
         <v>-0.37607500000000005</v>
       </c>
       <c r="BD192" s="3">
-        <v>8.0030012787788998E-2</v>
+        <v>8.1492797114471605E-2</v>
       </c>
       <c r="BE192" s="3">
-        <v>0.44026266913119</v>
+        <v>0.42964781413515302</v>
       </c>
       <c r="BF192" s="3">
-        <v>1417943.302006</v>
+        <v>1464728.7177500001</v>
       </c>
       <c r="BG192" s="3">
         <v>1.2848999999999999</v>
@@ -39752,13 +39752,13 @@
         <v>-0.34962499999999996</v>
       </c>
       <c r="BD193" s="3">
-        <v>8.2690759157363999E-2</v>
+        <v>8.3481963562084399E-2</v>
       </c>
       <c r="BE193" s="3">
-        <v>0.460430589618607</v>
+        <v>0.44285541325515498</v>
       </c>
       <c r="BF193" s="3">
-        <v>1541428.3677399999</v>
+        <v>1573055.449297</v>
       </c>
       <c r="BG193" s="3">
         <v>1.3058000000000001</v>
@@ -39995,13 +39995,13 @@
         <v>-0.42622499999999997</v>
       </c>
       <c r="BD194" s="3">
-        <v>8.0970213447365005E-2</v>
+        <v>8.1343622425269102E-2</v>
       </c>
       <c r="BE194" s="3">
-        <v>0.45005784346244099</v>
+        <v>0.43259274029622502</v>
       </c>
       <c r="BF194" s="3">
-        <v>1516576.454445</v>
+        <v>1550285.888909</v>
       </c>
       <c r="BG194" s="3">
         <v>1.2424999999999999</v>
@@ -40238,13 +40238,13 @@
         <v>-0.48419999999999996</v>
       </c>
       <c r="BD195" s="3">
-        <v>7.9326846731240006E-2</v>
+        <v>7.9228891426911294E-2</v>
       </c>
       <c r="BE195" s="3">
-        <v>0.44081880865453599</v>
+        <v>0.42483540383970297</v>
       </c>
       <c r="BF195" s="3">
-        <v>1484302.863905</v>
+        <v>1520779.5674419899</v>
       </c>
       <c r="BG195" s="3">
         <v>1.1975</v>
@@ -40481,13 +40481,13 @@
         <v>-0.49975000000000003</v>
       </c>
       <c r="BD196" s="3">
-        <v>8.2045091853422999E-2</v>
+        <v>8.1961991960999195E-2</v>
       </c>
       <c r="BE196" s="3">
-        <v>0.45897740179574398</v>
+        <v>0.44309622786608999</v>
       </c>
       <c r="BF196" s="3">
-        <v>1585697.855064</v>
+        <v>1622946.4541859999</v>
       </c>
       <c r="BG196" s="3">
         <v>1.2225999999999999</v>
@@ -40724,13 +40724,13 @@
         <v>-0.37725000000000009</v>
       </c>
       <c r="BD197" s="3">
-        <v>8.5682340685590996E-2</v>
+        <v>8.7257391043650295E-2</v>
       </c>
       <c r="BE197" s="3">
-        <v>0.49363399903577398</v>
+        <v>0.484113939898701</v>
       </c>
       <c r="BF197" s="3">
-        <v>1774877.924722</v>
+        <v>1856432.698355</v>
       </c>
       <c r="BG197" s="3">
         <v>1.3562000000000001</v>
@@ -40967,13 +40967,13 @@
         <v>-0.37787500000000002</v>
       </c>
       <c r="BD198" s="3">
-        <v>8.4254035535221997E-2</v>
+        <v>8.9069311208941904E-2</v>
       </c>
       <c r="BE198" s="3">
-        <v>0.50112710073391997</v>
+        <v>0.50102763382000504</v>
       </c>
       <c r="BF198" s="3">
-        <v>1820395.1988979999</v>
+        <v>1963260.6869020001</v>
       </c>
       <c r="BG198" s="3">
         <v>1.3443000000000001</v>
@@ -41210,13 +41210,13 @@
         <v>-0.39492499999999997</v>
       </c>
       <c r="BD199" s="3">
-        <v>8.0544981765361998E-2</v>
+        <v>8.5774298540575999E-2</v>
       </c>
       <c r="BE199" s="3">
-        <v>0.49029347246113503</v>
+        <v>0.491069598143279</v>
       </c>
       <c r="BF199" s="3">
-        <v>1794671.0088839999</v>
+        <v>1944667.7211130001</v>
       </c>
       <c r="BG199" s="3">
         <v>1.3249</v>
@@ -41453,13 +41453,13 @@
         <v>-2.6275000000000007E-2</v>
       </c>
       <c r="BD200" s="3">
-        <v>7.9751550107385993E-2</v>
+        <v>8.3830668884080597E-2</v>
       </c>
       <c r="BE200" s="3">
-        <v>0.48786582443825299</v>
+        <v>0.48713464359083303</v>
       </c>
       <c r="BF200" s="3">
-        <v>1841793.121387</v>
+        <v>1973962.0342659999</v>
       </c>
       <c r="BG200" s="3">
         <v>2.0169000000000001</v>
@@ -41696,13 +41696,13 @@
         <v>9.9324999999999997E-2</v>
       </c>
       <c r="BD201" s="3">
-        <v>8.0584860121308E-2</v>
+        <v>8.5485815289618697E-2</v>
       </c>
       <c r="BE201" s="3">
-        <v>0.49544549404110499</v>
+        <v>0.50542849417748903</v>
       </c>
       <c r="BF201" s="3">
-        <v>1934358.572381</v>
+        <v>2095529.3774039999</v>
       </c>
       <c r="BG201" s="3">
         <v>2.1269</v>
@@ -41939,13 +41939,13 @@
         <v>-0.14847500000000002</v>
       </c>
       <c r="BD202" s="3">
-        <v>7.8429057882262995E-2</v>
+        <v>8.7200331549039806E-2</v>
       </c>
       <c r="BE202" s="3">
-        <v>0.48747814581998999</v>
+        <v>0.51458915218921397</v>
       </c>
       <c r="BF202" s="3">
-        <v>1918496.6387130001</v>
+        <v>2141942.8826970002</v>
       </c>
       <c r="BG202" s="3">
         <v>1.833</v>
@@ -42182,13 +42182,13 @@
         <v>-0.183</v>
       </c>
       <c r="BD203" s="3">
-        <v>7.6543500877357007E-2</v>
+        <v>8.6837262262623394E-2</v>
       </c>
       <c r="BE203" s="3">
-        <v>0.48314940686660002</v>
+        <v>0.51306388873522701</v>
       </c>
       <c r="BF203" s="3">
-        <v>1914998.750609</v>
+        <v>2153899.3396999999</v>
       </c>
       <c r="BG203" s="3">
         <v>1.7621</v>
@@ -42425,13 +42425,13 @@
         <v>-1.4574999999999998E-2</v>
       </c>
       <c r="BD204" s="3">
-        <v>7.8530144732589999E-2</v>
+        <v>8.5441149045543993E-2</v>
       </c>
       <c r="BE204" s="3">
-        <v>0.491563541252311</v>
+        <v>0.50530179899408101</v>
       </c>
       <c r="BF204" s="3">
-        <v>2033460.790418</v>
+        <v>2198009.4816919998</v>
       </c>
       <c r="BG204" s="3">
         <v>2.0268999999999999</v>
@@ -42668,13 +42668,13 @@
         <v>-4.1075E-2</v>
       </c>
       <c r="BD205" s="3">
-        <v>8.1921579105803E-2</v>
+        <v>8.5583091674896097E-2</v>
       </c>
       <c r="BE205" s="3">
-        <v>0.51001163083462198</v>
+        <v>0.51733370630320896</v>
       </c>
       <c r="BF205" s="3">
-        <v>2239412.315339</v>
+        <v>2401940.4380979999</v>
       </c>
       <c r="BG205" s="3">
         <v>2.0446</v>
@@ -42911,13 +42911,13 @@
         <v>0.14902500000000002</v>
       </c>
       <c r="BD206" s="3">
-        <v>8.1545071333401997E-2</v>
+        <v>8.6126926882751406E-2</v>
       </c>
       <c r="BE206" s="3">
-        <v>0.50335288148540103</v>
+        <v>0.51769974380684702</v>
       </c>
       <c r="BF206" s="3">
-        <v>2306907.4125040001</v>
+        <v>2548321.8655079999</v>
       </c>
       <c r="BG206" s="3">
         <v>2.3315999999999999</v>
@@ -43154,13 +43154,13 @@
         <v>0.58607500000000001</v>
       </c>
       <c r="BD207" s="3">
-        <v>7.8792418978004E-2</v>
+        <v>8.4088242013658096E-2</v>
       </c>
       <c r="BE207" s="3">
-        <v>0.48944490148430098</v>
+        <v>0.50203399727648401</v>
       </c>
       <c r="BF207" s="3">
-        <v>2303722.6324570002</v>
+        <v>2562218.7626140001</v>
       </c>
       <c r="BG207" s="3">
         <v>2.835</v>
@@ -43397,13 +43397,13 @@
         <v>0.96545000000000003</v>
       </c>
       <c r="BD208" s="3">
-        <v>7.7684153700989994E-2</v>
+        <v>8.1606393118093201E-2</v>
       </c>
       <c r="BE208" s="3">
-        <v>0.48361475057809999</v>
+        <v>0.49066970492885897</v>
       </c>
       <c r="BF208" s="3">
-        <v>2341169.599314</v>
+        <v>2561597.767488</v>
       </c>
       <c r="BG208" s="3">
         <v>3.2391999999999999</v>
@@ -43640,13 +43640,13 @@
         <v>1.261725</v>
       </c>
       <c r="BD209" s="3">
-        <v>7.7357900511360003E-2</v>
+        <v>8.1288271296230993E-2</v>
       </c>
       <c r="BE209" s="3">
-        <v>0.480007273716543</v>
+        <v>0.49993537013274703</v>
       </c>
       <c r="BF209" s="3">
-        <v>2382246.484313</v>
+        <v>2656825.0827310001</v>
       </c>
       <c r="BG209" s="3">
         <v>3.6334</v>
@@ -43883,13 +43883,13 @@
         <v>0.95327500000000009</v>
       </c>
       <c r="BD210" s="3">
-        <v>7.4588046961187995E-2</v>
+        <v>8.1795689006737296E-2</v>
       </c>
       <c r="BE210" s="3">
-        <v>0.45632314436406601</v>
+        <v>0.49883236894402799</v>
       </c>
       <c r="BF210" s="3">
-        <v>2291416.4393150001</v>
+        <v>2663676.4441800001</v>
       </c>
       <c r="BG210" s="3">
         <v>3.2886000000000002</v>
@@ -44126,13 +44126,13 @@
         <v>0.80967500000000003</v>
       </c>
       <c r="BD211" s="3">
-        <v>7.4693695538186E-2</v>
+        <v>8.3312012602712093E-2</v>
       </c>
       <c r="BE211" s="3">
-        <v>0.46130447551179199</v>
+        <v>0.50174876537059399</v>
       </c>
       <c r="BF211" s="3">
-        <v>2335282.9905829998</v>
+        <v>2720618.7734070001</v>
       </c>
       <c r="BG211" s="3">
         <v>3.1236000000000002</v>
@@ -44369,13 +44369,13 @@
         <v>0.91379999999999995</v>
       </c>
       <c r="BD212" s="3">
-        <v>7.8657056769207007E-2</v>
+        <v>8.4283830472676097E-2</v>
       </c>
       <c r="BE212" s="3">
-        <v>0.49027660024477498</v>
+        <v>0.50662322712076302</v>
       </c>
       <c r="BF212" s="3">
-        <v>2504881.8178569898</v>
+        <v>2787436.30204099</v>
       </c>
       <c r="BG212" s="3">
         <v>3.3347000000000002</v>
@@ -44612,13 +44612,13 @@
         <v>0.41409999999999997</v>
       </c>
       <c r="BD213" s="3">
-        <v>8.3427035885646997E-2</v>
+        <v>8.59482791044692E-2</v>
       </c>
       <c r="BE213" s="3">
-        <v>0.53551218990688598</v>
+        <v>0.54032342122226495</v>
       </c>
       <c r="BF213" s="3">
-        <v>2735988.5041949898</v>
+        <v>2977749.7124359901</v>
       </c>
       <c r="BG213" s="3">
         <v>3.0945</v>
@@ -44855,13 +44855,13 @@
         <v>0.43317500000000003</v>
       </c>
       <c r="BD214" s="3">
-        <v>8.3372046053063004E-2</v>
+        <v>8.7356355338351996E-2</v>
       </c>
       <c r="BE214" s="3">
-        <v>0.54440205988254697</v>
+        <v>0.56728672572210703</v>
       </c>
       <c r="BF214" s="3">
-        <v>2750809.8607439902</v>
+        <v>3081500.5056769899</v>
       </c>
       <c r="BG214" s="3">
         <v>2.7568000000000001</v>
@@ -45098,13 +45098,13 @@
         <v>0.78210000000000002</v>
       </c>
       <c r="BD215" s="3">
-        <v>8.1883194951639995E-2</v>
+        <v>8.9613732612615696E-2</v>
       </c>
       <c r="BE215" s="3">
-        <v>0.54848724410233995</v>
+        <v>0.592813071789696</v>
       </c>
       <c r="BF215" s="3">
-        <v>2740736.2332159998</v>
+        <v>3175606.8052019998</v>
       </c>
       <c r="BG215" s="3">
         <v>3.1526999999999998</v>
@@ -45341,13 +45341,13 @@
         <v>1.4215750000000003</v>
       </c>
       <c r="BD216" s="3">
-        <v>8.2792040033692005E-2</v>
+        <v>9.1172940003264799E-2</v>
       </c>
       <c r="BE216" s="3">
-        <v>0.56759313568248204</v>
+        <v>0.61266999625742902</v>
       </c>
       <c r="BF216" s="3">
-        <v>2845020.9377390002</v>
+        <v>3274913.8419539998</v>
       </c>
       <c r="BG216" s="3">
         <v>4.1440999999999999</v>
@@ -45584,13 +45584,13 @@
         <v>1.0042</v>
       </c>
       <c r="BD217" s="3">
-        <v>8.4252753061261995E-2</v>
+        <v>9.0724245279500196E-2</v>
       </c>
       <c r="BE217" s="3">
-        <v>0.59450429116210701</v>
+        <v>0.62202407657130998</v>
       </c>
       <c r="BF217" s="3">
-        <v>3019994.3116159998</v>
+        <v>3403907.5050849998</v>
       </c>
       <c r="BG217" s="3">
         <v>3.87</v>
@@ -45827,13 +45827,13 @@
         <v>0.35760000000000003</v>
       </c>
       <c r="BD218" s="3">
-        <v>8.1503732207594007E-2</v>
+        <v>8.7471484827057994E-2</v>
       </c>
       <c r="BE218" s="3">
-        <v>0.58244151503849595</v>
+        <v>0.60130187508627897</v>
       </c>
       <c r="BF218" s="3">
-        <v>2995803.7217069999</v>
+        <v>3369746.6348669999</v>
       </c>
       <c r="BG218" s="3">
         <v>3.2366999999999999</v>
@@ -46070,13 +46070,13 @@
         <v>-0.5616000000000001</v>
       </c>
       <c r="BD219" s="3">
-        <v>8.0532308597004998E-2</v>
+        <v>8.6376307936715496E-2</v>
       </c>
       <c r="BE219" s="3">
-        <v>0.58167793978111004</v>
+        <v>0.59881882312801404</v>
       </c>
       <c r="BF219" s="3">
-        <v>3088969.8194550001</v>
+        <v>3484856.151606</v>
       </c>
       <c r="BG219" s="3">
         <v>2.6349999999999998</v>
@@ -46313,13 +46313,13 @@
         <v>-0.62172499999999997</v>
       </c>
       <c r="BD220" s="3">
-        <v>8.3240160109828001E-2</v>
+        <v>8.7694823605026798E-2</v>
       </c>
       <c r="BE220" s="3">
-        <v>0.58847565992775197</v>
+        <v>0.60769688407141997</v>
       </c>
       <c r="BF220" s="3">
-        <v>3279793.776143</v>
+        <v>3695097.5630950001</v>
       </c>
       <c r="BG220" s="3">
         <v>2.359</v>
@@ -46556,13 +46556,13 @@
         <v>-0.57804999999999995</v>
       </c>
       <c r="BD221" s="3">
-        <v>8.7948816730821E-2</v>
+        <v>9.0300949247276496E-2</v>
       </c>
       <c r="BE221" s="3">
-        <v>0.61012965267277797</v>
+        <v>0.62036871395604198</v>
       </c>
       <c r="BF221" s="3">
-        <v>3576108.3148480002</v>
+        <v>3943891.9401670098</v>
       </c>
       <c r="BG221" s="3">
         <v>1.982</v>
@@ -46799,13 +46799,13 @@
         <v>-0.58327499999999999</v>
       </c>
       <c r="BD222" s="3">
-        <v>8.9164097769559997E-2</v>
+        <v>9.2462568095499104E-2</v>
       </c>
       <c r="BE222" s="3">
-        <v>0.59890714238583898</v>
+        <v>0.60497682808174003</v>
       </c>
       <c r="BF222" s="3">
-        <v>3607723.47969101</v>
+        <v>3941210.9591390099</v>
       </c>
       <c r="BG222" s="3">
         <v>1.8884000000000001</v>
@@ -47042,13 +47042,13 @@
         <v>-0.44525000000000003</v>
       </c>
       <c r="BD223" s="3">
-        <v>9.0859515105452995E-2</v>
+        <v>9.6949187151510005E-2</v>
       </c>
       <c r="BE223" s="3">
-        <v>0.60112151750699305</v>
+        <v>0.60940290284809495</v>
       </c>
       <c r="BF223" s="3">
-        <v>3714065.60151301</v>
+        <v>4104680.27256501</v>
       </c>
       <c r="BG223" s="3">
         <v>1.8445</v>
@@ -47285,13 +47285,13 @@
         <v>-0.46884999999999999</v>
       </c>
       <c r="BD224" s="3">
-        <v>9.3660634224333003E-2</v>
+        <v>0.102507832387635</v>
       </c>
       <c r="BE224" s="3">
-        <v>0.616210432773317</v>
+        <v>0.64878326058607805</v>
       </c>
       <c r="BF224" s="3">
-        <v>3928666.9853550098</v>
+        <v>4510936.3091000104</v>
       </c>
       <c r="BG224" s="3">
         <v>1.8208</v>
@@ -47528,13 +47528,13 @@
         <v>-0.69082499999999991</v>
       </c>
       <c r="BD225" s="3">
-        <v>9.3612301015254001E-2</v>
+        <v>0.105321815034882</v>
       </c>
       <c r="BE225" s="3">
-        <v>0.63596782603104096</v>
+        <v>0.69706632328084805</v>
       </c>
       <c r="BF225" s="3">
-        <v>4175518.8345320099</v>
+        <v>4972443.697985</v>
       </c>
       <c r="BG225" s="3">
         <v>1.6519999999999999</v>
@@ -47771,13 +47771,13 @@
         <v>-0.74007500000000004</v>
       </c>
       <c r="BD226" s="3">
-        <v>8.8029764138720004E-2</v>
+        <v>0.102737572557624</v>
       </c>
       <c r="BE226" s="3">
-        <v>0.615428487177201</v>
+        <v>0.68655077343851401</v>
       </c>
       <c r="BF226" s="3">
-        <v>4060756.0510710101</v>
+        <v>4916068.3207399901</v>
       </c>
       <c r="BG226" s="3">
         <v>1.8519000000000001</v>
@@ -48014,13 +48014,13 @@
         <v>-0.55317500000000008</v>
       </c>
       <c r="BD227" s="3">
-        <v>8.4569949682673007E-2</v>
+        <v>9.8239531573195593E-2</v>
       </c>
       <c r="BE227" s="3">
-        <v>0.60070404696318902</v>
+        <v>0.651688658367503</v>
       </c>
       <c r="BF227" s="3">
-        <v>3967814.75508</v>
+        <v>4670458.50287499</v>
       </c>
       <c r="BG227" s="3">
         <v>1.9699</v>
@@ -48257,13 +48257,13 @@
         <v>-0.62437500000000001</v>
       </c>
       <c r="BD228" s="3">
-        <v>8.6673684993683997E-2</v>
+        <v>9.5080999525865198E-2</v>
       </c>
       <c r="BE228" s="3">
-        <v>0.59568661454204197</v>
+        <v>0.62028946111899597</v>
       </c>
       <c r="BF228" s="3">
-        <v>3981673.3224490001</v>
+        <v>4478498.2211169899</v>
       </c>
       <c r="BG228" s="3">
         <v>1.7806999999999999</v>
@@ -48500,13 +48500,13 @@
         <v>-0.48800000000000004</v>
       </c>
       <c r="BD229" s="3">
-        <v>8.9853553156928001E-2</v>
+        <v>9.2631190271571198E-2</v>
       </c>
       <c r="BE229" s="3">
-        <v>0.60346780512793696</v>
+        <v>0.61071028725975196</v>
       </c>
       <c r="BF229" s="3">
-        <v>4182304.4128479999</v>
+        <v>4535829.8696919996</v>
       </c>
       <c r="BG229" s="3">
         <v>1.8502000000000001</v>
@@ -48743,13 +48743,13 @@
         <v>-0.52727500000000005</v>
       </c>
       <c r="BD230" s="3">
-        <v>8.7384372049983006E-2</v>
+        <v>8.9206374125823995E-2</v>
       </c>
       <c r="BE230" s="3">
-        <v>0.57712685641266404</v>
+        <v>0.58357305720296004</v>
       </c>
       <c r="BF230" s="3">
-        <v>4109927.3895089999</v>
+        <v>4414276.3657280104</v>
       </c>
       <c r="BG230" s="3">
         <v>1.6903999999999999</v>
@@ -48986,13 +48986,13 @@
         <v>-0.47494999999999998</v>
       </c>
       <c r="BD231" s="3">
-        <v>8.3974511972031998E-2</v>
+        <v>8.5374414205811197E-2</v>
       </c>
       <c r="BE231" s="3">
-        <v>0.56024326812598602</v>
+        <v>0.56116200427825502</v>
       </c>
       <c r="BF231" s="3">
-        <v>4106470.0907999999</v>
+        <v>4372594.3995310096</v>
       </c>
       <c r="BG231" s="3">
         <v>1.6846000000000001</v>
@@ -49229,13 +49229,13 @@
         <v>-0.44802500000000001</v>
       </c>
       <c r="BD232" s="3">
-        <v>8.5402259644087E-2</v>
+        <v>8.4994133561557703E-2</v>
       </c>
       <c r="BE232" s="3">
-        <v>0.56625310057322198</v>
+        <v>0.55799248291292602</v>
       </c>
       <c r="BF232" s="3">
-        <v>4247936.5680830004</v>
+        <v>4472036.7364800004</v>
       </c>
       <c r="BG232" s="3">
         <v>1.772</v>
@@ -49472,13 +49472,13 @@
         <v>-0.55820000000000003</v>
       </c>
       <c r="BD233" s="3">
-        <v>8.9375468530747001E-2</v>
+        <v>8.77285452016522E-2</v>
       </c>
       <c r="BE233" s="3">
-        <v>0.60471564550571899</v>
+        <v>0.59287934278586196</v>
       </c>
       <c r="BF233" s="3">
-        <v>4652148.7742259996</v>
+        <v>4890956.5496389996</v>
       </c>
       <c r="BG233" s="3">
         <v>1.6173999999999999</v>
@@ -49715,13 +49715,13 @@
         <v>-0.55722499999999997</v>
       </c>
       <c r="BD234" s="3">
-        <v>9.0920914567916997E-2</v>
+        <v>8.95479340568687E-2</v>
       </c>
       <c r="BE234" s="3">
-        <v>0.62282246590900103</v>
+        <v>0.61462134855205697</v>
       </c>
       <c r="BF234" s="3">
-        <v>4840215.1360240001</v>
+        <v>5139590.8901770003</v>
       </c>
       <c r="BG234" s="3">
         <v>1.5329999999999999</v>
@@ -49958,13 +49958,13 @@
         <v>-0.420825</v>
       </c>
       <c r="BD235" s="3">
-        <v>9.0517642669864007E-2</v>
+        <v>8.9492930720289798E-2</v>
       </c>
       <c r="BE235" s="3">
-        <v>0.63980613325249502</v>
+        <v>0.63129220306723099</v>
       </c>
       <c r="BF235" s="3">
-        <v>5049163.8098390102</v>
+        <v>5344047.5036310097</v>
       </c>
       <c r="BG235" s="3">
         <v>1.6978</v>
@@ -50201,13 +50201,13 @@
         <v>-4.7349999999999996E-2</v>
       </c>
       <c r="BD236" s="3">
-        <v>9.2736412060644993E-2</v>
+        <v>9.0094968485261898E-2</v>
       </c>
       <c r="BE236" s="3">
-        <v>0.66078901129704404</v>
+        <v>0.65486239956091297</v>
       </c>
       <c r="BF236" s="3">
-        <v>5267143.5087880101</v>
+        <v>5583666.3671540096</v>
       </c>
       <c r="BG236" s="3">
         <v>2.2343999999999999</v>
@@ -50444,13 +50444,13 @@
         <v>0.25547500000000001</v>
       </c>
       <c r="BD237" s="3">
-        <v>9.4904020186513005E-2</v>
+        <v>9.0758016547488302E-2</v>
       </c>
       <c r="BE237" s="3">
-        <v>0.695161899961248</v>
+        <v>0.69753720393809004</v>
       </c>
       <c r="BF237" s="3">
-        <v>5648177.3395640096</v>
+        <v>6089851.5676150098</v>
       </c>
       <c r="BG237" s="3">
         <v>2.7972999999999999</v>
@@ -50687,13 +50687,13 @@
         <v>0.74192499999999995</v>
       </c>
       <c r="BD238" s="3">
-        <v>9.4167504094957E-2</v>
+        <v>9.05416549638937E-2</v>
       </c>
       <c r="BE238" s="3">
-        <v>0.69582812982576203</v>
+        <v>0.70673600383133395</v>
       </c>
       <c r="BF238" s="3">
-        <v>5666142.1126809996</v>
+        <v>6258135.1088190004</v>
       </c>
       <c r="BG238" s="3">
         <v>3.5019999999999998</v>
@@ -50930,13 +50930,13 @@
         <v>0.66260000000000008</v>
       </c>
       <c r="BD239" s="3">
-        <v>9.0368501537136006E-2</v>
+        <v>8.8673406143471703E-2</v>
       </c>
       <c r="BE239" s="3">
-        <v>0.68642527723577296</v>
+        <v>0.70694138721217004</v>
       </c>
       <c r="BF239" s="3">
-        <v>5489451.6482739998</v>
+        <v>6225421.2761209998</v>
       </c>
       <c r="BG239" s="3">
         <v>3.4013</v>
@@ -51173,13 +51173,13 @@
         <v>1.614125</v>
       </c>
       <c r="BD240" s="3">
-        <v>8.8548799670930003E-2</v>
+        <v>8.90314366492964E-2</v>
       </c>
       <c r="BE240" s="3">
-        <v>0.68413512737292004</v>
+        <v>0.72001544771900705</v>
       </c>
       <c r="BF240" s="3">
-        <v>5135900.18566899</v>
+        <v>5963122.9381859899</v>
       </c>
       <c r="BG240" s="3">
         <v>4.8465999999999996</v>
@@ -51416,13 +51416,13 @@
         <v>2.5589249999999999</v>
       </c>
       <c r="BD241" s="3">
-        <v>8.8800902606725005E-2</v>
+        <v>9.0697847347261898E-2</v>
       </c>
       <c r="BE241" s="3">
-        <v>0.70987957638340904</v>
+        <v>0.75865602097137996</v>
       </c>
       <c r="BF241" s="3">
-        <v>5027189.2391590001</v>
+        <v>5858776.8492699899</v>
       </c>
       <c r="BG241" s="3">
         <v>7.2518000000000002</v>
@@ -51659,13 +51659,13 @@
         <v>2.3615000000000004</v>
       </c>
       <c r="BD242" s="3">
-        <v>9.0394203497413006E-2</v>
+        <v>9.1914431229790303E-2</v>
       </c>
       <c r="BE242" s="3">
-        <v>0.715997654719989</v>
+        <v>0.76353802109560098</v>
       </c>
       <c r="BF242" s="3">
-        <v>4934471.3104849998</v>
+        <v>5680795.1202640003</v>
       </c>
       <c r="BG242" s="3">
         <v>6.0926</v>
@@ -51902,13 +51902,13 @@
         <v>0.977275</v>
       </c>
       <c r="BD243" s="3">
-        <v>9.3473623287093993E-2</v>
+        <v>9.3991087468097506E-2</v>
       </c>
       <c r="BE243" s="3">
-        <v>0.71506832572467904</v>
+        <v>0.746561141142012</v>
       </c>
       <c r="BF243" s="3">
-        <v>5153166.8890020102</v>
+        <v>5735226.8599150097</v>
       </c>
       <c r="BG243" s="3">
         <v>4.5029000000000003</v>
@@ -52145,13 +52145,13 @@
         <v>-0.10685</v>
       </c>
       <c r="BD244" s="3">
-        <v>9.8543847077089006E-2</v>
+        <v>9.7090200470377405E-2</v>
       </c>
       <c r="BE244" s="3">
-        <v>0.71044071844678303</v>
+        <v>0.73147581910949</v>
       </c>
       <c r="BF244" s="3">
-        <v>5398701.6815689998</v>
+        <v>5964205.7262290101</v>
       </c>
       <c r="BG244" s="3">
         <v>3.1901999999999999</v>
@@ -52388,13 +52388,13 @@
         <v>-0.31840000000000002</v>
       </c>
       <c r="BD245" s="3">
-        <v>0.10063453274742699</v>
+        <v>9.75961714763834E-2</v>
       </c>
       <c r="BE245" s="3">
-        <v>0.72354366315951602</v>
+        <v>0.73604486818006998</v>
       </c>
       <c r="BF245" s="3">
-        <v>5711297.0364199998</v>
+        <v>6334266.7337579997</v>
       </c>
       <c r="BG245" s="3">
         <v>2.6547999999999998</v>
@@ -52631,13 +52631,13 @@
         <v>-0.19042500000000001</v>
       </c>
       <c r="BD246" s="3">
-        <v>9.8354822355158994E-2</v>
+        <v>9.6093148846950804E-2</v>
       </c>
       <c r="BE246" s="3">
-        <v>0.713884416693641</v>
+        <v>0.71497346051473998</v>
       </c>
       <c r="BF246" s="3">
-        <v>5677925.6653460003</v>
+        <v>6337770.2450099904</v>
       </c>
       <c r="BG246" s="3">
         <v>2.3338000000000001</v>
@@ -52874,13 +52874,13 @@
         <v>-0.13297500000000001</v>
       </c>
       <c r="BD247" s="3">
-        <v>9.6099663872733998E-2</v>
+        <v>9.4547232513405202E-2</v>
       </c>
       <c r="BE247" s="3">
-        <v>0.70998455238674396</v>
+        <v>0.69785912804619998</v>
       </c>
       <c r="BF247" s="3">
-        <v>5773586.6631939998</v>
+        <v>6397047.4544949904</v>
       </c>
       <c r="BG247" s="3">
         <v>2.5171999999999999</v>
@@ -53117,13 +53117,13 @@
         <v>-0.13464999999999999</v>
       </c>
       <c r="BD248" s="3">
-        <v>9.7292009750287997E-2</v>
+        <v>9.86677459273856E-2</v>
       </c>
       <c r="BE248" s="3">
-        <v>0.71160119145474299</v>
+        <v>0.72118900836142097</v>
       </c>
       <c r="BF248" s="3">
-        <v>5964945.3999199998</v>
+        <v>6840674.0853270004</v>
       </c>
       <c r="BG248" s="3">
         <v>2.5743</v>
@@ -53360,13 +53360,13 @@
         <v>-0.16390000000000002</v>
       </c>
       <c r="BD249" s="3">
-        <v>0.100704839928955</v>
+        <v>0.104755457745825</v>
       </c>
       <c r="BE249" s="3">
-        <v>0.73305781799091696</v>
+        <v>0.78098239938526204</v>
       </c>
       <c r="BF249" s="3">
-        <v>6444698.6985480003</v>
+        <v>7785301.4370280001</v>
       </c>
       <c r="BG249" s="3">
         <v>2.3157999999999999</v>
@@ -53603,13 +53603,13 @@
         <v>-0.2001</v>
       </c>
       <c r="BD250" s="3">
-        <v>0.10184445786646</v>
+        <v>0.105812944586542</v>
       </c>
       <c r="BE250" s="3">
-        <v>0.738830908614722</v>
+        <v>0.79685336743980895</v>
       </c>
       <c r="BF250" s="3">
-        <v>6692351.2768890001</v>
+        <v>8311218.8123629997</v>
       </c>
       <c r="BG250" s="3">
         <v>2.0299</v>
@@ -53846,13 +53846,13 @@
         <v>-0.12257499999999999</v>
       </c>
       <c r="BD251" s="3">
-        <v>0.102683897988842</v>
+        <v>0.104243192079483</v>
       </c>
       <c r="BE251" s="3">
-        <v>0.74968316846670302</v>
+        <v>0.78362885759638601</v>
       </c>
       <c r="BF251" s="3">
-        <v>6923534.7012789901</v>
+        <v>8293989.30873599</v>
       </c>
       <c r="BG251" s="3">
         <v>2.1107</v>
@@ -54089,13 +54089,13 @@
         <v>-0.10205</v>
       </c>
       <c r="BD252" s="3">
-        <v>0.103939626411853</v>
+        <v>0.102203513786695</v>
       </c>
       <c r="BE252" s="3">
-        <v>0.75195009403217605</v>
+        <v>0.76902253953984301</v>
       </c>
       <c r="BF252" s="3">
-        <v>6969741.3217599904</v>
+        <v>8036547.6815779898</v>
       </c>
       <c r="BG252" s="3">
         <v>2.7482000000000002</v>
@@ -54308,13 +54308,13 @@
         <v>2.5049999999999989E-2</v>
       </c>
       <c r="BD253" s="3">
-        <v>0.105473445879523</v>
+        <v>0.10291828270195599</v>
       </c>
       <c r="BE253" s="3">
-        <v>0.75795647585162895</v>
+        <v>0.78492833611912805</v>
       </c>
       <c r="BF253" s="3">
-        <v>7064151.8047820004</v>
+        <v>8103247.2093869997</v>
       </c>
       <c r="BG253" s="3">
         <v>2.8654000000000002</v>
@@ -54527,13 +54527,13 @@
         <v>-0.25905</v>
       </c>
       <c r="BD254" s="3">
-        <v>0.10565478964223</v>
+        <v>0.10618597712367001</v>
       </c>
       <c r="BE254" s="3">
-        <v>0.76144005392360903</v>
+        <v>0.80746694900210203</v>
       </c>
       <c r="BF254" s="3">
-        <v>7120991.0151549997</v>
+        <v>8427415.3296180107</v>
       </c>
       <c r="BG254" s="3">
         <v>2.5446</v>
@@ -54746,13 +54746,13 @@
         <v>-0.25342500000000001</v>
       </c>
       <c r="BD255" s="3">
-        <v>0.106907679242241</v>
+        <v>0.108694306846668</v>
       </c>
       <c r="BE255" s="3">
-        <v>0.77648060561029997</v>
+        <v>0.82166768738821105</v>
       </c>
       <c r="BF255" s="3">
-        <v>7410524.6845183996</v>
+        <v>8820076.4102024008</v>
       </c>
       <c r="BG255" s="3">
         <v>2.6608999999999998</v>
@@ -54965,13 +54965,13 @@
         <v>-0.343725</v>
       </c>
       <c r="BD256" s="3">
-        <v>0.10722100350283301</v>
+        <v>0.107700685363146</v>
       </c>
       <c r="BE256" s="3">
-        <v>0.78056306829565703</v>
+        <v>0.81562488862194504</v>
       </c>
       <c r="BF256" s="3">
-        <v>7605885.9432226</v>
+        <v>8949204.4518245906</v>
       </c>
       <c r="BG256" s="3">
         <v>2.4359999999999999</v>
@@ -55184,13 +55184,13 @@
         <v>-0.26882499999999998</v>
       </c>
       <c r="BD257" s="3">
-        <v>0.10777845808825399</v>
+        <v>0.105373951345423</v>
       </c>
       <c r="BE257" s="3">
-        <v>0.77954390686548103</v>
+        <v>0.79900445815154997</v>
       </c>
       <c r="BF257" s="3">
-        <v>7714342.8174075997</v>
+        <v>8864786.5669855792</v>
       </c>
       <c r="BG257" s="3">
         <v>2.2204999999999999</v>
@@ -55403,13 +55403,13 @@
         <v>-0.201875</v>
       </c>
       <c r="BD258" s="3">
-        <v>0.10728999211141001</v>
+        <v>0.103642921692826</v>
       </c>
       <c r="BE258" s="3">
-        <v>0.76788620883138503</v>
+        <v>0.77551292275828898</v>
       </c>
       <c r="BF258" s="3">
-        <v>7594126.5465988005</v>
+        <v>8694283.8634268008</v>
       </c>
       <c r="BG258" s="3">
         <v>2.1053999999999999</v>
@@ -55622,13 +55622,13 @@
         <v>-0.34557500000000002</v>
       </c>
       <c r="BD259" s="3">
-        <v>0.10862856843363</v>
+        <v>0.10612370754334501</v>
       </c>
       <c r="BE259" s="3">
-        <v>0.76459704126625305</v>
+        <v>0.76951017977812697</v>
       </c>
       <c r="BF259" s="3">
-        <v>7627943.4226056002</v>
+        <v>8753077.4897136092</v>
       </c>
       <c r="BG259" s="3">
         <v>2.0493000000000001</v>
@@ -55841,13 +55841,13 @@
         <v>-0.11365</v>
       </c>
       <c r="BD260" s="3">
-        <v>0.11056801859465699</v>
+        <v>0.109675293947521</v>
       </c>
       <c r="BE260" s="3">
-        <v>0.76309632996370902</v>
+        <v>0.77874273153669005</v>
       </c>
       <c r="BF260" s="3">
-        <v>7770564.5117295999</v>
+        <v>8949898.6297166198</v>
       </c>
       <c r="BG260" s="3">
         <v>2.0004</v>
@@ -56060,13 +56060,13 @@
         <v>-0.12620000000000001</v>
       </c>
       <c r="BD261" s="3">
-        <v>0.11248740624912799</v>
+        <v>0.111915766299071</v>
       </c>
       <c r="BE261" s="3">
-        <v>0.76247423265619796</v>
+        <v>0.78932816940640504</v>
       </c>
       <c r="BF261" s="3">
-        <v>7988308.2359253997</v>
+        <v>9114404.0081404205</v>
       </c>
       <c r="BG261" s="3">
         <v>1.8586</v>
@@ -56279,13 +56279,13 @@
         <v>-0.30115000000000003</v>
       </c>
       <c r="BD262" s="3">
-        <v>0.11186646401436599</v>
+        <v>0.111458985286585</v>
       </c>
       <c r="BE262" s="3">
-        <v>0.75433863617858898</v>
+        <v>0.78367598998256305</v>
       </c>
       <c r="BF262" s="3">
-        <v>8039005.9909459902</v>
+        <v>9231827.9545130096</v>
       </c>
       <c r="BG262" s="3">
         <v>1.6918</v>
@@ -56498,13 +56498,13 @@
         <v>-0.36865000000000003</v>
       </c>
       <c r="BD263" s="3">
-        <v>0.110896153037965</v>
+        <v>0.110464202009379</v>
       </c>
       <c r="BE263" s="3">
-        <v>0.74541432451989897</v>
+        <v>0.76625126137547295</v>
       </c>
       <c r="BF263" s="3">
-        <v>8009921.3953829901</v>
+        <v>9300161.9677649997</v>
       </c>
       <c r="BG263" s="3">
         <v>1.5889</v>
@@ -56717,13 +56717,13 @@
         <v>-0.31905</v>
       </c>
       <c r="BD264" s="3">
-        <v>0.110056201659051</v>
+        <v>0.10939995171092801</v>
       </c>
       <c r="BE264" s="3">
-        <v>0.73970938827211996</v>
+        <v>0.75328185534726899</v>
       </c>
       <c r="BF264" s="3">
-        <v>7927580.5353049999</v>
+        <v>9290172.55363</v>
       </c>
       <c r="BG264" s="3">
         <v>1.6941999999999999</v>
@@ -56936,13 +56936,13 @@
         <v>-0.16302499999999998</v>
       </c>
       <c r="BD265" s="3">
-        <v>0.11064948473436</v>
+        <v>0.109327597742057</v>
       </c>
       <c r="BE265" s="3">
-        <v>0.74234860625396204</v>
+        <v>0.75319794254986805</v>
       </c>
       <c r="BF265" s="3">
-        <v>7904768.8357140003</v>
+        <v>9274517.3236290105</v>
       </c>
       <c r="BG265" s="3">
         <v>1.9925999999999999</v>
@@ -57155,13 +57155,13 @@
         <v>-0.26582499999999998</v>
       </c>
       <c r="BD266" s="3">
-        <v>0.11091883233761</v>
+        <v>0.10902974490378201</v>
       </c>
       <c r="BE266" s="3">
-        <v>0.74730824519333205</v>
+        <v>0.75875145258501697</v>
       </c>
       <c r="BF266" s="3">
-        <v>7869259.1561740097</v>
+        <v>9210331.8705920205</v>
       </c>
       <c r="BG266" s="3">
         <v>2.0068999999999999</v>
@@ -57374,13 +57374,13 @@
         <v>1.6199999999999999E-2</v>
       </c>
       <c r="BD267" s="3">
-        <v>0.11126215120496</v>
+        <v>0.108728453330884</v>
       </c>
       <c r="BE267" s="3">
-        <v>0.74558651332711701</v>
+        <v>0.75864456785934498</v>
       </c>
       <c r="BF267" s="3">
-        <v>7825937.1072070096</v>
+        <v>9136399.0658940393</v>
       </c>
       <c r="BG267" s="3">
         <v>2.0863999999999998</v>
@@ -57593,13 +57593,13 @@
         <v>0.2757</v>
       </c>
       <c r="BD268" s="3">
-        <v>0.110246226918173</v>
+        <v>0.107514298534767</v>
       </c>
       <c r="BE268" s="3">
-        <v>0.73232936936190596</v>
+        <v>0.74557559538318496</v>
       </c>
       <c r="BF268" s="3">
-        <v>7659761.6533350199</v>
+        <v>8913493.7999510393</v>
       </c>
       <c r="BG268" s="3">
         <v>2.3969999999999998</v>
@@ -57809,13 +57809,13 @@
         <v>0.49834999999999996</v>
       </c>
       <c r="BD269" s="3">
-        <v>0.109590111068558</v>
+        <v>0.106880121992855</v>
       </c>
       <c r="BE269" s="3">
-        <v>0.72609058077815303</v>
+        <v>0.738206622686162</v>
       </c>
       <c r="BF269" s="3">
-        <v>7572438.9285230199</v>
+        <v>8650945.8629610296</v>
       </c>
       <c r="BG269" s="3">
         <v>2.6116000000000001</v>
@@ -58025,13 +58025,13 @@
         <v>0.48517500000000002</v>
       </c>
       <c r="BD270" s="3">
-        <v>0.108956253547199</v>
+        <v>0.108121971490504</v>
       </c>
       <c r="BE270" s="3">
-        <v>0.72897378478852803</v>
+        <v>0.75451626074989697</v>
       </c>
       <c r="BF270" s="3">
-        <v>7587074.5321890097</v>
+        <v>8664171.4152450096</v>
       </c>
       <c r="BG270" s="3">
         <v>2.6930000000000001</v>
@@ -58241,13 +58241,13 @@
         <v>-0.15785000000000002</v>
       </c>
       <c r="BD271" s="3">
-        <v>0.110042348731199</v>
+        <v>0.110840740556282</v>
       </c>
       <c r="BE271" s="3">
-        <v>0.73883262312384801</v>
+        <v>0.77899950214850999</v>
       </c>
       <c r="BF271" s="3">
-        <v>7739304.60931399</v>
+        <v>8963266.5944539905</v>
       </c>
       <c r="BG271" s="3">
         <v>2.0855000000000001</v>
@@ -58455,13 +58455,13 @@
       </c>
       <c r="BC272" s="15"/>
       <c r="BD272" s="3">
-        <v>0.111991615600868</v>
+        <v>0.112532278003487</v>
       </c>
       <c r="BE272" s="3">
-        <v>0.74757298223563295</v>
+        <v>0.78068260723795802</v>
       </c>
       <c r="BF272" s="3">
-        <v>7864884.5255679898</v>
+        <v>9131131.2330459803</v>
       </c>
       <c r="BH272" s="3">
         <v>104</v>
@@ -58666,13 +58666,13 @@
       </c>
       <c r="BC273" s="15"/>
       <c r="BD273" s="3">
-        <v>0.115037580443903</v>
+        <v>0.11517370371451199</v>
       </c>
       <c r="BE273" s="3">
-        <v>0.75829779440719203</v>
+        <v>0.78627226024902996</v>
       </c>
       <c r="BF273" s="3">
-        <v>8026413.9860739997</v>
+        <v>9442333.3688729908</v>
       </c>
       <c r="BH273" s="3">
         <v>110</v>
@@ -58877,13 +58877,13 @@
       </c>
       <c r="BC274" s="15"/>
       <c r="BD274" s="3">
-        <v>0.117047429968654</v>
+        <v>0.11875117025418599</v>
       </c>
       <c r="BE274" s="3">
-        <v>0.76896329085972503</v>
+        <v>0.80250408799958495</v>
       </c>
       <c r="BF274" s="3">
-        <v>8197313.0779109998</v>
+        <v>9809755.2384499907</v>
       </c>
       <c r="BH274" s="3">
         <v>117</v>
@@ -59086,13 +59086,13 @@
       </c>
       <c r="BC275" s="15"/>
       <c r="BD275" s="3">
-        <v>0.119165318989712</v>
+        <v>0.12158161037408299</v>
       </c>
       <c r="BE275" s="3">
-        <v>0.78020201605956097</v>
+        <v>0.81180675838613003</v>
       </c>
       <c r="BF275" s="3">
-        <v>8502357.1960300002</v>
+        <v>10049062.680808</v>
       </c>
       <c r="BH275" s="3">
         <v>114</v>
@@ -59295,13 +59295,13 @@
       </c>
       <c r="BC276" s="15"/>
       <c r="BD276" s="3">
-        <v>0.120803588445183</v>
+        <v>0.122377588345172</v>
       </c>
       <c r="BE276" s="3">
-        <v>0.78437595822168105</v>
+        <v>0.80864872476127903</v>
       </c>
       <c r="BF276" s="3">
-        <v>8794222.4364869893</v>
+        <v>10148839.078023</v>
       </c>
       <c r="BH276" s="3">
         <v>106</v>
@@ -59501,13 +59501,13 @@
       </c>
       <c r="BC277" s="15"/>
       <c r="BD277" s="3">
-        <v>0.120581787184065</v>
+        <v>0.120592831632753</v>
       </c>
       <c r="BE277" s="3">
-        <v>0.78120358557897696</v>
+        <v>0.79584916020778895</v>
       </c>
       <c r="BF277" s="3">
-        <v>11051764.7461234</v>
+        <v>12610062.3198811</v>
       </c>
       <c r="BH277" s="3">
         <v>111</v>
@@ -59707,13 +59707,13 @@
       </c>
       <c r="BC278" s="15"/>
       <c r="BD278" s="3">
-        <v>0.11944488587704601</v>
+        <v>0.11991690019283301</v>
       </c>
       <c r="BE278" s="3">
-        <v>0.77853570086592505</v>
+        <v>0.79753993458693795</v>
       </c>
       <c r="BF278" s="3">
-        <v>10944034.5394175</v>
+        <v>12663747.820432</v>
       </c>
       <c r="BH278" s="3">
         <v>113</v>
@@ -59894,13 +59894,13 @@
       </c>
       <c r="BC279" s="10"/>
       <c r="BD279" s="3">
-        <v>0.11728081822831</v>
+        <v>0.119227990024406</v>
       </c>
       <c r="BE279" s="3">
-        <v>0.77323048293112395</v>
+        <v>0.79932699407939101</v>
       </c>
       <c r="BF279" s="3">
-        <v>11837285.5927434</v>
+        <v>13961350.381428299</v>
       </c>
       <c r="BH279" s="3">
         <v>107</v>

</xml_diff>